<commit_message>
Add new graph distance to compliance like document COM(2017) 749 final https://eur-lex.europa.eu/legal-content/FR/TXT/?uri=COM:2017:749:FIN
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2018_register_model_20181015.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2018_register_model_20181015.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.vincent\Documents\siif\20181022\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.vincent\Documents\siif\20181024\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="17" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="546">
   <si>
     <t>Sensitive areas reported for reference date</t>
   </si>
@@ -2200,7 +2200,7 @@
     <numFmt numFmtId="167" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="77" x14ac:knownFonts="1">
+  <fonts count="78" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2751,6 +2751,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333300"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="43">
@@ -3920,7 +3928,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="839">
+  <cellXfs count="840">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5567,6 +5575,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="76" fillId="42" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="77" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6009,9 +6023,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="76" fillId="42" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Hyperlink 2" xfId="9"/>
@@ -6198,6 +6209,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF333300"/>
+      <color rgb="FFCCFFCC"/>
       <color rgb="FF33CC33"/>
       <color rgb="FF663300"/>
       <color rgb="FF6600FF"/>
@@ -6206,8 +6219,6 @@
       <color rgb="FFFFCCCC"/>
       <color rgb="FF604A7B"/>
       <color rgb="FFCCC1DA"/>
-      <color rgb="FF660066"/>
-      <color rgb="FFCCCCFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -6266,6 +6277,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6342,12 +6354,13 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{46DFFB82-EC97-4210-B72D-04D2B1B00EC1}" type="CELLRANGE">
+                    <a:fld id="{62F2E86C-083F-435F-8772-482FE995B353}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6365,6 +6378,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -6372,12 +6386,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4059B624-E533-456F-93DA-9C6127F43E56}" type="CELLRANGE">
+                    <a:fld id="{51F33832-80FC-4287-898B-808E5E653548}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6395,6 +6410,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -6403,12 +6419,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60B85D52-FF8D-4E2D-9C05-FC9898F84326}" type="CELLRANGE">
+                    <a:fld id="{2D58B840-B8CC-47D1-A17F-6BB98A1BCA3C}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6426,6 +6443,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -6471,6 +6489,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -6577,12 +6596,13 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6639160-F3AB-496A-833E-A4412FF7F3F2}" type="CELLRANGE">
+                    <a:fld id="{6436A324-10C8-45FB-B520-CC0FFB67F1A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6600,6 +6620,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -6607,12 +6628,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4690637A-AF1A-45E9-9BD7-E7D4E8C22473}" type="CELLRANGE">
+                    <a:fld id="{B753F9E7-DB98-4E30-8C03-B471B572CFCD}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6630,6 +6652,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -6638,12 +6661,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1EADC2E5-9592-42CC-BF3C-0A84951AB3BC}" type="CELLRANGE">
+                    <a:fld id="{BDDF6030-4E13-430B-85F2-F0D24B2A471E}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6661,6 +6685,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -6706,6 +6731,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -6793,11 +6819,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1304513392"/>
-        <c:axId val="-1304512848"/>
+        <c:axId val="-1989722032"/>
+        <c:axId val="-1989728560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1304513392"/>
+        <c:axId val="-1989722032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6840,7 +6866,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1304512848"/>
+        <c:crossAx val="-1989728560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6848,7 +6874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1304512848"/>
+        <c:axId val="-1989728560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6880,6 +6906,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6940,7 +6967,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1304513392"/>
+        <c:crossAx val="-1989722032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7075,6 +7102,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7326,11 +7354,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1300273824"/>
-        <c:axId val="-1300268384"/>
+        <c:axId val="-1989728016"/>
+        <c:axId val="-1989719312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1300273824"/>
+        <c:axId val="-1989728016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7362,6 +7390,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7428,7 +7457,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300268384"/>
+        <c:crossAx val="-1989719312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7436,7 +7465,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1300268384"/>
+        <c:axId val="-1989719312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7556,7 +7585,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300273824"/>
+        <c:crossAx val="-1989728016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7686,6 +7715,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8440,11 +8470,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1300272192"/>
-        <c:axId val="-1300264032"/>
+        <c:axId val="-1989726384"/>
+        <c:axId val="-1989722576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1300272192"/>
+        <c:axId val="-1989726384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8547,7 +8577,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300264032"/>
+        <c:crossAx val="-1989722576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8555,7 +8585,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1300264032"/>
+        <c:axId val="-1989722576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8606,7 +8636,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300272192"/>
+        <c:crossAx val="-1989726384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8971,11 +9001,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1300276544"/>
-        <c:axId val="-1300270560"/>
+        <c:axId val="-1989717680"/>
+        <c:axId val="-1989716048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1300276544"/>
+        <c:axId val="-1989717680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9086,7 +9116,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300270560"/>
+        <c:crossAx val="-1989716048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9094,7 +9124,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1300270560"/>
+        <c:axId val="-1989716048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9200,7 +9230,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300276544"/>
+        <c:crossAx val="-1989717680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9570,11 +9600,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1300267296"/>
-        <c:axId val="-1300276000"/>
+        <c:axId val="-1989725296"/>
+        <c:axId val="-1989719856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1300267296"/>
+        <c:axId val="-1989725296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9685,7 +9715,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300276000"/>
+        <c:crossAx val="-1989719856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9693,7 +9723,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1300276000"/>
+        <c:axId val="-1989719856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9807,7 +9837,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300267296"/>
+        <c:crossAx val="-1989725296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9942,6 +9972,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10288,11 +10319,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1300270016"/>
-        <c:axId val="-1300263488"/>
+        <c:axId val="-1989718768"/>
+        <c:axId val="-1989718224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1300270016"/>
+        <c:axId val="-1989718768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10398,7 +10429,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300263488"/>
+        <c:crossAx val="-1989718224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10406,7 +10437,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1300263488"/>
+        <c:axId val="-1989718224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10528,7 +10559,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300270016"/>
+        <c:crossAx val="-1989718768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10864,11 +10895,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1300269472"/>
-        <c:axId val="-1300265120"/>
+        <c:axId val="-1989717136"/>
+        <c:axId val="-1989715504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1300269472"/>
+        <c:axId val="-1989717136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10979,7 +11010,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300265120"/>
+        <c:crossAx val="-1989715504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10987,7 +11018,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1300265120"/>
+        <c:axId val="-1989715504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11101,7 +11132,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300269472"/>
+        <c:crossAx val="-1989717136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11437,11 +11468,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1300262400"/>
-        <c:axId val="-1300268928"/>
+        <c:axId val="-1987468016"/>
+        <c:axId val="-1987468560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1300262400"/>
+        <c:axId val="-1987468016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11552,7 +11583,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300268928"/>
+        <c:crossAx val="-1987468560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11560,7 +11591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1300268928"/>
+        <c:axId val="-1987468560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11674,7 +11705,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300262400"/>
+        <c:crossAx val="-1987468016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11809,6 +11840,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12055,11 +12087,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1300277632"/>
-        <c:axId val="-1300271104"/>
+        <c:axId val="-1987473456"/>
+        <c:axId val="-1987470192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1300277632"/>
+        <c:axId val="-1987473456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12091,6 +12123,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12157,7 +12190,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300271104"/>
+        <c:crossAx val="-1987470192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12165,7 +12198,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1300271104"/>
+        <c:axId val="-1987470192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12284,7 +12317,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300277632"/>
+        <c:crossAx val="-1987473456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12789,11 +12822,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1300275456"/>
-        <c:axId val="-1300272736"/>
+        <c:axId val="-1987475632"/>
+        <c:axId val="-1987474544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1300275456"/>
+        <c:axId val="-1987475632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12836,7 +12869,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300272736"/>
+        <c:crossAx val="-1987474544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12844,7 +12877,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1300272736"/>
+        <c:axId val="-1987474544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12950,7 +12983,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300275456"/>
+        <c:crossAx val="-1987475632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13075,6 +13108,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13151,12 +13185,13 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{012F04F7-A534-486E-8336-B485FB9EE501}" type="CELLRANGE">
+                    <a:fld id="{5173D7CE-2C95-4584-8C0A-96B9CA809F47}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13174,6 +13209,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -13181,12 +13217,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FDB3AF30-4049-4B1B-8594-EF4BC721BB6C}" type="CELLRANGE">
+                    <a:fld id="{CEAAA4D9-8776-40CD-9ACF-48DDE5164D11}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13204,6 +13241,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -13212,12 +13250,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D293D90-ED98-4746-8B5C-0CF860BC6DD4}" type="CELLRANGE">
+                    <a:fld id="{A0F27F48-D8CF-4B63-A31A-3468F562054F}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13235,6 +13274,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -13280,6 +13320,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -13386,12 +13427,13 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47633502-74A1-45E7-A2D7-B4FBDEAEDD89}" type="CELLRANGE">
+                    <a:fld id="{4BB92A20-24BF-4B4D-AEB2-FBB27C6B1F03}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13409,6 +13451,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -13416,12 +13459,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F41DD68-1CDE-4915-A16A-E2AFEC0B80D2}" type="CELLRANGE">
+                    <a:fld id="{FF6568E4-7599-4C53-BB3A-8693A87E91FD}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13439,6 +13483,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -13447,12 +13492,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{449A2049-479A-46C7-91E2-7D430F48249D}" type="CELLRANGE">
+                    <a:fld id="{402E5C3B-FCD3-4CC2-A62E-4F0FA16C0817}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13470,6 +13516,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -13515,6 +13562,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -13602,11 +13650,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1304511760"/>
-        <c:axId val="-1304518832"/>
+        <c:axId val="-1989725840"/>
+        <c:axId val="-1989723664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1304511760"/>
+        <c:axId val="-1989725840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13638,6 +13686,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -13704,7 +13753,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1304518832"/>
+        <c:crossAx val="-1989723664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13712,7 +13761,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1304518832"/>
+        <c:axId val="-1989723664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13812,7 +13861,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1304511760"/>
+        <c:crossAx val="-1989725840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13836,6 +13885,556 @@
           <c:h val="0.387786093462337"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Distance to compliance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graphs!$AA$128</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>[#previous_year#]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$Z$129:$Z$131</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Collection 
+[#current_year#]  : target 0 p.e.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Secondary treatment 
+[#current_year#]  : target 0 p.e.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tertiary treatment 
+[#current_year#]  : target 0 p.e.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$AA$129:$AA$131</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graphs!$AB$128</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>[#current_year#] </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$Z$129:$Z$131</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Collection 
+[#current_year#]  : target 0 p.e.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Secondary treatment 
+[#current_year#]  : target 0 p.e.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tertiary treatment 
+[#current_year#]  : target 0 p.e.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$AB$129:$AB$131</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-1987466928"/>
+        <c:axId val="-1987469648"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1987466928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1987469648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1987469648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1987466928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13942,6 +14541,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14172,7 +14772,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -14376,6 +14978,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14730,11 +15333,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1304511216"/>
-        <c:axId val="-1304510672"/>
+        <c:axId val="-1989723120"/>
+        <c:axId val="-1989729648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1304511216"/>
+        <c:axId val="-1989723120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14766,6 +15369,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14832,7 +15436,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1304510672"/>
+        <c:crossAx val="-1989729648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14840,7 +15444,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1304510672"/>
+        <c:axId val="-1989729648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14886,6 +15490,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14946,7 +15551,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1304511216"/>
+        <c:crossAx val="-1989723120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15077,6 +15682,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15404,11 +16010,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1416690128"/>
-        <c:axId val="-1416686864"/>
+        <c:axId val="-1989724752"/>
+        <c:axId val="-1989730736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1416690128"/>
+        <c:axId val="-1989724752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15440,6 +16046,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15506,7 +16113,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1416686864"/>
+        <c:crossAx val="-1989730736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15514,7 +16121,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1416686864"/>
+        <c:axId val="-1989730736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15614,7 +16221,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1416690128"/>
+        <c:crossAx val="-1989724752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15745,6 +16352,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16072,11 +16680,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1300264576"/>
-        <c:axId val="-1300262944"/>
+        <c:axId val="-1989716592"/>
+        <c:axId val="-1989727472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1300264576"/>
+        <c:axId val="-1989716592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16108,6 +16716,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16174,7 +16783,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300262944"/>
+        <c:crossAx val="-1989727472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16182,7 +16791,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1300262944"/>
+        <c:axId val="-1989727472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16282,7 +16891,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300264576"/>
+        <c:crossAx val="-1989716592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16418,6 +17027,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16813,11 +17423,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1300274912"/>
-        <c:axId val="-1300271648"/>
+        <c:axId val="-1989720400"/>
+        <c:axId val="-1989726928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1300274912"/>
+        <c:axId val="-1989720400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16860,7 +17470,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300271648"/>
+        <c:crossAx val="-1989726928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16868,7 +17478,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1300271648"/>
+        <c:axId val="-1989726928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16919,6 +17529,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16979,7 +17590,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300274912"/>
+        <c:crossAx val="-1989720400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17509,11 +18120,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1300267840"/>
-        <c:axId val="-1300274368"/>
+        <c:axId val="-1989724208"/>
+        <c:axId val="-1989730192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1300267840"/>
+        <c:axId val="-1989724208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17556,7 +18167,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300274368"/>
+        <c:crossAx val="-1989730192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17564,7 +18175,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1300274368"/>
+        <c:axId val="-1989730192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17683,7 +18294,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300267840"/>
+        <c:crossAx val="-1989724208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17777,6 +18388,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18023,11 +18635,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1300277088"/>
-        <c:axId val="-1300273280"/>
+        <c:axId val="-1989721488"/>
+        <c:axId val="-1989729104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1300277088"/>
+        <c:axId val="-1989721488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18056,6 +18668,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -18122,7 +18735,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300273280"/>
+        <c:crossAx val="-1989729104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18130,7 +18743,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1300273280"/>
+        <c:axId val="-1989729104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -18250,7 +18863,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300277088"/>
+        <c:crossAx val="-1989721488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18820,6 +19433,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors20.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -25208,6 +25861,509 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style20.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -29355,6 +30511,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>260536</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>174812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -29981,23 +31167,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="574" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="690" t="s">
+      <c r="A1" s="694" t="s">
         <v>271</v>
       </c>
-      <c r="B1" s="691"/>
-      <c r="C1" s="691"/>
-      <c r="D1" s="691"/>
+      <c r="B1" s="695"/>
+      <c r="C1" s="695"/>
+      <c r="D1" s="695"/>
       <c r="E1" s="565"/>
-      <c r="F1" s="807" t="s">
+      <c r="F1" s="811" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="808"/>
-      <c r="H1" s="808"/>
+      <c r="G1" s="812"/>
+      <c r="H1" s="812"/>
       <c r="I1" s="570"/>
       <c r="J1" s="255"/>
       <c r="K1" s="570"/>
       <c r="L1" s="256"/>
-      <c r="M1" s="802" t="s">
+      <c r="M1" s="806" t="s">
         <v>272</v>
       </c>
       <c r="N1" s="257"/>
@@ -30009,19 +31195,19 @@
       <c r="R1" s="255"/>
       <c r="S1" s="570"/>
       <c r="T1" s="256"/>
-      <c r="U1" s="802" t="s">
+      <c r="U1" s="806" t="s">
         <v>274</v>
       </c>
       <c r="V1" s="257"/>
-      <c r="W1" s="809" t="s">
+      <c r="W1" s="813" t="s">
         <v>275</v>
       </c>
-      <c r="X1" s="809"/>
-      <c r="Y1" s="809"/>
-      <c r="Z1" s="809"/>
-      <c r="AA1" s="809"/>
-      <c r="AB1" s="810"/>
-      <c r="AC1" s="802" t="s">
+      <c r="X1" s="813"/>
+      <c r="Y1" s="813"/>
+      <c r="Z1" s="813"/>
+      <c r="AA1" s="813"/>
+      <c r="AB1" s="814"/>
+      <c r="AC1" s="806" t="s">
         <v>276</v>
       </c>
     </row>
@@ -30035,52 +31221,52 @@
       <c r="C2" s="569" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="804" t="s">
+      <c r="D2" s="808" t="s">
         <v>454</v>
       </c>
-      <c r="E2" s="804"/>
+      <c r="E2" s="808"/>
       <c r="F2" s="259"/>
-      <c r="G2" s="805" t="s">
+      <c r="G2" s="809" t="s">
         <v>160</v>
       </c>
-      <c r="H2" s="805"/>
-      <c r="I2" s="805" t="s">
+      <c r="H2" s="809"/>
+      <c r="I2" s="809" t="s">
         <v>161</v>
       </c>
-      <c r="J2" s="805"/>
-      <c r="K2" s="805" t="s">
+      <c r="J2" s="809"/>
+      <c r="K2" s="809" t="s">
         <v>162</v>
       </c>
-      <c r="L2" s="806"/>
-      <c r="M2" s="803"/>
+      <c r="L2" s="810"/>
+      <c r="M2" s="807"/>
       <c r="N2" s="260"/>
-      <c r="O2" s="805" t="s">
+      <c r="O2" s="809" t="s">
         <v>160</v>
       </c>
-      <c r="P2" s="805"/>
-      <c r="Q2" s="805" t="s">
+      <c r="P2" s="809"/>
+      <c r="Q2" s="809" t="s">
         <v>161</v>
       </c>
-      <c r="R2" s="805"/>
-      <c r="S2" s="805" t="s">
+      <c r="R2" s="809"/>
+      <c r="S2" s="809" t="s">
         <v>162</v>
       </c>
-      <c r="T2" s="806"/>
-      <c r="U2" s="803"/>
+      <c r="T2" s="810"/>
+      <c r="U2" s="807"/>
       <c r="V2" s="260"/>
-      <c r="W2" s="805" t="s">
+      <c r="W2" s="809" t="s">
         <v>160</v>
       </c>
-      <c r="X2" s="805"/>
-      <c r="Y2" s="805" t="s">
+      <c r="X2" s="809"/>
+      <c r="Y2" s="809" t="s">
         <v>161</v>
       </c>
-      <c r="Z2" s="805"/>
-      <c r="AA2" s="805" t="s">
+      <c r="Z2" s="809"/>
+      <c r="AA2" s="809" t="s">
         <v>162</v>
       </c>
-      <c r="AB2" s="806"/>
-      <c r="AC2" s="803"/>
+      <c r="AB2" s="810"/>
+      <c r="AC2" s="807"/>
     </row>
     <row r="3" spans="1:29" s="589" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A3" s="45"/>
@@ -30449,8 +31635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF178"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="P104" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z132" sqref="Z132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30475,35 +31661,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="811" t="s">
+      <c r="A1" s="815" t="s">
         <v>437</v>
       </c>
-      <c r="B1" s="812"/>
-      <c r="C1" s="812"/>
+      <c r="B1" s="816"/>
+      <c r="C1" s="816"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="820" t="s">
+      <c r="A3" s="824" t="s">
         <v>319</v>
       </c>
-      <c r="B3" s="822" t="s">
+      <c r="B3" s="826" t="s">
         <v>411</v>
       </c>
-      <c r="C3" s="823"/>
-      <c r="D3" s="818" t="s">
+      <c r="C3" s="827"/>
+      <c r="D3" s="822" t="s">
         <v>438</v>
       </c>
-      <c r="E3" s="819"/>
-      <c r="AA3" s="835" t="s">
+      <c r="E3" s="823"/>
+      <c r="AA3" s="839" t="s">
         <v>332</v>
       </c>
-      <c r="AB3" s="835"/>
-      <c r="AC3" s="835" t="s">
+      <c r="AB3" s="839"/>
+      <c r="AC3" s="839" t="s">
         <v>416</v>
       </c>
-      <c r="AD3" s="835"/>
+      <c r="AD3" s="839"/>
     </row>
     <row r="4" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="821"/>
+      <c r="A4" s="825"/>
       <c r="B4" s="311" t="s">
         <v>415</v>
       </c>
@@ -30646,14 +31832,14 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="Z10" s="363"/>
-      <c r="AA10" s="835" t="s">
+      <c r="AA10" s="839" t="s">
         <v>417</v>
       </c>
-      <c r="AB10" s="835"/>
-      <c r="AC10" s="835" t="s">
+      <c r="AB10" s="839"/>
+      <c r="AC10" s="839" t="s">
         <v>418</v>
       </c>
-      <c r="AD10" s="835"/>
+      <c r="AD10" s="839"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="Z11" s="363" t="s">
@@ -30698,7 +31884,7 @@
       </c>
     </row>
     <row r="13" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="820" t="s">
+      <c r="A13" s="824" t="s">
         <v>320</v>
       </c>
       <c r="B13" s="310" t="str">
@@ -30730,7 +31916,7 @@
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="821"/>
+      <c r="A14" s="825"/>
       <c r="B14" s="313" t="s">
         <v>321</v>
       </c>
@@ -30816,27 +32002,27 @@
       <c r="A21" t="s">
         <v>422</v>
       </c>
-      <c r="B21" s="813" t="s">
+      <c r="B21" s="817" t="s">
         <v>431</v>
       </c>
-      <c r="C21" s="813"/>
-      <c r="D21" s="813"/>
-      <c r="E21" s="813"/>
+      <c r="C21" s="817"/>
+      <c r="D21" s="817"/>
+      <c r="E21" s="817"/>
     </row>
     <row r="22" spans="1:32" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="315" t="s">
         <v>283</v>
       </c>
-      <c r="B22" s="824" t="str">
+      <c r="B22" s="828" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C22" s="825"/>
-      <c r="D22" s="824" t="str">
+      <c r="C22" s="829"/>
+      <c r="D22" s="828" t="str">
         <f>D3</f>
         <v>[#previous_year#]*</v>
       </c>
-      <c r="E22" s="825"/>
+      <c r="E22" s="829"/>
     </row>
     <row r="23" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="316"/>
@@ -31211,16 +32397,16 @@
       <c r="A41" s="318" t="s">
         <v>330</v>
       </c>
-      <c r="B41" s="814" t="str">
+      <c r="B41" s="818" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C41" s="815"/>
-      <c r="D41" s="816" t="str">
+      <c r="C41" s="819"/>
+      <c r="D41" s="820" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E41" s="817"/>
+      <c r="E41" s="821"/>
       <c r="AA41" t="s">
         <v>412</v>
       </c>
@@ -31370,11 +32556,11 @@
       <c r="AA48" t="s">
         <v>422</v>
       </c>
-      <c r="AB48" s="813" t="s">
+      <c r="AB48" s="817" t="s">
         <v>443</v>
       </c>
-      <c r="AC48" s="813"/>
-      <c r="AD48" s="813"/>
+      <c r="AC48" s="817"/>
+      <c r="AD48" s="817"/>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" s="384" t="s">
@@ -31648,11 +32834,11 @@
       <c r="AA62" t="s">
         <v>422</v>
       </c>
-      <c r="AB62" s="813" t="s">
+      <c r="AB62" s="817" t="s">
         <v>444</v>
       </c>
-      <c r="AC62" s="813"/>
-      <c r="AD62" s="813"/>
+      <c r="AC62" s="817"/>
+      <c r="AD62" s="817"/>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A63" s="312"/>
@@ -31887,12 +33073,12 @@
       <c r="A74" s="530" t="s">
         <v>426</v>
       </c>
-      <c r="B74" s="813" t="s">
+      <c r="B74" s="817" t="s">
         <v>427</v>
       </c>
-      <c r="C74" s="813"/>
-      <c r="D74" s="813"/>
-      <c r="E74" s="813"/>
+      <c r="C74" s="817"/>
+      <c r="D74" s="817"/>
+      <c r="E74" s="817"/>
     </row>
     <row r="75" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="333" t="s">
@@ -32185,16 +33371,16 @@
       </c>
     </row>
     <row r="85" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B85" s="828" t="str">
+      <c r="B85" s="832" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C85" s="829"/>
-      <c r="D85" s="828" t="str">
+      <c r="C85" s="833"/>
+      <c r="D85" s="832" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E85" s="829"/>
+      <c r="E85" s="833"/>
       <c r="Z85" t="s">
         <v>401</v>
       </c>
@@ -32208,14 +33394,14 @@
     </row>
     <row r="86" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="201"/>
-      <c r="B86" s="830" t="s">
+      <c r="B86" s="834" t="s">
         <v>233</v>
       </c>
-      <c r="C86" s="777"/>
-      <c r="D86" s="830" t="s">
+      <c r="C86" s="781"/>
+      <c r="D86" s="834" t="s">
         <v>233</v>
       </c>
-      <c r="E86" s="777"/>
+      <c r="E86" s="781"/>
       <c r="Z86" s="341" t="s">
         <v>234</v>
       </c>
@@ -32421,27 +33607,27 @@
       </c>
     </row>
     <row r="101" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B101" s="828" t="str">
+      <c r="B101" s="832" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C101" s="829"/>
-      <c r="D101" s="828" t="str">
+      <c r="C101" s="833"/>
+      <c r="D101" s="832" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E101" s="829"/>
+      <c r="E101" s="833"/>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A102" s="201"/>
-      <c r="B102" s="830" t="s">
+      <c r="B102" s="834" t="s">
         <v>233</v>
       </c>
-      <c r="C102" s="777"/>
-      <c r="D102" s="830" t="s">
+      <c r="C102" s="781"/>
+      <c r="D102" s="834" t="s">
         <v>233</v>
       </c>
-      <c r="E102" s="777"/>
+      <c r="E102" s="781"/>
       <c r="Z102" t="s">
         <v>401</v>
       </c>
@@ -32655,27 +33841,27 @@
       </c>
     </row>
     <row r="116" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B116" s="831" t="str">
+      <c r="B116" s="835" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C116" s="832"/>
-      <c r="D116" s="831" t="str">
+      <c r="C116" s="836"/>
+      <c r="D116" s="835" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E116" s="832"/>
+      <c r="E116" s="836"/>
     </row>
     <row r="117" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A117" s="346"/>
-      <c r="B117" s="833" t="s">
+      <c r="B117" s="837" t="s">
         <v>233</v>
       </c>
-      <c r="C117" s="834"/>
-      <c r="D117" s="833" t="s">
+      <c r="C117" s="838"/>
+      <c r="D117" s="837" t="s">
         <v>233</v>
       </c>
-      <c r="E117" s="834"/>
+      <c r="E117" s="838"/>
       <c r="Z117" t="s">
         <v>401</v>
       </c>
@@ -32891,18 +34077,44 @@
       <c r="D127" s="488"/>
       <c r="E127" s="319"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z128" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA128" s="537" t="s">
+        <v>409</v>
+      </c>
+      <c r="AB128" s="689" t="str">
+        <f>B3</f>
+        <v xml:space="preserve">[#current_year#] </v>
+      </c>
+    </row>
+    <row r="129" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="350" t="s">
         <v>320</v>
       </c>
-      <c r="B129" s="826" t="str">
+      <c r="B129" s="830" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C129" s="827"/>
-      <c r="D129" s="827"/>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C129" s="831"/>
+      <c r="D129" s="831"/>
+      <c r="Z129" t="str">
+        <f>CONCATENATE("Collection 
+", B3, " : target ", AB118, " p.e.")</f>
+        <v>Collection 
+[#current_year#]  : target 0 p.e.</v>
+      </c>
+      <c r="AA129" s="364">
+        <f>E120</f>
+        <v>0</v>
+      </c>
+      <c r="AB129" s="364">
+        <f>C120</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="351"/>
       <c r="B130" s="352" t="s">
         <v>124</v>
@@ -32913,8 +34125,22 @@
       <c r="D130" s="353" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="Z130" t="str">
+        <f>CONCATENATE("Secondary treatment 
+", B3, " : target ", AB120, " p.e.")</f>
+        <v>Secondary treatment 
+[#current_year#]  : target 0 p.e.</v>
+      </c>
+      <c r="AA130" s="364">
+        <f>E122+E123</f>
+        <v>0</v>
+      </c>
+      <c r="AB130" s="364">
+        <f>C122+C123</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="354" t="s">
         <v>361</v>
       </c>
@@ -32923,8 +34149,22 @@
       </c>
       <c r="C131" s="375"/>
       <c r="D131" s="486"/>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="Z131" t="str">
+        <f>CONCATENATE("Tertiary treatment 
+", B3, " : target ", AB123, " p.e.")</f>
+        <v>Tertiary treatment 
+[#current_year#]  : target 0 p.e.</v>
+      </c>
+      <c r="AA131" s="364">
+        <f>E125+E126</f>
+        <v>0</v>
+      </c>
+      <c r="AB131" s="364">
+        <f>C125+C126</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A132" s="312" t="s">
         <v>362</v>
       </c>
@@ -32932,7 +34172,7 @@
       <c r="C132" s="319"/>
       <c r="D132" s="396"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A133" s="312" t="s">
         <v>236</v>
       </c>
@@ -32940,7 +34180,7 @@
       <c r="C133" s="319"/>
       <c r="D133" s="396"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A134" s="312" t="s">
         <v>363</v>
       </c>
@@ -32948,7 +34188,7 @@
       <c r="C134" s="319"/>
       <c r="D134" s="396"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A135" s="312" t="s">
         <v>364</v>
       </c>
@@ -32956,7 +34196,7 @@
       <c r="C135" s="319"/>
       <c r="D135" s="396"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A136" s="312" t="s">
         <v>365</v>
       </c>
@@ -32964,7 +34204,7 @@
       <c r="C136" s="319"/>
       <c r="D136" s="396"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A137" s="312" t="s">
         <v>366</v>
       </c>
@@ -32972,7 +34212,7 @@
       <c r="C137" s="319"/>
       <c r="D137" s="396"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A138" s="312" t="s">
         <v>367</v>
       </c>
@@ -32980,7 +34220,7 @@
       <c r="C138" s="319"/>
       <c r="D138" s="396"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A139" s="312" t="s">
         <v>368</v>
       </c>
@@ -32988,7 +34228,7 @@
       <c r="C139" s="319"/>
       <c r="D139" s="396"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B140" s="355"/>
     </row>
     <row r="147" spans="1:29" ht="31.5" x14ac:dyDescent="0.25">
@@ -33882,7 +35122,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33985,54 +35225,54 @@
       <c r="AR3" s="5"/>
     </row>
     <row r="4" spans="1:44" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="686" t="s">
+      <c r="A4" s="690" t="s">
         <v>448</v>
       </c>
-      <c r="B4" s="687"/>
-      <c r="C4" s="687"/>
-      <c r="D4" s="687"/>
-      <c r="E4" s="688"/>
-      <c r="F4" s="688"/>
-      <c r="G4" s="688"/>
-      <c r="H4" s="688"/>
-      <c r="I4" s="688"/>
-      <c r="J4" s="688"/>
-      <c r="K4" s="688"/>
-      <c r="L4" s="688"/>
-      <c r="M4" s="688"/>
-      <c r="N4" s="688"/>
-      <c r="O4" s="688"/>
-      <c r="P4" s="688"/>
-      <c r="Q4" s="688"/>
-      <c r="R4" s="688"/>
-      <c r="S4" s="688"/>
-      <c r="T4" s="688"/>
-      <c r="U4" s="688"/>
-      <c r="V4" s="688"/>
-      <c r="W4" s="688"/>
-      <c r="X4" s="688"/>
-      <c r="Y4" s="688"/>
-      <c r="Z4" s="688"/>
-      <c r="AA4" s="688"/>
-      <c r="AB4" s="688"/>
-      <c r="AC4" s="688"/>
-      <c r="AD4" s="688"/>
-      <c r="AE4" s="688"/>
-      <c r="AF4" s="688"/>
-      <c r="AG4" s="688"/>
-      <c r="AH4" s="688"/>
-      <c r="AI4" s="688"/>
-      <c r="AJ4" s="688"/>
-      <c r="AK4" s="688"/>
-      <c r="AL4" s="688"/>
-      <c r="AM4" s="688"/>
-      <c r="AN4" s="688"/>
-      <c r="AO4" s="688"/>
-      <c r="AP4" s="688"/>
-      <c r="AQ4" s="689" t="s">
+      <c r="B4" s="691"/>
+      <c r="C4" s="691"/>
+      <c r="D4" s="691"/>
+      <c r="E4" s="692"/>
+      <c r="F4" s="692"/>
+      <c r="G4" s="692"/>
+      <c r="H4" s="692"/>
+      <c r="I4" s="692"/>
+      <c r="J4" s="692"/>
+      <c r="K4" s="692"/>
+      <c r="L4" s="692"/>
+      <c r="M4" s="692"/>
+      <c r="N4" s="692"/>
+      <c r="O4" s="692"/>
+      <c r="P4" s="692"/>
+      <c r="Q4" s="692"/>
+      <c r="R4" s="692"/>
+      <c r="S4" s="692"/>
+      <c r="T4" s="692"/>
+      <c r="U4" s="692"/>
+      <c r="V4" s="692"/>
+      <c r="W4" s="692"/>
+      <c r="X4" s="692"/>
+      <c r="Y4" s="692"/>
+      <c r="Z4" s="692"/>
+      <c r="AA4" s="692"/>
+      <c r="AB4" s="692"/>
+      <c r="AC4" s="692"/>
+      <c r="AD4" s="692"/>
+      <c r="AE4" s="692"/>
+      <c r="AF4" s="692"/>
+      <c r="AG4" s="692"/>
+      <c r="AH4" s="692"/>
+      <c r="AI4" s="692"/>
+      <c r="AJ4" s="692"/>
+      <c r="AK4" s="692"/>
+      <c r="AL4" s="692"/>
+      <c r="AM4" s="692"/>
+      <c r="AN4" s="692"/>
+      <c r="AO4" s="692"/>
+      <c r="AP4" s="692"/>
+      <c r="AQ4" s="693" t="s">
         <v>2</v>
       </c>
-      <c r="AR4" s="689"/>
+      <c r="AR4" s="693"/>
     </row>
     <row r="5" spans="1:44" s="573" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="299" t="s">
@@ -34194,7 +35434,7 @@
   <dimension ref="A1:CQ16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
@@ -34220,123 +35460,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" s="574" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="690" t="s">
+      <c r="A1" s="694" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="691"/>
-      <c r="C1" s="691"/>
-      <c r="D1" s="691"/>
-      <c r="E1" s="691"/>
-      <c r="F1" s="691"/>
-      <c r="G1" s="691"/>
-      <c r="H1" s="692" t="s">
+      <c r="B1" s="695"/>
+      <c r="C1" s="695"/>
+      <c r="D1" s="695"/>
+      <c r="E1" s="695"/>
+      <c r="F1" s="695"/>
+      <c r="G1" s="695"/>
+      <c r="H1" s="696" t="s">
         <v>138</v>
       </c>
-      <c r="I1" s="693"/>
-      <c r="J1" s="693"/>
-      <c r="K1" s="693"/>
-      <c r="L1" s="693"/>
-      <c r="M1" s="694"/>
-      <c r="N1" s="695" t="s">
+      <c r="I1" s="697"/>
+      <c r="J1" s="697"/>
+      <c r="K1" s="697"/>
+      <c r="L1" s="697"/>
+      <c r="M1" s="698"/>
+      <c r="N1" s="699" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="696"/>
-      <c r="P1" s="696"/>
-      <c r="Q1" s="697"/>
-      <c r="R1" s="697"/>
-      <c r="S1" s="696"/>
-      <c r="T1" s="696"/>
-      <c r="U1" s="696"/>
-      <c r="V1" s="698" t="s">
+      <c r="O1" s="700"/>
+      <c r="P1" s="700"/>
+      <c r="Q1" s="701"/>
+      <c r="R1" s="701"/>
+      <c r="S1" s="700"/>
+      <c r="T1" s="700"/>
+      <c r="U1" s="700"/>
+      <c r="V1" s="702" t="s">
         <v>49</v>
       </c>
-      <c r="W1" s="699"/>
-      <c r="X1" s="700"/>
-      <c r="Y1" s="700"/>
-      <c r="Z1" s="701"/>
-      <c r="AA1" s="702" t="s">
+      <c r="W1" s="703"/>
+      <c r="X1" s="704"/>
+      <c r="Y1" s="704"/>
+      <c r="Z1" s="705"/>
+      <c r="AA1" s="706" t="s">
         <v>50</v>
       </c>
-      <c r="AB1" s="703"/>
-      <c r="AC1" s="703"/>
-      <c r="AD1" s="703"/>
-      <c r="AE1" s="703"/>
-      <c r="AF1" s="703"/>
-      <c r="AG1" s="703"/>
-      <c r="AH1" s="703"/>
-      <c r="AI1" s="703"/>
-      <c r="AJ1" s="703"/>
-      <c r="AK1" s="703"/>
-      <c r="AL1" s="703"/>
-      <c r="AM1" s="703"/>
+      <c r="AB1" s="707"/>
+      <c r="AC1" s="707"/>
+      <c r="AD1" s="707"/>
+      <c r="AE1" s="707"/>
+      <c r="AF1" s="707"/>
+      <c r="AG1" s="707"/>
+      <c r="AH1" s="707"/>
+      <c r="AI1" s="707"/>
+      <c r="AJ1" s="707"/>
+      <c r="AK1" s="707"/>
+      <c r="AL1" s="707"/>
+      <c r="AM1" s="707"/>
       <c r="AN1" s="7"/>
       <c r="AO1" s="8"/>
-      <c r="AP1" s="715" t="s">
+      <c r="AP1" s="719" t="s">
         <v>51</v>
       </c>
-      <c r="AQ1" s="696"/>
-      <c r="AR1" s="696"/>
-      <c r="AS1" s="696"/>
-      <c r="AT1" s="696"/>
-      <c r="AU1" s="696"/>
-      <c r="AV1" s="696"/>
-      <c r="AW1" s="716"/>
-      <c r="AX1" s="723" t="s">
+      <c r="AQ1" s="700"/>
+      <c r="AR1" s="700"/>
+      <c r="AS1" s="700"/>
+      <c r="AT1" s="700"/>
+      <c r="AU1" s="700"/>
+      <c r="AV1" s="700"/>
+      <c r="AW1" s="720"/>
+      <c r="AX1" s="727" t="s">
         <v>52</v>
       </c>
-      <c r="AY1" s="724"/>
-      <c r="AZ1" s="724"/>
-      <c r="BA1" s="724"/>
-      <c r="BB1" s="724"/>
-      <c r="BC1" s="725"/>
-      <c r="BD1" s="726" t="s">
+      <c r="AY1" s="728"/>
+      <c r="AZ1" s="728"/>
+      <c r="BA1" s="728"/>
+      <c r="BB1" s="728"/>
+      <c r="BC1" s="729"/>
+      <c r="BD1" s="730" t="s">
         <v>53</v>
       </c>
-      <c r="BE1" s="727"/>
-      <c r="BF1" s="727"/>
-      <c r="BG1" s="727"/>
-      <c r="BH1" s="727"/>
-      <c r="BI1" s="728"/>
-      <c r="BJ1" s="729" t="s">
+      <c r="BE1" s="731"/>
+      <c r="BF1" s="731"/>
+      <c r="BG1" s="731"/>
+      <c r="BH1" s="731"/>
+      <c r="BI1" s="732"/>
+      <c r="BJ1" s="733" t="s">
         <v>54</v>
       </c>
-      <c r="BK1" s="730"/>
-      <c r="BL1" s="730"/>
-      <c r="BM1" s="730"/>
-      <c r="BN1" s="730"/>
-      <c r="BO1" s="730"/>
-      <c r="BP1" s="731"/>
-      <c r="BQ1" s="704" t="s">
+      <c r="BK1" s="734"/>
+      <c r="BL1" s="734"/>
+      <c r="BM1" s="734"/>
+      <c r="BN1" s="734"/>
+      <c r="BO1" s="734"/>
+      <c r="BP1" s="735"/>
+      <c r="BQ1" s="708" t="s">
         <v>55</v>
       </c>
-      <c r="BR1" s="705"/>
-      <c r="BS1" s="705"/>
-      <c r="BT1" s="705"/>
-      <c r="BU1" s="705"/>
-      <c r="BV1" s="705"/>
+      <c r="BR1" s="709"/>
+      <c r="BS1" s="709"/>
+      <c r="BT1" s="709"/>
+      <c r="BU1" s="709"/>
+      <c r="BV1" s="709"/>
       <c r="BW1" s="8"/>
       <c r="BX1" s="9"/>
-      <c r="BY1" s="706" t="s">
+      <c r="BY1" s="710" t="s">
         <v>56</v>
       </c>
-      <c r="BZ1" s="707"/>
-      <c r="CA1" s="707"/>
-      <c r="CB1" s="707"/>
-      <c r="CC1" s="707"/>
-      <c r="CD1" s="707"/>
-      <c r="CE1" s="707"/>
-      <c r="CF1" s="708"/>
-      <c r="CG1" s="708"/>
-      <c r="CH1" s="708"/>
-      <c r="CI1" s="708"/>
-      <c r="CJ1" s="708"/>
-      <c r="CK1" s="708"/>
-      <c r="CL1" s="708"/>
-      <c r="CM1" s="708"/>
-      <c r="CN1" s="708"/>
-      <c r="CO1" s="708"/>
-      <c r="CP1" s="708"/>
-      <c r="CQ1" s="708"/>
+      <c r="BZ1" s="711"/>
+      <c r="CA1" s="711"/>
+      <c r="CB1" s="711"/>
+      <c r="CC1" s="711"/>
+      <c r="CD1" s="711"/>
+      <c r="CE1" s="711"/>
+      <c r="CF1" s="712"/>
+      <c r="CG1" s="712"/>
+      <c r="CH1" s="712"/>
+      <c r="CI1" s="712"/>
+      <c r="CJ1" s="712"/>
+      <c r="CK1" s="712"/>
+      <c r="CL1" s="712"/>
+      <c r="CM1" s="712"/>
+      <c r="CN1" s="712"/>
+      <c r="CO1" s="712"/>
+      <c r="CP1" s="712"/>
+      <c r="CQ1" s="712"/>
     </row>
     <row r="2" spans="1:95" s="574" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -34360,18 +35600,18 @@
       <c r="G2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="709" t="s">
+      <c r="H2" s="713" t="s">
         <v>155</v>
       </c>
-      <c r="I2" s="710"/>
-      <c r="J2" s="710" t="s">
+      <c r="I2" s="714"/>
+      <c r="J2" s="714" t="s">
         <v>64</v>
       </c>
-      <c r="K2" s="710"/>
-      <c r="L2" s="710" t="s">
+      <c r="K2" s="714"/>
+      <c r="L2" s="714" t="s">
         <v>65</v>
       </c>
-      <c r="M2" s="711"/>
+      <c r="M2" s="715"/>
       <c r="N2" s="12" t="s">
         <v>57</v>
       </c>
@@ -34480,36 +35720,36 @@
       <c r="AW2" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="AX2" s="712" t="s">
+      <c r="AX2" s="716" t="s">
         <v>90</v>
       </c>
-      <c r="AY2" s="713"/>
-      <c r="AZ2" s="713"/>
-      <c r="BA2" s="713" t="s">
+      <c r="AY2" s="717"/>
+      <c r="AZ2" s="717"/>
+      <c r="BA2" s="717" t="s">
         <v>91</v>
       </c>
-      <c r="BB2" s="713"/>
-      <c r="BC2" s="714"/>
-      <c r="BD2" s="717" t="s">
+      <c r="BB2" s="717"/>
+      <c r="BC2" s="718"/>
+      <c r="BD2" s="721" t="s">
         <v>90</v>
       </c>
-      <c r="BE2" s="718"/>
-      <c r="BF2" s="718"/>
-      <c r="BG2" s="718" t="s">
+      <c r="BE2" s="722"/>
+      <c r="BF2" s="722"/>
+      <c r="BG2" s="722" t="s">
         <v>91</v>
       </c>
-      <c r="BH2" s="718"/>
-      <c r="BI2" s="719"/>
-      <c r="BJ2" s="720" t="s">
+      <c r="BH2" s="722"/>
+      <c r="BI2" s="723"/>
+      <c r="BJ2" s="724" t="s">
         <v>90</v>
       </c>
-      <c r="BK2" s="721"/>
-      <c r="BL2" s="721"/>
-      <c r="BM2" s="721" t="s">
+      <c r="BK2" s="725"/>
+      <c r="BL2" s="725"/>
+      <c r="BM2" s="725" t="s">
         <v>91</v>
       </c>
-      <c r="BN2" s="722"/>
-      <c r="BO2" s="722"/>
+      <c r="BN2" s="726"/>
+      <c r="BO2" s="726"/>
       <c r="BP2" s="24" t="s">
         <v>92</v>
       </c>
@@ -35550,7 +36790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CV51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -35622,124 +36862,124 @@
         <v>135</v>
       </c>
       <c r="L1" s="42"/>
-      <c r="M1" s="736" t="s">
+      <c r="M1" s="740" t="s">
         <v>136</v>
       </c>
-      <c r="N1" s="737" t="s">
+      <c r="N1" s="741" t="s">
         <v>137</v>
       </c>
-      <c r="O1" s="738"/>
-      <c r="P1" s="738"/>
-      <c r="Q1" s="738"/>
-      <c r="R1" s="739" t="s">
+      <c r="O1" s="742"/>
+      <c r="P1" s="742"/>
+      <c r="Q1" s="742"/>
+      <c r="R1" s="743" t="s">
         <v>138</v>
       </c>
-      <c r="S1" s="740"/>
-      <c r="T1" s="740"/>
-      <c r="U1" s="740"/>
-      <c r="V1" s="740"/>
-      <c r="W1" s="740"/>
-      <c r="X1" s="741"/>
-      <c r="Y1" s="742" t="s">
+      <c r="S1" s="744"/>
+      <c r="T1" s="744"/>
+      <c r="U1" s="744"/>
+      <c r="V1" s="744"/>
+      <c r="W1" s="744"/>
+      <c r="X1" s="745"/>
+      <c r="Y1" s="746" t="s">
         <v>139</v>
       </c>
-      <c r="Z1" s="743"/>
-      <c r="AA1" s="746" t="s">
+      <c r="Z1" s="747"/>
+      <c r="AA1" s="750" t="s">
         <v>140</v>
       </c>
-      <c r="AB1" s="748" t="s">
+      <c r="AB1" s="752" t="s">
         <v>141</v>
       </c>
-      <c r="AC1" s="756" t="s">
+      <c r="AC1" s="760" t="s">
         <v>457</v>
       </c>
-      <c r="AD1" s="757"/>
-      <c r="AE1" s="757"/>
-      <c r="AF1" s="758"/>
-      <c r="AG1" s="759" t="s">
+      <c r="AD1" s="761"/>
+      <c r="AE1" s="761"/>
+      <c r="AF1" s="762"/>
+      <c r="AG1" s="763" t="s">
         <v>142</v>
       </c>
-      <c r="AH1" s="740"/>
-      <c r="AI1" s="740"/>
-      <c r="AJ1" s="740"/>
-      <c r="AK1" s="740"/>
-      <c r="AL1" s="740"/>
-      <c r="AM1" s="740"/>
-      <c r="AN1" s="740"/>
-      <c r="AO1" s="748" t="s">
+      <c r="AH1" s="744"/>
+      <c r="AI1" s="744"/>
+      <c r="AJ1" s="744"/>
+      <c r="AK1" s="744"/>
+      <c r="AL1" s="744"/>
+      <c r="AM1" s="744"/>
+      <c r="AN1" s="744"/>
+      <c r="AO1" s="752" t="s">
         <v>143</v>
       </c>
-      <c r="AP1" s="742" t="s">
+      <c r="AP1" s="746" t="s">
         <v>144</v>
       </c>
-      <c r="AQ1" s="743"/>
-      <c r="AR1" s="743"/>
-      <c r="AS1" s="728"/>
-      <c r="AT1" s="760" t="s">
+      <c r="AQ1" s="747"/>
+      <c r="AR1" s="747"/>
+      <c r="AS1" s="732"/>
+      <c r="AT1" s="764" t="s">
         <v>145</v>
       </c>
-      <c r="AU1" s="761"/>
-      <c r="AV1" s="761"/>
-      <c r="AW1" s="761"/>
-      <c r="AX1" s="761"/>
-      <c r="AY1" s="761"/>
-      <c r="AZ1" s="761"/>
-      <c r="BA1" s="761"/>
-      <c r="BB1" s="761"/>
-      <c r="BC1" s="761"/>
-      <c r="BD1" s="761"/>
-      <c r="BE1" s="761"/>
-      <c r="BF1" s="761"/>
-      <c r="BG1" s="761"/>
-      <c r="BH1" s="761"/>
-      <c r="BI1" s="761"/>
-      <c r="BJ1" s="761"/>
-      <c r="BK1" s="761"/>
-      <c r="BL1" s="761"/>
-      <c r="BM1" s="761"/>
-      <c r="BN1" s="761"/>
-      <c r="BO1" s="761"/>
-      <c r="BP1" s="761"/>
-      <c r="BQ1" s="761"/>
-      <c r="BR1" s="761"/>
-      <c r="BS1" s="761"/>
-      <c r="BT1" s="761"/>
-      <c r="BU1" s="761"/>
-      <c r="BV1" s="761"/>
-      <c r="BW1" s="748" t="s">
+      <c r="AU1" s="765"/>
+      <c r="AV1" s="765"/>
+      <c r="AW1" s="765"/>
+      <c r="AX1" s="765"/>
+      <c r="AY1" s="765"/>
+      <c r="AZ1" s="765"/>
+      <c r="BA1" s="765"/>
+      <c r="BB1" s="765"/>
+      <c r="BC1" s="765"/>
+      <c r="BD1" s="765"/>
+      <c r="BE1" s="765"/>
+      <c r="BF1" s="765"/>
+      <c r="BG1" s="765"/>
+      <c r="BH1" s="765"/>
+      <c r="BI1" s="765"/>
+      <c r="BJ1" s="765"/>
+      <c r="BK1" s="765"/>
+      <c r="BL1" s="765"/>
+      <c r="BM1" s="765"/>
+      <c r="BN1" s="765"/>
+      <c r="BO1" s="765"/>
+      <c r="BP1" s="765"/>
+      <c r="BQ1" s="765"/>
+      <c r="BR1" s="765"/>
+      <c r="BS1" s="765"/>
+      <c r="BT1" s="765"/>
+      <c r="BU1" s="765"/>
+      <c r="BV1" s="765"/>
+      <c r="BW1" s="752" t="s">
         <v>146</v>
       </c>
-      <c r="BX1" s="742" t="s">
+      <c r="BX1" s="746" t="s">
         <v>147</v>
       </c>
-      <c r="BY1" s="743"/>
-      <c r="BZ1" s="743"/>
-      <c r="CA1" s="728"/>
-      <c r="CB1" s="750" t="s">
+      <c r="BY1" s="747"/>
+      <c r="BZ1" s="747"/>
+      <c r="CA1" s="732"/>
+      <c r="CB1" s="754" t="s">
         <v>50</v>
       </c>
-      <c r="CC1" s="750"/>
-      <c r="CD1" s="750"/>
-      <c r="CE1" s="750"/>
-      <c r="CF1" s="750"/>
-      <c r="CG1" s="750"/>
-      <c r="CH1" s="750"/>
-      <c r="CI1" s="750"/>
-      <c r="CJ1" s="750"/>
-      <c r="CK1" s="750"/>
-      <c r="CL1" s="750"/>
-      <c r="CM1" s="750"/>
+      <c r="CC1" s="754"/>
+      <c r="CD1" s="754"/>
+      <c r="CE1" s="754"/>
+      <c r="CF1" s="754"/>
+      <c r="CG1" s="754"/>
+      <c r="CH1" s="754"/>
+      <c r="CI1" s="754"/>
+      <c r="CJ1" s="754"/>
+      <c r="CK1" s="754"/>
+      <c r="CL1" s="754"/>
+      <c r="CM1" s="754"/>
       <c r="CN1" s="43"/>
-      <c r="CO1" s="751" t="s">
+      <c r="CO1" s="755" t="s">
         <v>55</v>
       </c>
-      <c r="CP1" s="697"/>
-      <c r="CQ1" s="697"/>
-      <c r="CR1" s="697"/>
-      <c r="CS1" s="697"/>
-      <c r="CT1" s="697"/>
-      <c r="CU1" s="697"/>
-      <c r="CV1" s="716"/>
+      <c r="CP1" s="701"/>
+      <c r="CQ1" s="701"/>
+      <c r="CR1" s="701"/>
+      <c r="CS1" s="701"/>
+      <c r="CT1" s="701"/>
+      <c r="CU1" s="701"/>
+      <c r="CV1" s="720"/>
     </row>
     <row r="2" spans="1:100" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
@@ -35778,7 +37018,7 @@
       <c r="L2" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="M2" s="736"/>
+      <c r="M2" s="740"/>
       <c r="N2" s="49" t="s">
         <v>152</v>
       </c>
@@ -35794,22 +37034,22 @@
       <c r="R2" s="579" t="s">
         <v>397</v>
       </c>
-      <c r="S2" s="752" t="s">
+      <c r="S2" s="756" t="s">
         <v>155</v>
       </c>
-      <c r="T2" s="722"/>
-      <c r="U2" s="753" t="s">
+      <c r="T2" s="726"/>
+      <c r="U2" s="757" t="s">
         <v>64</v>
       </c>
-      <c r="V2" s="753"/>
-      <c r="W2" s="753" t="s">
+      <c r="V2" s="757"/>
+      <c r="W2" s="757" t="s">
         <v>65</v>
       </c>
-      <c r="X2" s="754"/>
-      <c r="Y2" s="744"/>
-      <c r="Z2" s="745"/>
-      <c r="AA2" s="747"/>
-      <c r="AB2" s="749"/>
+      <c r="X2" s="758"/>
+      <c r="Y2" s="748"/>
+      <c r="Z2" s="749"/>
+      <c r="AA2" s="751"/>
+      <c r="AB2" s="753"/>
       <c r="AC2" s="50" t="s">
         <v>156</v>
       </c>
@@ -35822,81 +37062,81 @@
       <c r="AF2" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="AG2" s="755" t="s">
+      <c r="AG2" s="759" t="s">
         <v>160</v>
       </c>
-      <c r="AH2" s="734"/>
-      <c r="AI2" s="734" t="s">
+      <c r="AH2" s="738"/>
+      <c r="AI2" s="738" t="s">
         <v>161</v>
       </c>
-      <c r="AJ2" s="734"/>
-      <c r="AK2" s="734" t="s">
+      <c r="AJ2" s="738"/>
+      <c r="AK2" s="738" t="s">
         <v>162</v>
       </c>
-      <c r="AL2" s="734"/>
+      <c r="AL2" s="738"/>
       <c r="AM2" s="51" t="s">
         <v>461</v>
       </c>
       <c r="AN2" s="51" t="s">
         <v>462</v>
       </c>
-      <c r="AO2" s="749"/>
-      <c r="AP2" s="744" t="s">
+      <c r="AO2" s="753"/>
+      <c r="AP2" s="748" t="s">
         <v>163</v>
       </c>
-      <c r="AQ2" s="745"/>
-      <c r="AR2" s="732" t="s">
+      <c r="AQ2" s="749"/>
+      <c r="AR2" s="736" t="s">
         <v>164</v>
       </c>
-      <c r="AS2" s="733"/>
-      <c r="AT2" s="734" t="s">
+      <c r="AS2" s="737"/>
+      <c r="AT2" s="738" t="s">
         <v>165</v>
       </c>
-      <c r="AU2" s="734"/>
-      <c r="AV2" s="735" t="s">
+      <c r="AU2" s="738"/>
+      <c r="AV2" s="739" t="s">
         <v>166</v>
       </c>
-      <c r="AW2" s="735"/>
-      <c r="AX2" s="735" t="s">
+      <c r="AW2" s="739"/>
+      <c r="AX2" s="739" t="s">
         <v>167</v>
       </c>
-      <c r="AY2" s="735"/>
+      <c r="AY2" s="739"/>
       <c r="AZ2" s="51" t="s">
         <v>463</v>
       </c>
       <c r="BA2" s="51" t="s">
         <v>464</v>
       </c>
-      <c r="BB2" s="734" t="s">
+      <c r="BB2" s="738" t="s">
         <v>168</v>
       </c>
-      <c r="BC2" s="734"/>
-      <c r="BD2" s="735" t="s">
+      <c r="BC2" s="738"/>
+      <c r="BD2" s="739" t="s">
         <v>169</v>
       </c>
-      <c r="BE2" s="735"/>
-      <c r="BF2" s="735" t="s">
+      <c r="BE2" s="739"/>
+      <c r="BF2" s="739" t="s">
         <v>170</v>
       </c>
-      <c r="BG2" s="735"/>
+      <c r="BG2" s="739"/>
       <c r="BH2" s="51" t="s">
         <v>465</v>
       </c>
       <c r="BI2" s="51" t="s">
         <v>466</v>
       </c>
-      <c r="BJ2" s="734" t="s">
+      <c r="BJ2" s="738" t="s">
         <v>171</v>
       </c>
-      <c r="BK2" s="734"/>
-      <c r="BL2" s="735" t="s">
+      <c r="BK2" s="738"/>
+      <c r="BL2" s="739" t="s">
         <v>172</v>
       </c>
-      <c r="BM2" s="735"/>
-      <c r="BN2" s="735" t="s">
+      <c r="BM2" s="739"/>
+      <c r="BN2" s="739" t="s">
         <v>173</v>
       </c>
-      <c r="BO2" s="735"/>
+      <c r="BO2" s="739"/>
       <c r="BP2" s="51" t="s">
         <v>467</v>
       </c>
@@ -35918,15 +37158,15 @@
       <c r="BV2" s="51" t="s">
         <v>469</v>
       </c>
-      <c r="BW2" s="749"/>
-      <c r="BX2" s="744" t="s">
+      <c r="BW2" s="753"/>
+      <c r="BX2" s="748" t="s">
         <v>163</v>
       </c>
-      <c r="BY2" s="745"/>
-      <c r="BZ2" s="732" t="s">
+      <c r="BY2" s="749"/>
+      <c r="BZ2" s="736" t="s">
         <v>164</v>
       </c>
-      <c r="CA2" s="733"/>
+      <c r="CA2" s="737"/>
       <c r="CB2" s="20" t="s">
         <v>71</v>
       </c>
@@ -35966,22 +37206,22 @@
       <c r="CN2" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="CO2" s="764" t="s">
+      <c r="CO2" s="768" t="s">
         <v>178</v>
       </c>
-      <c r="CP2" s="765"/>
-      <c r="CQ2" s="762" t="s">
+      <c r="CP2" s="769"/>
+      <c r="CQ2" s="766" t="s">
         <v>179</v>
       </c>
-      <c r="CR2" s="762"/>
-      <c r="CS2" s="765" t="s">
+      <c r="CR2" s="766"/>
+      <c r="CS2" s="769" t="s">
         <v>180</v>
       </c>
-      <c r="CT2" s="765"/>
-      <c r="CU2" s="762" t="s">
+      <c r="CT2" s="769"/>
+      <c r="CU2" s="766" t="s">
         <v>181</v>
       </c>
-      <c r="CV2" s="763"/>
+      <c r="CV2" s="767"/>
     </row>
     <row r="3" spans="1:100" s="2" customFormat="1" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A3" s="597"/>
@@ -36314,7 +37554,7 @@
     <row r="5" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A5" s="596"/>
       <c r="B5" s="596"/>
-      <c r="C5" s="838"/>
+      <c r="C5" s="688"/>
       <c r="D5" s="596"/>
       <c r="E5" s="596"/>
       <c r="F5" s="596"/>
@@ -36328,69 +37568,69 @@
       <c r="N5" s="674"/>
       <c r="O5" s="675"/>
       <c r="P5" s="676"/>
-      <c r="Q5" s="836"/>
+      <c r="Q5" s="686"/>
       <c r="R5" s="685"/>
-      <c r="S5" s="837"/>
-      <c r="T5" s="838"/>
-      <c r="U5" s="837"/>
-      <c r="V5" s="838"/>
-      <c r="W5" s="837"/>
-      <c r="X5" s="838"/>
-      <c r="Y5" s="837"/>
-      <c r="Z5" s="838"/>
+      <c r="S5" s="687"/>
+      <c r="T5" s="688"/>
+      <c r="U5" s="687"/>
+      <c r="V5" s="688"/>
+      <c r="W5" s="687"/>
+      <c r="X5" s="688"/>
+      <c r="Y5" s="687"/>
+      <c r="Z5" s="688"/>
       <c r="AA5" s="596"/>
       <c r="AB5" s="596"/>
-      <c r="AC5" s="838"/>
-      <c r="AD5" s="837"/>
-      <c r="AE5" s="838"/>
-      <c r="AF5" s="837"/>
-      <c r="AG5" s="837"/>
-      <c r="AH5" s="838"/>
-      <c r="AI5" s="837"/>
-      <c r="AJ5" s="838"/>
-      <c r="AK5" s="837"/>
-      <c r="AL5" s="838"/>
+      <c r="AC5" s="688"/>
+      <c r="AD5" s="687"/>
+      <c r="AE5" s="688"/>
+      <c r="AF5" s="687"/>
+      <c r="AG5" s="687"/>
+      <c r="AH5" s="688"/>
+      <c r="AI5" s="687"/>
+      <c r="AJ5" s="688"/>
+      <c r="AK5" s="687"/>
+      <c r="AL5" s="688"/>
       <c r="AM5" s="596"/>
       <c r="AN5" s="596"/>
       <c r="AO5" s="596"/>
-      <c r="AP5" s="837"/>
-      <c r="AQ5" s="838"/>
-      <c r="AR5" s="837"/>
-      <c r="AS5" s="838"/>
-      <c r="AT5" s="837"/>
-      <c r="AU5" s="838"/>
-      <c r="AV5" s="837"/>
-      <c r="AW5" s="838"/>
-      <c r="AX5" s="837"/>
-      <c r="AY5" s="838"/>
+      <c r="AP5" s="687"/>
+      <c r="AQ5" s="688"/>
+      <c r="AR5" s="687"/>
+      <c r="AS5" s="688"/>
+      <c r="AT5" s="687"/>
+      <c r="AU5" s="688"/>
+      <c r="AV5" s="687"/>
+      <c r="AW5" s="688"/>
+      <c r="AX5" s="687"/>
+      <c r="AY5" s="688"/>
       <c r="AZ5" s="596"/>
       <c r="BA5" s="596"/>
-      <c r="BB5" s="837"/>
-      <c r="BC5" s="838"/>
-      <c r="BD5" s="837"/>
-      <c r="BE5" s="838"/>
-      <c r="BF5" s="837"/>
-      <c r="BG5" s="838"/>
+      <c r="BB5" s="687"/>
+      <c r="BC5" s="688"/>
+      <c r="BD5" s="687"/>
+      <c r="BE5" s="688"/>
+      <c r="BF5" s="687"/>
+      <c r="BG5" s="688"/>
       <c r="BH5" s="596"/>
       <c r="BI5" s="596"/>
-      <c r="BJ5" s="837"/>
-      <c r="BK5" s="838"/>
-      <c r="BL5" s="837"/>
-      <c r="BM5" s="838"/>
-      <c r="BN5" s="837"/>
-      <c r="BO5" s="838"/>
+      <c r="BJ5" s="687"/>
+      <c r="BK5" s="688"/>
+      <c r="BL5" s="687"/>
+      <c r="BM5" s="688"/>
+      <c r="BN5" s="687"/>
+      <c r="BO5" s="688"/>
       <c r="BP5" s="596"/>
       <c r="BQ5" s="596"/>
-      <c r="BR5" s="838"/>
-      <c r="BS5" s="838"/>
-      <c r="BT5" s="838"/>
+      <c r="BR5" s="688"/>
+      <c r="BS5" s="688"/>
+      <c r="BT5" s="688"/>
       <c r="BU5" s="596"/>
       <c r="BV5" s="596"/>
       <c r="BW5" s="596"/>
-      <c r="BX5" s="837"/>
-      <c r="BY5" s="838"/>
-      <c r="BZ5" s="837"/>
-      <c r="CA5" s="838"/>
+      <c r="BX5" s="687"/>
+      <c r="BY5" s="688"/>
+      <c r="BZ5" s="687"/>
+      <c r="CA5" s="688"/>
       <c r="CB5" s="596"/>
       <c r="CC5" s="596"/>
       <c r="CD5" s="596"/>
@@ -36404,19 +37644,19 @@
       <c r="CL5" s="596"/>
       <c r="CM5" s="596"/>
       <c r="CN5" s="596"/>
-      <c r="CO5" s="837"/>
-      <c r="CP5" s="838"/>
-      <c r="CQ5" s="837"/>
-      <c r="CR5" s="838"/>
-      <c r="CS5" s="837"/>
-      <c r="CT5" s="838"/>
-      <c r="CU5" s="837"/>
-      <c r="CV5" s="838"/>
+      <c r="CO5" s="687"/>
+      <c r="CP5" s="688"/>
+      <c r="CQ5" s="687"/>
+      <c r="CR5" s="688"/>
+      <c r="CS5" s="687"/>
+      <c r="CT5" s="688"/>
+      <c r="CU5" s="687"/>
+      <c r="CV5" s="688"/>
     </row>
     <row r="6" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A6" s="596"/>
       <c r="B6" s="596"/>
-      <c r="C6" s="838"/>
+      <c r="C6" s="688"/>
       <c r="D6" s="596"/>
       <c r="E6" s="596"/>
       <c r="F6" s="596"/>
@@ -36430,69 +37670,69 @@
       <c r="N6" s="674"/>
       <c r="O6" s="675"/>
       <c r="P6" s="676"/>
-      <c r="Q6" s="836"/>
+      <c r="Q6" s="686"/>
       <c r="R6" s="596"/>
-      <c r="S6" s="837"/>
-      <c r="T6" s="838"/>
-      <c r="U6" s="837"/>
-      <c r="V6" s="838"/>
-      <c r="W6" s="837"/>
-      <c r="X6" s="838"/>
-      <c r="Y6" s="837"/>
-      <c r="Z6" s="838"/>
+      <c r="S6" s="687"/>
+      <c r="T6" s="688"/>
+      <c r="U6" s="687"/>
+      <c r="V6" s="688"/>
+      <c r="W6" s="687"/>
+      <c r="X6" s="688"/>
+      <c r="Y6" s="687"/>
+      <c r="Z6" s="688"/>
       <c r="AA6" s="596"/>
       <c r="AB6" s="596"/>
-      <c r="AC6" s="838"/>
-      <c r="AD6" s="837"/>
-      <c r="AE6" s="838"/>
-      <c r="AF6" s="837"/>
-      <c r="AG6" s="837"/>
-      <c r="AH6" s="838"/>
-      <c r="AI6" s="837"/>
-      <c r="AJ6" s="838"/>
-      <c r="AK6" s="837"/>
-      <c r="AL6" s="838"/>
+      <c r="AC6" s="688"/>
+      <c r="AD6" s="687"/>
+      <c r="AE6" s="688"/>
+      <c r="AF6" s="687"/>
+      <c r="AG6" s="687"/>
+      <c r="AH6" s="688"/>
+      <c r="AI6" s="687"/>
+      <c r="AJ6" s="688"/>
+      <c r="AK6" s="687"/>
+      <c r="AL6" s="688"/>
       <c r="AM6" s="596"/>
       <c r="AN6" s="596"/>
       <c r="AO6" s="596"/>
-      <c r="AP6" s="837"/>
-      <c r="AQ6" s="838"/>
-      <c r="AR6" s="837"/>
-      <c r="AS6" s="838"/>
-      <c r="AT6" s="837"/>
-      <c r="AU6" s="838"/>
-      <c r="AV6" s="837"/>
-      <c r="AW6" s="838"/>
-      <c r="AX6" s="837"/>
-      <c r="AY6" s="838"/>
+      <c r="AP6" s="687"/>
+      <c r="AQ6" s="688"/>
+      <c r="AR6" s="687"/>
+      <c r="AS6" s="688"/>
+      <c r="AT6" s="687"/>
+      <c r="AU6" s="688"/>
+      <c r="AV6" s="687"/>
+      <c r="AW6" s="688"/>
+      <c r="AX6" s="687"/>
+      <c r="AY6" s="688"/>
       <c r="AZ6" s="596"/>
       <c r="BA6" s="596"/>
-      <c r="BB6" s="837"/>
-      <c r="BC6" s="838"/>
-      <c r="BD6" s="837"/>
-      <c r="BE6" s="838"/>
-      <c r="BF6" s="837"/>
-      <c r="BG6" s="838"/>
+      <c r="BB6" s="687"/>
+      <c r="BC6" s="688"/>
+      <c r="BD6" s="687"/>
+      <c r="BE6" s="688"/>
+      <c r="BF6" s="687"/>
+      <c r="BG6" s="688"/>
       <c r="BH6" s="596"/>
       <c r="BI6" s="596"/>
-      <c r="BJ6" s="837"/>
-      <c r="BK6" s="838"/>
-      <c r="BL6" s="837"/>
-      <c r="BM6" s="838"/>
-      <c r="BN6" s="837"/>
-      <c r="BO6" s="838"/>
+      <c r="BJ6" s="687"/>
+      <c r="BK6" s="688"/>
+      <c r="BL6" s="687"/>
+      <c r="BM6" s="688"/>
+      <c r="BN6" s="687"/>
+      <c r="BO6" s="688"/>
       <c r="BP6" s="596"/>
       <c r="BQ6" s="596"/>
-      <c r="BR6" s="838"/>
-      <c r="BS6" s="838"/>
-      <c r="BT6" s="838"/>
+      <c r="BR6" s="688"/>
+      <c r="BS6" s="688"/>
+      <c r="BT6" s="688"/>
       <c r="BU6" s="596"/>
       <c r="BV6" s="596"/>
       <c r="BW6" s="596"/>
-      <c r="BX6" s="837"/>
-      <c r="BY6" s="838"/>
-      <c r="BZ6" s="837"/>
-      <c r="CA6" s="838"/>
+      <c r="BX6" s="687"/>
+      <c r="BY6" s="688"/>
+      <c r="BZ6" s="687"/>
+      <c r="CA6" s="688"/>
       <c r="CB6" s="596"/>
       <c r="CC6" s="596"/>
       <c r="CD6" s="596"/>
@@ -36506,14 +37746,14 @@
       <c r="CL6" s="596"/>
       <c r="CM6" s="596"/>
       <c r="CN6" s="596"/>
-      <c r="CO6" s="837"/>
-      <c r="CP6" s="838"/>
-      <c r="CQ6" s="837"/>
-      <c r="CR6" s="838"/>
-      <c r="CS6" s="837"/>
-      <c r="CT6" s="838"/>
-      <c r="CU6" s="837"/>
-      <c r="CV6" s="838"/>
+      <c r="CO6" s="687"/>
+      <c r="CP6" s="688"/>
+      <c r="CQ6" s="687"/>
+      <c r="CR6" s="688"/>
+      <c r="CS6" s="687"/>
+      <c r="CT6" s="688"/>
+      <c r="CU6" s="687"/>
+      <c r="CV6" s="688"/>
     </row>
     <row r="7" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
@@ -41263,8 +42503,8 @@
       <c r="B2" s="113" t="s">
         <v>196</v>
       </c>
-      <c r="C2" s="766"/>
-      <c r="D2" s="766"/>
+      <c r="C2" s="770"/>
+      <c r="D2" s="770"/>
       <c r="E2" s="111"/>
       <c r="F2" s="111"/>
       <c r="G2" s="111"/>
@@ -41389,32 +42629,32 @@
     </row>
     <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="110"/>
-      <c r="B7" s="767" t="s">
+      <c r="B7" s="771" t="s">
         <v>436</v>
       </c>
-      <c r="C7" s="767"/>
-      <c r="D7" s="767"/>
+      <c r="C7" s="771"/>
+      <c r="D7" s="771"/>
       <c r="E7" s="111"/>
       <c r="F7" s="111"/>
       <c r="G7" s="111"/>
       <c r="H7" s="111"/>
       <c r="I7" s="111"/>
-      <c r="J7" s="767" t="s">
+      <c r="J7" s="771" t="s">
         <v>200</v>
       </c>
-      <c r="K7" s="767"/>
-      <c r="L7" s="767"/>
+      <c r="K7" s="771"/>
+      <c r="L7" s="771"/>
       <c r="M7" s="111"/>
       <c r="N7" s="111"/>
       <c r="O7" s="111"/>
       <c r="P7" s="112" t="s">
         <v>201</v>
       </c>
-      <c r="Q7" s="767" t="s">
+      <c r="Q7" s="771" t="s">
         <v>200</v>
       </c>
-      <c r="R7" s="767"/>
-      <c r="S7" s="767"/>
+      <c r="R7" s="771"/>
+      <c r="S7" s="771"/>
       <c r="T7" s="111"/>
       <c r="U7" s="125" t="s">
         <v>202</v>
@@ -41448,41 +42688,41 @@
       <c r="B9" s="126" t="s">
         <v>433</v>
       </c>
-      <c r="C9" s="768" t="s">
+      <c r="C9" s="772" t="s">
         <v>204</v>
       </c>
-      <c r="D9" s="769"/>
-      <c r="E9" s="768" t="s">
+      <c r="D9" s="773"/>
+      <c r="E9" s="772" t="s">
         <v>205</v>
       </c>
-      <c r="F9" s="769"/>
+      <c r="F9" s="773"/>
       <c r="G9" s="111"/>
       <c r="H9" s="111"/>
       <c r="I9" s="111"/>
       <c r="J9" s="126" t="s">
         <v>433</v>
       </c>
-      <c r="K9" s="768" t="s">
+      <c r="K9" s="772" t="s">
         <v>204</v>
       </c>
-      <c r="L9" s="769"/>
-      <c r="M9" s="768" t="s">
+      <c r="L9" s="773"/>
+      <c r="M9" s="772" t="s">
         <v>205</v>
       </c>
-      <c r="N9" s="769"/>
+      <c r="N9" s="773"/>
       <c r="O9" s="111"/>
       <c r="P9" s="111"/>
       <c r="Q9" s="126" t="s">
         <v>203</v>
       </c>
-      <c r="R9" s="768" t="s">
+      <c r="R9" s="772" t="s">
         <v>204</v>
       </c>
-      <c r="S9" s="769"/>
-      <c r="T9" s="768" t="s">
+      <c r="S9" s="773"/>
+      <c r="T9" s="772" t="s">
         <v>205</v>
       </c>
-      <c r="U9" s="769"/>
+      <c r="U9" s="773"/>
     </row>
     <row r="10" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="110"/>
@@ -41544,10 +42784,10 @@
       </c>
       <c r="C11" s="131"/>
       <c r="D11" s="131"/>
-      <c r="E11" s="770" t="s">
+      <c r="E11" s="774" t="s">
         <v>210</v>
       </c>
-      <c r="F11" s="771"/>
+      <c r="F11" s="775"/>
       <c r="G11" s="132"/>
       <c r="H11" s="132"/>
       <c r="I11" s="132"/>
@@ -41556,10 +42796,10 @@
       </c>
       <c r="K11" s="111"/>
       <c r="L11" s="111"/>
-      <c r="M11" s="773" t="s">
+      <c r="M11" s="777" t="s">
         <v>210</v>
       </c>
-      <c r="N11" s="774"/>
+      <c r="N11" s="778"/>
       <c r="O11" s="132"/>
       <c r="P11" s="132"/>
       <c r="Q11" s="130" t="s">
@@ -41567,10 +42807,10 @@
       </c>
       <c r="R11" s="131"/>
       <c r="S11" s="131"/>
-      <c r="T11" s="770" t="s">
+      <c r="T11" s="774" t="s">
         <v>210</v>
       </c>
-      <c r="U11" s="771"/>
+      <c r="U11" s="775"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="110"/>
@@ -41805,10 +43045,10 @@
       </c>
       <c r="C20" s="426"/>
       <c r="D20" s="159"/>
-      <c r="E20" s="770" t="s">
+      <c r="E20" s="774" t="s">
         <v>449</v>
       </c>
-      <c r="F20" s="771"/>
+      <c r="F20" s="775"/>
       <c r="G20" s="140"/>
       <c r="H20" s="140"/>
       <c r="I20" s="111"/>
@@ -41817,10 +43057,10 @@
       </c>
       <c r="K20" s="426"/>
       <c r="L20" s="159"/>
-      <c r="M20" s="770" t="s">
+      <c r="M20" s="774" t="s">
         <v>449</v>
       </c>
-      <c r="N20" s="771"/>
+      <c r="N20" s="775"/>
       <c r="O20" s="150"/>
       <c r="P20" s="150"/>
       <c r="Q20" s="130" t="s">
@@ -41828,10 +43068,10 @@
       </c>
       <c r="R20" s="426"/>
       <c r="S20" s="159"/>
-      <c r="T20" s="770" t="s">
+      <c r="T20" s="774" t="s">
         <v>449</v>
       </c>
-      <c r="U20" s="771"/>
+      <c r="U20" s="775"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="110"/>
@@ -42095,10 +43335,10 @@
       </c>
       <c r="C30" s="426"/>
       <c r="D30" s="159"/>
-      <c r="E30" s="770" t="s">
+      <c r="E30" s="774" t="s">
         <v>449</v>
       </c>
-      <c r="F30" s="771"/>
+      <c r="F30" s="775"/>
       <c r="G30" s="140"/>
       <c r="H30" s="140"/>
       <c r="I30" s="111"/>
@@ -42107,10 +43347,10 @@
       </c>
       <c r="K30" s="426"/>
       <c r="L30" s="159"/>
-      <c r="M30" s="770" t="s">
+      <c r="M30" s="774" t="s">
         <v>449</v>
       </c>
-      <c r="N30" s="771"/>
+      <c r="N30" s="775"/>
       <c r="O30" s="150"/>
       <c r="P30" s="150"/>
       <c r="Q30" s="130" t="s">
@@ -42118,10 +43358,10 @@
       </c>
       <c r="R30" s="426"/>
       <c r="S30" s="159"/>
-      <c r="T30" s="770" t="s">
+      <c r="T30" s="774" t="s">
         <v>449</v>
       </c>
-      <c r="U30" s="771"/>
+      <c r="U30" s="775"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="172"/>
@@ -42444,11 +43684,11 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="110"/>
-      <c r="B42" s="772"/>
-      <c r="C42" s="772"/>
-      <c r="D42" s="772"/>
-      <c r="E42" s="772"/>
-      <c r="F42" s="772"/>
+      <c r="B42" s="776"/>
+      <c r="C42" s="776"/>
+      <c r="D42" s="776"/>
+      <c r="E42" s="776"/>
+      <c r="F42" s="776"/>
       <c r="G42" s="150"/>
       <c r="H42" s="111"/>
       <c r="I42" s="150"/>
@@ -42644,8 +43884,8 @@
       <c r="B3" s="194" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="775"/>
-      <c r="D3" s="775"/>
+      <c r="C3" s="779"/>
+      <c r="D3" s="779"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C4" s="195"/>
@@ -42678,10 +43918,10 @@
       <c r="D10" s="203" t="s">
         <v>232</v>
       </c>
-      <c r="E10" s="776" t="s">
+      <c r="E10" s="780" t="s">
         <v>233</v>
       </c>
-      <c r="F10" s="777"/>
+      <c r="F10" s="781"/>
     </row>
     <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="204" t="s">
@@ -42832,10 +44072,10 @@
       <c r="D30" s="215" t="s">
         <v>232</v>
       </c>
-      <c r="E30" s="776" t="s">
+      <c r="E30" s="780" t="s">
         <v>233</v>
       </c>
-      <c r="F30" s="777"/>
+      <c r="F30" s="781"/>
     </row>
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="204" t="s">
@@ -42983,10 +44223,10 @@
       <c r="D49" s="215" t="s">
         <v>232</v>
       </c>
-      <c r="E49" s="776" t="s">
+      <c r="E49" s="780" t="s">
         <v>233</v>
       </c>
-      <c r="F49" s="777"/>
+      <c r="F49" s="781"/>
     </row>
     <row r="50" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="204" t="s">
@@ -43154,8 +44394,8 @@
       </c>
       <c r="C2" s="113"/>
       <c r="D2" s="113"/>
-      <c r="E2" s="766"/>
-      <c r="F2" s="766"/>
+      <c r="E2" s="770"/>
+      <c r="F2" s="770"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="112"/>
@@ -43187,13 +44427,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="110"/>
-      <c r="B6" s="767" t="s">
+      <c r="B6" s="771" t="s">
         <v>432</v>
       </c>
-      <c r="C6" s="767"/>
-      <c r="D6" s="767"/>
-      <c r="E6" s="767"/>
-      <c r="F6" s="767"/>
+      <c r="C6" s="771"/>
+      <c r="D6" s="771"/>
+      <c r="E6" s="771"/>
+      <c r="F6" s="771"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="110"/>
@@ -43208,14 +44448,14 @@
       <c r="B8" s="461" t="s">
         <v>203</v>
       </c>
-      <c r="C8" s="778" t="s">
+      <c r="C8" s="782" t="s">
         <v>204</v>
       </c>
-      <c r="D8" s="779"/>
-      <c r="E8" s="780" t="s">
+      <c r="D8" s="783"/>
+      <c r="E8" s="784" t="s">
         <v>205</v>
       </c>
-      <c r="F8" s="779"/>
+      <c r="F8" s="783"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="110"/>
@@ -43351,11 +44591,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="110"/>
-      <c r="B22" s="772"/>
-      <c r="C22" s="772"/>
-      <c r="D22" s="772"/>
-      <c r="E22" s="772"/>
-      <c r="F22" s="772"/>
+      <c r="B22" s="776"/>
+      <c r="C22" s="776"/>
+      <c r="D22" s="776"/>
+      <c r="E22" s="776"/>
+      <c r="F22" s="776"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="110"/>
@@ -43425,13 +44665,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="781" t="s">
+      <c r="B2" s="785" t="s">
         <v>250</v>
       </c>
-      <c r="C2" s="782" t="s">
+      <c r="C2" s="786" t="s">
         <v>251</v>
       </c>
-      <c r="D2" s="782" t="s">
+      <c r="D2" s="786" t="s">
         <v>150</v>
       </c>
       <c r="E2" s="232" t="s">
@@ -43466,9 +44706,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="781"/>
-      <c r="C3" s="783"/>
-      <c r="D3" s="783"/>
+      <c r="B3" s="785"/>
+      <c r="C3" s="787"/>
+      <c r="D3" s="787"/>
       <c r="E3" s="672" t="s">
         <v>259</v>
       </c>
@@ -43501,7 +44741,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="784" t="s">
+      <c r="B4" s="788" t="s">
         <v>262</v>
       </c>
       <c r="C4" s="233" t="s">
@@ -43520,7 +44760,7 @@
       <c r="N4" s="235"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="784"/>
+      <c r="B5" s="788"/>
       <c r="C5" s="233" t="s">
         <v>60</v>
       </c>
@@ -43537,7 +44777,7 @@
       <c r="N5" s="235"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="785"/>
+      <c r="B6" s="789"/>
       <c r="C6" s="562" t="s">
         <v>453</v>
       </c>
@@ -43651,24 +44891,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="588" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="786" t="s">
+      <c r="A1" s="790" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="787"/>
-      <c r="C1" s="788"/>
-      <c r="D1" s="789" t="s">
+      <c r="B1" s="791"/>
+      <c r="C1" s="792"/>
+      <c r="D1" s="793" t="s">
         <v>458</v>
       </c>
-      <c r="E1" s="789"/>
-      <c r="F1" s="790"/>
-      <c r="G1" s="799" t="s">
+      <c r="E1" s="793"/>
+      <c r="F1" s="794"/>
+      <c r="G1" s="803" t="s">
         <v>264</v>
       </c>
-      <c r="H1" s="800"/>
-      <c r="I1" s="800"/>
-      <c r="J1" s="800"/>
-      <c r="K1" s="801"/>
-      <c r="L1" s="791" t="s">
+      <c r="H1" s="804"/>
+      <c r="I1" s="804"/>
+      <c r="J1" s="804"/>
+      <c r="K1" s="805"/>
+      <c r="L1" s="795" t="s">
         <v>265</v>
       </c>
     </row>
@@ -43706,7 +44946,7 @@
       <c r="K2" s="251" t="s">
         <v>269</v>
       </c>
-      <c r="L2" s="792"/>
+      <c r="L2" s="796"/>
     </row>
     <row r="3" spans="1:12" s="588" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="252"/>
@@ -43714,19 +44954,19 @@
       <c r="C3" s="254" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="793" t="s">
+      <c r="D3" s="797" t="s">
         <v>270</v>
       </c>
-      <c r="E3" s="794"/>
-      <c r="F3" s="795"/>
-      <c r="G3" s="796" t="s">
+      <c r="E3" s="798"/>
+      <c r="F3" s="799"/>
+      <c r="G3" s="800" t="s">
         <v>270</v>
       </c>
-      <c r="H3" s="797"/>
-      <c r="I3" s="797"/>
-      <c r="J3" s="797"/>
-      <c r="K3" s="798"/>
-      <c r="L3" s="792"/>
+      <c r="H3" s="801"/>
+      <c r="I3" s="801"/>
+      <c r="J3" s="801"/>
+      <c r="K3" s="802"/>
+      <c r="L3" s="796"/>
     </row>
     <row r="4" spans="1:12" s="588" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="252"/>

</xml_diff>

<commit_message>
Register    - sheet graph : correction on new diagram distance to compliance on model xlsx    - sheet summary big city : for 10th report, the method change to fill the sheet (big dischargers + big cities)      add 1 column to say if big dischargers or not      add 2 columns at the end (for debug) with the list of the agglo of the big city
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2018_register_model_20181015.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2018_register_model_20181015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="17" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'New agglomerations'!$A$5:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'New treatment plants'!$A$4:$F$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Nuts2_level analyse'!$A$4:$AC$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Summary_big_cities!$A$4:$L$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Summary_big_cities!$A$4:$O$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'UWWTP Level'!$A$4:$CQ$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">UWWTPsout!$A$5:$F$5</definedName>
   </definedNames>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="547">
   <si>
     <t>Sensitive areas reported for reference date</t>
   </si>
@@ -2186,6 +2186,9 @@
   </si>
   <si>
     <t>IAS [Individual &amp; appropriated system] in place</t>
+  </si>
+  <si>
+    <t>Big dischargers</t>
   </si>
 </sst>
 </file>
@@ -3015,7 +3018,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="70">
+  <borders count="72">
     <border>
       <left/>
       <right/>
@@ -3906,6 +3909,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3928,7 +3957,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="840">
+  <cellXfs count="842">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5580,6 +5609,12 @@
     <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="77" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="70" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="71" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6277,7 +6312,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6354,13 +6388,12 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{62F2E86C-083F-435F-8772-482FE995B353}" type="CELLRANGE">
+                    <a:fld id="{0CC6E555-A852-4B8F-AB60-78455AB107F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6378,7 +6411,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -6386,13 +6418,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{51F33832-80FC-4287-898B-808E5E653548}" type="CELLRANGE">
+                    <a:fld id="{378FA0FC-5683-4112-B6CE-BA8C54FBCB51}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6410,7 +6441,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -6419,13 +6449,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D58B840-B8CC-47D1-A17F-6BB98A1BCA3C}" type="CELLRANGE">
+                    <a:fld id="{424299A1-3C1B-4B78-9F9F-852CF1FB76B5}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6443,7 +6472,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -6489,7 +6517,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -6596,13 +6623,12 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6436A324-10C8-45FB-B520-CC0FFB67F1A7}" type="CELLRANGE">
+                    <a:fld id="{F037B659-BC67-4D52-8A2C-D92474CA0FD4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6620,7 +6646,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -6628,13 +6653,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B753F9E7-DB98-4E30-8C03-B471B572CFCD}" type="CELLRANGE">
+                    <a:fld id="{758EB137-1BB7-4883-9F17-FD2D027EB38F}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6652,7 +6676,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -6661,13 +6684,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BDDF6030-4E13-430B-85F2-F0D24B2A471E}" type="CELLRANGE">
+                    <a:fld id="{84933F70-C383-4929-9ED6-46C39D52AFC1}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6685,7 +6707,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -6731,7 +6752,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -6819,11 +6839,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1989722032"/>
-        <c:axId val="-1989728560"/>
+        <c:axId val="-1583083968"/>
+        <c:axId val="-1435657152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989722032"/>
+        <c:axId val="-1583083968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6866,7 +6886,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989728560"/>
+        <c:crossAx val="-1435657152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6874,7 +6894,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989728560"/>
+        <c:axId val="-1435657152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6906,7 +6926,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6967,7 +6986,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989722032"/>
+        <c:crossAx val="-1583083968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7102,7 +7121,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7354,11 +7372,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1989728016"/>
-        <c:axId val="-1989719312"/>
+        <c:axId val="-1401760048"/>
+        <c:axId val="-1401755696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989728016"/>
+        <c:axId val="-1401760048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7390,7 +7408,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7457,7 +7474,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989719312"/>
+        <c:crossAx val="-1401755696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7465,7 +7482,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989719312"/>
+        <c:axId val="-1401755696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7585,7 +7602,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989728016"/>
+        <c:crossAx val="-1401760048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7715,7 +7732,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8470,11 +8486,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1989726384"/>
-        <c:axId val="-1989722576"/>
+        <c:axId val="-1401758960"/>
+        <c:axId val="-1401758416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989726384"/>
+        <c:axId val="-1401758960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8577,7 +8593,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989722576"/>
+        <c:crossAx val="-1401758416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8585,7 +8601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989722576"/>
+        <c:axId val="-1401758416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8636,7 +8652,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989726384"/>
+        <c:crossAx val="-1401758960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9001,11 +9017,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1989717680"/>
-        <c:axId val="-1989716048"/>
+        <c:axId val="-1401748624"/>
+        <c:axId val="-1401756784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989717680"/>
+        <c:axId val="-1401748624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9116,7 +9132,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989716048"/>
+        <c:crossAx val="-1401756784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9124,7 +9140,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989716048"/>
+        <c:axId val="-1401756784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9230,7 +9246,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989717680"/>
+        <c:crossAx val="-1401748624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9600,11 +9616,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1989725296"/>
-        <c:axId val="-1989719856"/>
+        <c:axId val="-1401757872"/>
+        <c:axId val="-1401746448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989725296"/>
+        <c:axId val="-1401757872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9715,7 +9731,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989719856"/>
+        <c:crossAx val="-1401746448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9723,7 +9739,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989719856"/>
+        <c:axId val="-1401746448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9837,7 +9853,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989725296"/>
+        <c:crossAx val="-1401757872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9972,7 +9988,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10319,11 +10334,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1989718768"/>
-        <c:axId val="-1989718224"/>
+        <c:axId val="-1401757328"/>
+        <c:axId val="-1401755152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989718768"/>
+        <c:axId val="-1401757328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10429,7 +10444,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989718224"/>
+        <c:crossAx val="-1401755152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10437,7 +10452,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989718224"/>
+        <c:axId val="-1401755152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10559,7 +10574,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989718768"/>
+        <c:crossAx val="-1401757328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10895,11 +10910,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1989717136"/>
-        <c:axId val="-1989715504"/>
+        <c:axId val="-1401752432"/>
+        <c:axId val="-1401751888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989717136"/>
+        <c:axId val="-1401752432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11010,7 +11025,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989715504"/>
+        <c:crossAx val="-1401751888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11018,7 +11033,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989715504"/>
+        <c:axId val="-1401751888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11132,7 +11147,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989717136"/>
+        <c:crossAx val="-1401752432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11468,11 +11483,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1987468016"/>
-        <c:axId val="-1987468560"/>
+        <c:axId val="-1401750800"/>
+        <c:axId val="-1401750256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1987468016"/>
+        <c:axId val="-1401750800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11583,7 +11598,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1987468560"/>
+        <c:crossAx val="-1401750256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11591,7 +11606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1987468560"/>
+        <c:axId val="-1401750256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11705,7 +11720,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1987468016"/>
+        <c:crossAx val="-1401750800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11840,7 +11855,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12087,11 +12101,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1987473456"/>
-        <c:axId val="-1987470192"/>
+        <c:axId val="-1401749168"/>
+        <c:axId val="-1428994944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1987473456"/>
+        <c:axId val="-1401749168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12123,7 +12137,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12190,7 +12203,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1987470192"/>
+        <c:crossAx val="-1428994944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12198,7 +12211,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1987470192"/>
+        <c:axId val="-1428994944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12317,7 +12330,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1987473456"/>
+        <c:crossAx val="-1401749168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12822,11 +12835,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1987475632"/>
-        <c:axId val="-1987474544"/>
+        <c:axId val="-1428990048"/>
+        <c:axId val="-1428996032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1987475632"/>
+        <c:axId val="-1428990048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12869,7 +12882,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1987474544"/>
+        <c:crossAx val="-1428996032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12877,7 +12890,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1987474544"/>
+        <c:axId val="-1428996032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12983,7 +12996,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1987475632"/>
+        <c:crossAx val="-1428990048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13108,7 +13121,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13185,13 +13197,12 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5173D7CE-2C95-4584-8C0A-96B9CA809F47}" type="CELLRANGE">
+                    <a:fld id="{E3341B8A-4DAB-4788-96C0-C168F4A7C6AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13209,7 +13220,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -13217,13 +13227,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CEAAA4D9-8776-40CD-9ACF-48DDE5164D11}" type="CELLRANGE">
+                    <a:fld id="{DF965D3E-EFC0-4F68-B177-0A3487EA7BFB}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13241,7 +13250,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -13250,13 +13258,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A0F27F48-D8CF-4B63-A31A-3468F562054F}" type="CELLRANGE">
+                    <a:fld id="{E168B9EC-FC07-483C-96B5-9270A40B4746}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13274,7 +13281,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -13320,7 +13326,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -13427,13 +13432,12 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4BB92A20-24BF-4B4D-AEB2-FBB27C6B1F03}" type="CELLRANGE">
+                    <a:fld id="{AC77DA9F-8F71-456E-949A-A31DC08B4835}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13451,7 +13455,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -13459,13 +13462,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF6568E4-7599-4C53-BB3A-8693A87E91FD}" type="CELLRANGE">
+                    <a:fld id="{27882B1C-79FF-43C1-AAC0-CFAF3E949A24}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13483,7 +13485,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -13492,13 +13493,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{402E5C3B-FCD3-4CC2-A62E-4F0FA16C0817}" type="CELLRANGE">
+                    <a:fld id="{C84AF084-78C5-411A-9446-E19DA60A4CEE}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13516,7 +13516,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -13562,7 +13561,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -13650,11 +13648,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1989725840"/>
-        <c:axId val="-1989723664"/>
+        <c:axId val="-1401754064"/>
+        <c:axId val="-1401760592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989725840"/>
+        <c:axId val="-1401754064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13686,7 +13684,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -13753,7 +13750,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989723664"/>
+        <c:crossAx val="-1401760592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13761,7 +13758,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989723664"/>
+        <c:axId val="-1401760592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13861,7 +13858,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989725840"/>
+        <c:crossAx val="-1401754064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13991,7 +13988,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14092,7 +14088,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -14214,7 +14209,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -14283,11 +14277,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1987466928"/>
-        <c:axId val="-1987469648"/>
+        <c:axId val="-1429004192"/>
+        <c:axId val="-1428993856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1987466928"/>
+        <c:axId val="-1429004192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14330,7 +14324,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1987469648"/>
+        <c:crossAx val="-1428993856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14338,7 +14332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1987469648"/>
+        <c:axId val="-1428993856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14359,7 +14353,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14420,7 +14413,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1987466928"/>
+        <c:crossAx val="-1429004192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14434,7 +14427,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14541,7 +14533,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14772,9 +14763,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -14978,7 +14967,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15333,11 +15321,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1989723120"/>
-        <c:axId val="-1989729648"/>
+        <c:axId val="-1401753520"/>
+        <c:axId val="-1401754608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989723120"/>
+        <c:axId val="-1401753520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15369,7 +15357,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15436,7 +15423,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989729648"/>
+        <c:crossAx val="-1401754608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15444,7 +15431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989729648"/>
+        <c:axId val="-1401754608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15490,7 +15477,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15551,7 +15537,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989723120"/>
+        <c:crossAx val="-1401753520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15682,7 +15668,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16010,11 +15995,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1989724752"/>
-        <c:axId val="-1989730736"/>
+        <c:axId val="-1401748080"/>
+        <c:axId val="-1401759504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989724752"/>
+        <c:axId val="-1401748080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16046,7 +16031,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16113,7 +16097,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989730736"/>
+        <c:crossAx val="-1401759504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16121,7 +16105,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989730736"/>
+        <c:axId val="-1401759504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16221,7 +16205,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989724752"/>
+        <c:crossAx val="-1401748080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16352,7 +16336,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16680,11 +16663,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1989716592"/>
-        <c:axId val="-1989727472"/>
+        <c:axId val="-1401761680"/>
+        <c:axId val="-1401761136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989716592"/>
+        <c:axId val="-1401761680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16716,7 +16699,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16783,7 +16765,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989727472"/>
+        <c:crossAx val="-1401761136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16791,7 +16773,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989727472"/>
+        <c:axId val="-1401761136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16891,7 +16873,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989716592"/>
+        <c:crossAx val="-1401761680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17027,7 +17009,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17423,11 +17404,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1989720400"/>
-        <c:axId val="-1989726928"/>
+        <c:axId val="-1401751344"/>
+        <c:axId val="-1401749712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989720400"/>
+        <c:axId val="-1401751344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17470,7 +17451,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989726928"/>
+        <c:crossAx val="-1401749712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17478,7 +17459,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989726928"/>
+        <c:axId val="-1401749712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17529,7 +17510,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -17590,7 +17570,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989720400"/>
+        <c:crossAx val="-1401751344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18120,11 +18100,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1989724208"/>
-        <c:axId val="-1989730192"/>
+        <c:axId val="-1401752976"/>
+        <c:axId val="-1401747536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989724208"/>
+        <c:axId val="-1401752976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18167,7 +18147,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989730192"/>
+        <c:crossAx val="-1401747536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18175,7 +18155,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989730192"/>
+        <c:axId val="-1401747536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18294,7 +18274,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989724208"/>
+        <c:crossAx val="-1401752976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18388,7 +18368,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18635,11 +18614,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1989721488"/>
-        <c:axId val="-1989729104"/>
+        <c:axId val="-1401756240"/>
+        <c:axId val="-1401746992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989721488"/>
+        <c:axId val="-1401756240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18668,7 +18647,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -18735,7 +18713,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989729104"/>
+        <c:crossAx val="-1401746992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18743,7 +18721,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989729104"/>
+        <c:axId val="-1401746992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -18863,7 +18841,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1989721488"/>
+        <c:crossAx val="-1401756240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -31167,23 +31145,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="574" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="694" t="s">
+      <c r="A1" s="696" t="s">
         <v>271</v>
       </c>
-      <c r="B1" s="695"/>
-      <c r="C1" s="695"/>
-      <c r="D1" s="695"/>
+      <c r="B1" s="697"/>
+      <c r="C1" s="697"/>
+      <c r="D1" s="697"/>
       <c r="E1" s="565"/>
-      <c r="F1" s="811" t="s">
+      <c r="F1" s="813" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="812"/>
-      <c r="H1" s="812"/>
+      <c r="G1" s="814"/>
+      <c r="H1" s="814"/>
       <c r="I1" s="570"/>
       <c r="J1" s="255"/>
       <c r="K1" s="570"/>
       <c r="L1" s="256"/>
-      <c r="M1" s="806" t="s">
+      <c r="M1" s="808" t="s">
         <v>272</v>
       </c>
       <c r="N1" s="257"/>
@@ -31195,19 +31173,19 @@
       <c r="R1" s="255"/>
       <c r="S1" s="570"/>
       <c r="T1" s="256"/>
-      <c r="U1" s="806" t="s">
+      <c r="U1" s="808" t="s">
         <v>274</v>
       </c>
       <c r="V1" s="257"/>
-      <c r="W1" s="813" t="s">
+      <c r="W1" s="815" t="s">
         <v>275</v>
       </c>
-      <c r="X1" s="813"/>
-      <c r="Y1" s="813"/>
-      <c r="Z1" s="813"/>
-      <c r="AA1" s="813"/>
-      <c r="AB1" s="814"/>
-      <c r="AC1" s="806" t="s">
+      <c r="X1" s="815"/>
+      <c r="Y1" s="815"/>
+      <c r="Z1" s="815"/>
+      <c r="AA1" s="815"/>
+      <c r="AB1" s="816"/>
+      <c r="AC1" s="808" t="s">
         <v>276</v>
       </c>
     </row>
@@ -31221,52 +31199,52 @@
       <c r="C2" s="569" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="808" t="s">
+      <c r="D2" s="810" t="s">
         <v>454</v>
       </c>
-      <c r="E2" s="808"/>
+      <c r="E2" s="810"/>
       <c r="F2" s="259"/>
-      <c r="G2" s="809" t="s">
+      <c r="G2" s="811" t="s">
         <v>160</v>
       </c>
-      <c r="H2" s="809"/>
-      <c r="I2" s="809" t="s">
+      <c r="H2" s="811"/>
+      <c r="I2" s="811" t="s">
         <v>161</v>
       </c>
-      <c r="J2" s="809"/>
-      <c r="K2" s="809" t="s">
+      <c r="J2" s="811"/>
+      <c r="K2" s="811" t="s">
         <v>162</v>
       </c>
-      <c r="L2" s="810"/>
-      <c r="M2" s="807"/>
+      <c r="L2" s="812"/>
+      <c r="M2" s="809"/>
       <c r="N2" s="260"/>
-      <c r="O2" s="809" t="s">
+      <c r="O2" s="811" t="s">
         <v>160</v>
       </c>
-      <c r="P2" s="809"/>
-      <c r="Q2" s="809" t="s">
+      <c r="P2" s="811"/>
+      <c r="Q2" s="811" t="s">
         <v>161</v>
       </c>
-      <c r="R2" s="809"/>
-      <c r="S2" s="809" t="s">
+      <c r="R2" s="811"/>
+      <c r="S2" s="811" t="s">
         <v>162</v>
       </c>
-      <c r="T2" s="810"/>
-      <c r="U2" s="807"/>
+      <c r="T2" s="812"/>
+      <c r="U2" s="809"/>
       <c r="V2" s="260"/>
-      <c r="W2" s="809" t="s">
+      <c r="W2" s="811" t="s">
         <v>160</v>
       </c>
-      <c r="X2" s="809"/>
-      <c r="Y2" s="809" t="s">
+      <c r="X2" s="811"/>
+      <c r="Y2" s="811" t="s">
         <v>161</v>
       </c>
-      <c r="Z2" s="809"/>
-      <c r="AA2" s="809" t="s">
+      <c r="Z2" s="811"/>
+      <c r="AA2" s="811" t="s">
         <v>162</v>
       </c>
-      <c r="AB2" s="810"/>
-      <c r="AC2" s="807"/>
+      <c r="AB2" s="812"/>
+      <c r="AC2" s="809"/>
     </row>
     <row r="3" spans="1:29" s="589" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A3" s="45"/>
@@ -31635,8 +31613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P104" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z132" sqref="Z132"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB131" sqref="AB131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31661,35 +31639,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="815" t="s">
+      <c r="A1" s="817" t="s">
         <v>437</v>
       </c>
-      <c r="B1" s="816"/>
-      <c r="C1" s="816"/>
+      <c r="B1" s="818"/>
+      <c r="C1" s="818"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="824" t="s">
+      <c r="A3" s="826" t="s">
         <v>319</v>
       </c>
-      <c r="B3" s="826" t="s">
+      <c r="B3" s="828" t="s">
         <v>411</v>
       </c>
-      <c r="C3" s="827"/>
-      <c r="D3" s="822" t="s">
+      <c r="C3" s="829"/>
+      <c r="D3" s="824" t="s">
         <v>438</v>
       </c>
-      <c r="E3" s="823"/>
-      <c r="AA3" s="839" t="s">
+      <c r="E3" s="825"/>
+      <c r="AA3" s="841" t="s">
         <v>332</v>
       </c>
-      <c r="AB3" s="839"/>
-      <c r="AC3" s="839" t="s">
+      <c r="AB3" s="841"/>
+      <c r="AC3" s="841" t="s">
         <v>416</v>
       </c>
-      <c r="AD3" s="839"/>
+      <c r="AD3" s="841"/>
     </row>
     <row r="4" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="825"/>
+      <c r="A4" s="827"/>
       <c r="B4" s="311" t="s">
         <v>415</v>
       </c>
@@ -31832,14 +31810,14 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="Z10" s="363"/>
-      <c r="AA10" s="839" t="s">
+      <c r="AA10" s="841" t="s">
         <v>417</v>
       </c>
-      <c r="AB10" s="839"/>
-      <c r="AC10" s="839" t="s">
+      <c r="AB10" s="841"/>
+      <c r="AC10" s="841" t="s">
         <v>418</v>
       </c>
-      <c r="AD10" s="839"/>
+      <c r="AD10" s="841"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="Z11" s="363" t="s">
@@ -31884,7 +31862,7 @@
       </c>
     </row>
     <row r="13" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="824" t="s">
+      <c r="A13" s="826" t="s">
         <v>320</v>
       </c>
       <c r="B13" s="310" t="str">
@@ -31916,7 +31894,7 @@
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="825"/>
+      <c r="A14" s="827"/>
       <c r="B14" s="313" t="s">
         <v>321</v>
       </c>
@@ -32002,27 +31980,27 @@
       <c r="A21" t="s">
         <v>422</v>
       </c>
-      <c r="B21" s="817" t="s">
+      <c r="B21" s="819" t="s">
         <v>431</v>
       </c>
-      <c r="C21" s="817"/>
-      <c r="D21" s="817"/>
-      <c r="E21" s="817"/>
+      <c r="C21" s="819"/>
+      <c r="D21" s="819"/>
+      <c r="E21" s="819"/>
     </row>
     <row r="22" spans="1:32" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="315" t="s">
         <v>283</v>
       </c>
-      <c r="B22" s="828" t="str">
+      <c r="B22" s="830" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C22" s="829"/>
-      <c r="D22" s="828" t="str">
+      <c r="C22" s="831"/>
+      <c r="D22" s="830" t="str">
         <f>D3</f>
         <v>[#previous_year#]*</v>
       </c>
-      <c r="E22" s="829"/>
+      <c r="E22" s="831"/>
     </row>
     <row r="23" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="316"/>
@@ -32397,16 +32375,16 @@
       <c r="A41" s="318" t="s">
         <v>330</v>
       </c>
-      <c r="B41" s="818" t="str">
+      <c r="B41" s="820" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C41" s="819"/>
-      <c r="D41" s="820" t="str">
+      <c r="C41" s="821"/>
+      <c r="D41" s="822" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E41" s="821"/>
+      <c r="E41" s="823"/>
       <c r="AA41" t="s">
         <v>412</v>
       </c>
@@ -32556,11 +32534,11 @@
       <c r="AA48" t="s">
         <v>422</v>
       </c>
-      <c r="AB48" s="817" t="s">
+      <c r="AB48" s="819" t="s">
         <v>443</v>
       </c>
-      <c r="AC48" s="817"/>
-      <c r="AD48" s="817"/>
+      <c r="AC48" s="819"/>
+      <c r="AD48" s="819"/>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" s="384" t="s">
@@ -32834,11 +32812,11 @@
       <c r="AA62" t="s">
         <v>422</v>
       </c>
-      <c r="AB62" s="817" t="s">
+      <c r="AB62" s="819" t="s">
         <v>444</v>
       </c>
-      <c r="AC62" s="817"/>
-      <c r="AD62" s="817"/>
+      <c r="AC62" s="819"/>
+      <c r="AD62" s="819"/>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A63" s="312"/>
@@ -33073,12 +33051,12 @@
       <c r="A74" s="530" t="s">
         <v>426</v>
       </c>
-      <c r="B74" s="817" t="s">
+      <c r="B74" s="819" t="s">
         <v>427</v>
       </c>
-      <c r="C74" s="817"/>
-      <c r="D74" s="817"/>
-      <c r="E74" s="817"/>
+      <c r="C74" s="819"/>
+      <c r="D74" s="819"/>
+      <c r="E74" s="819"/>
     </row>
     <row r="75" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="333" t="s">
@@ -33371,16 +33349,16 @@
       </c>
     </row>
     <row r="85" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B85" s="832" t="str">
+      <c r="B85" s="834" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C85" s="833"/>
-      <c r="D85" s="832" t="str">
+      <c r="C85" s="835"/>
+      <c r="D85" s="834" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E85" s="833"/>
+      <c r="E85" s="835"/>
       <c r="Z85" t="s">
         <v>401</v>
       </c>
@@ -33394,14 +33372,14 @@
     </row>
     <row r="86" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="201"/>
-      <c r="B86" s="834" t="s">
+      <c r="B86" s="836" t="s">
         <v>233</v>
       </c>
-      <c r="C86" s="781"/>
-      <c r="D86" s="834" t="s">
+      <c r="C86" s="783"/>
+      <c r="D86" s="836" t="s">
         <v>233</v>
       </c>
-      <c r="E86" s="781"/>
+      <c r="E86" s="783"/>
       <c r="Z86" s="341" t="s">
         <v>234</v>
       </c>
@@ -33607,27 +33585,27 @@
       </c>
     </row>
     <row r="101" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B101" s="832" t="str">
+      <c r="B101" s="834" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C101" s="833"/>
-      <c r="D101" s="832" t="str">
+      <c r="C101" s="835"/>
+      <c r="D101" s="834" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E101" s="833"/>
+      <c r="E101" s="835"/>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A102" s="201"/>
-      <c r="B102" s="834" t="s">
+      <c r="B102" s="836" t="s">
         <v>233</v>
       </c>
-      <c r="C102" s="781"/>
-      <c r="D102" s="834" t="s">
+      <c r="C102" s="783"/>
+      <c r="D102" s="836" t="s">
         <v>233</v>
       </c>
-      <c r="E102" s="781"/>
+      <c r="E102" s="783"/>
       <c r="Z102" t="s">
         <v>401</v>
       </c>
@@ -33841,27 +33819,27 @@
       </c>
     </row>
     <row r="116" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B116" s="835" t="str">
+      <c r="B116" s="837" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C116" s="836"/>
-      <c r="D116" s="835" t="str">
+      <c r="C116" s="838"/>
+      <c r="D116" s="837" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E116" s="836"/>
+      <c r="E116" s="838"/>
     </row>
     <row r="117" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A117" s="346"/>
-      <c r="B117" s="837" t="s">
+      <c r="B117" s="839" t="s">
         <v>233</v>
       </c>
-      <c r="C117" s="838"/>
-      <c r="D117" s="837" t="s">
+      <c r="C117" s="840"/>
+      <c r="D117" s="839" t="s">
         <v>233</v>
       </c>
-      <c r="E117" s="838"/>
+      <c r="E117" s="840"/>
       <c r="Z117" t="s">
         <v>401</v>
       </c>
@@ -34093,12 +34071,12 @@
       <c r="A129" s="350" t="s">
         <v>320</v>
       </c>
-      <c r="B129" s="830" t="str">
+      <c r="B129" s="832" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C129" s="831"/>
-      <c r="D129" s="831"/>
+      <c r="C129" s="833"/>
+      <c r="D129" s="833"/>
       <c r="Z129" t="str">
         <f>CONCATENATE("Collection 
 ", B3, " : target ", AB118, " p.e.")</f>
@@ -34132,11 +34110,11 @@
 [#current_year#]  : target 0 p.e.</v>
       </c>
       <c r="AA130" s="364">
-        <f>E122+E123</f>
+        <f>E123</f>
         <v>0</v>
       </c>
       <c r="AB130" s="364">
-        <f>C122+C123</f>
+        <f>C123</f>
         <v>0</v>
       </c>
     </row>
@@ -34156,11 +34134,11 @@
 [#current_year#]  : target 0 p.e.</v>
       </c>
       <c r="AA131" s="364">
-        <f>E125+E126</f>
+        <f>E126</f>
         <v>0</v>
       </c>
       <c r="AB131" s="364">
-        <f>C125+C126</f>
+        <f>C126</f>
         <v>0</v>
       </c>
     </row>
@@ -35225,54 +35203,54 @@
       <c r="AR3" s="5"/>
     </row>
     <row r="4" spans="1:44" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="690" t="s">
+      <c r="A4" s="692" t="s">
         <v>448</v>
       </c>
-      <c r="B4" s="691"/>
-      <c r="C4" s="691"/>
-      <c r="D4" s="691"/>
-      <c r="E4" s="692"/>
-      <c r="F4" s="692"/>
-      <c r="G4" s="692"/>
-      <c r="H4" s="692"/>
-      <c r="I4" s="692"/>
-      <c r="J4" s="692"/>
-      <c r="K4" s="692"/>
-      <c r="L4" s="692"/>
-      <c r="M4" s="692"/>
-      <c r="N4" s="692"/>
-      <c r="O4" s="692"/>
-      <c r="P4" s="692"/>
-      <c r="Q4" s="692"/>
-      <c r="R4" s="692"/>
-      <c r="S4" s="692"/>
-      <c r="T4" s="692"/>
-      <c r="U4" s="692"/>
-      <c r="V4" s="692"/>
-      <c r="W4" s="692"/>
-      <c r="X4" s="692"/>
-      <c r="Y4" s="692"/>
-      <c r="Z4" s="692"/>
-      <c r="AA4" s="692"/>
-      <c r="AB4" s="692"/>
-      <c r="AC4" s="692"/>
-      <c r="AD4" s="692"/>
-      <c r="AE4" s="692"/>
-      <c r="AF4" s="692"/>
-      <c r="AG4" s="692"/>
-      <c r="AH4" s="692"/>
-      <c r="AI4" s="692"/>
-      <c r="AJ4" s="692"/>
-      <c r="AK4" s="692"/>
-      <c r="AL4" s="692"/>
-      <c r="AM4" s="692"/>
-      <c r="AN4" s="692"/>
-      <c r="AO4" s="692"/>
-      <c r="AP4" s="692"/>
-      <c r="AQ4" s="693" t="s">
+      <c r="B4" s="693"/>
+      <c r="C4" s="693"/>
+      <c r="D4" s="693"/>
+      <c r="E4" s="694"/>
+      <c r="F4" s="694"/>
+      <c r="G4" s="694"/>
+      <c r="H4" s="694"/>
+      <c r="I4" s="694"/>
+      <c r="J4" s="694"/>
+      <c r="K4" s="694"/>
+      <c r="L4" s="694"/>
+      <c r="M4" s="694"/>
+      <c r="N4" s="694"/>
+      <c r="O4" s="694"/>
+      <c r="P4" s="694"/>
+      <c r="Q4" s="694"/>
+      <c r="R4" s="694"/>
+      <c r="S4" s="694"/>
+      <c r="T4" s="694"/>
+      <c r="U4" s="694"/>
+      <c r="V4" s="694"/>
+      <c r="W4" s="694"/>
+      <c r="X4" s="694"/>
+      <c r="Y4" s="694"/>
+      <c r="Z4" s="694"/>
+      <c r="AA4" s="694"/>
+      <c r="AB4" s="694"/>
+      <c r="AC4" s="694"/>
+      <c r="AD4" s="694"/>
+      <c r="AE4" s="694"/>
+      <c r="AF4" s="694"/>
+      <c r="AG4" s="694"/>
+      <c r="AH4" s="694"/>
+      <c r="AI4" s="694"/>
+      <c r="AJ4" s="694"/>
+      <c r="AK4" s="694"/>
+      <c r="AL4" s="694"/>
+      <c r="AM4" s="694"/>
+      <c r="AN4" s="694"/>
+      <c r="AO4" s="694"/>
+      <c r="AP4" s="694"/>
+      <c r="AQ4" s="695" t="s">
         <v>2</v>
       </c>
-      <c r="AR4" s="693"/>
+      <c r="AR4" s="695"/>
     </row>
     <row r="5" spans="1:44" s="573" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="299" t="s">
@@ -35460,123 +35438,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" s="574" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="694" t="s">
+      <c r="A1" s="696" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="695"/>
-      <c r="C1" s="695"/>
-      <c r="D1" s="695"/>
-      <c r="E1" s="695"/>
-      <c r="F1" s="695"/>
-      <c r="G1" s="695"/>
-      <c r="H1" s="696" t="s">
+      <c r="B1" s="697"/>
+      <c r="C1" s="697"/>
+      <c r="D1" s="697"/>
+      <c r="E1" s="697"/>
+      <c r="F1" s="697"/>
+      <c r="G1" s="697"/>
+      <c r="H1" s="698" t="s">
         <v>138</v>
       </c>
-      <c r="I1" s="697"/>
-      <c r="J1" s="697"/>
-      <c r="K1" s="697"/>
-      <c r="L1" s="697"/>
-      <c r="M1" s="698"/>
-      <c r="N1" s="699" t="s">
+      <c r="I1" s="699"/>
+      <c r="J1" s="699"/>
+      <c r="K1" s="699"/>
+      <c r="L1" s="699"/>
+      <c r="M1" s="700"/>
+      <c r="N1" s="701" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="700"/>
-      <c r="P1" s="700"/>
-      <c r="Q1" s="701"/>
-      <c r="R1" s="701"/>
-      <c r="S1" s="700"/>
-      <c r="T1" s="700"/>
-      <c r="U1" s="700"/>
-      <c r="V1" s="702" t="s">
+      <c r="O1" s="702"/>
+      <c r="P1" s="702"/>
+      <c r="Q1" s="703"/>
+      <c r="R1" s="703"/>
+      <c r="S1" s="702"/>
+      <c r="T1" s="702"/>
+      <c r="U1" s="702"/>
+      <c r="V1" s="704" t="s">
         <v>49</v>
       </c>
-      <c r="W1" s="703"/>
-      <c r="X1" s="704"/>
-      <c r="Y1" s="704"/>
-      <c r="Z1" s="705"/>
-      <c r="AA1" s="706" t="s">
+      <c r="W1" s="705"/>
+      <c r="X1" s="706"/>
+      <c r="Y1" s="706"/>
+      <c r="Z1" s="707"/>
+      <c r="AA1" s="708" t="s">
         <v>50</v>
       </c>
-      <c r="AB1" s="707"/>
-      <c r="AC1" s="707"/>
-      <c r="AD1" s="707"/>
-      <c r="AE1" s="707"/>
-      <c r="AF1" s="707"/>
-      <c r="AG1" s="707"/>
-      <c r="AH1" s="707"/>
-      <c r="AI1" s="707"/>
-      <c r="AJ1" s="707"/>
-      <c r="AK1" s="707"/>
-      <c r="AL1" s="707"/>
-      <c r="AM1" s="707"/>
+      <c r="AB1" s="709"/>
+      <c r="AC1" s="709"/>
+      <c r="AD1" s="709"/>
+      <c r="AE1" s="709"/>
+      <c r="AF1" s="709"/>
+      <c r="AG1" s="709"/>
+      <c r="AH1" s="709"/>
+      <c r="AI1" s="709"/>
+      <c r="AJ1" s="709"/>
+      <c r="AK1" s="709"/>
+      <c r="AL1" s="709"/>
+      <c r="AM1" s="709"/>
       <c r="AN1" s="7"/>
       <c r="AO1" s="8"/>
-      <c r="AP1" s="719" t="s">
+      <c r="AP1" s="721" t="s">
         <v>51</v>
       </c>
-      <c r="AQ1" s="700"/>
-      <c r="AR1" s="700"/>
-      <c r="AS1" s="700"/>
-      <c r="AT1" s="700"/>
-      <c r="AU1" s="700"/>
-      <c r="AV1" s="700"/>
-      <c r="AW1" s="720"/>
-      <c r="AX1" s="727" t="s">
+      <c r="AQ1" s="702"/>
+      <c r="AR1" s="702"/>
+      <c r="AS1" s="702"/>
+      <c r="AT1" s="702"/>
+      <c r="AU1" s="702"/>
+      <c r="AV1" s="702"/>
+      <c r="AW1" s="722"/>
+      <c r="AX1" s="729" t="s">
         <v>52</v>
       </c>
-      <c r="AY1" s="728"/>
-      <c r="AZ1" s="728"/>
-      <c r="BA1" s="728"/>
-      <c r="BB1" s="728"/>
-      <c r="BC1" s="729"/>
-      <c r="BD1" s="730" t="s">
+      <c r="AY1" s="730"/>
+      <c r="AZ1" s="730"/>
+      <c r="BA1" s="730"/>
+      <c r="BB1" s="730"/>
+      <c r="BC1" s="731"/>
+      <c r="BD1" s="732" t="s">
         <v>53</v>
       </c>
-      <c r="BE1" s="731"/>
-      <c r="BF1" s="731"/>
-      <c r="BG1" s="731"/>
-      <c r="BH1" s="731"/>
-      <c r="BI1" s="732"/>
-      <c r="BJ1" s="733" t="s">
+      <c r="BE1" s="733"/>
+      <c r="BF1" s="733"/>
+      <c r="BG1" s="733"/>
+      <c r="BH1" s="733"/>
+      <c r="BI1" s="734"/>
+      <c r="BJ1" s="735" t="s">
         <v>54</v>
       </c>
-      <c r="BK1" s="734"/>
-      <c r="BL1" s="734"/>
-      <c r="BM1" s="734"/>
-      <c r="BN1" s="734"/>
-      <c r="BO1" s="734"/>
-      <c r="BP1" s="735"/>
-      <c r="BQ1" s="708" t="s">
+      <c r="BK1" s="736"/>
+      <c r="BL1" s="736"/>
+      <c r="BM1" s="736"/>
+      <c r="BN1" s="736"/>
+      <c r="BO1" s="736"/>
+      <c r="BP1" s="737"/>
+      <c r="BQ1" s="710" t="s">
         <v>55</v>
       </c>
-      <c r="BR1" s="709"/>
-      <c r="BS1" s="709"/>
-      <c r="BT1" s="709"/>
-      <c r="BU1" s="709"/>
-      <c r="BV1" s="709"/>
+      <c r="BR1" s="711"/>
+      <c r="BS1" s="711"/>
+      <c r="BT1" s="711"/>
+      <c r="BU1" s="711"/>
+      <c r="BV1" s="711"/>
       <c r="BW1" s="8"/>
       <c r="BX1" s="9"/>
-      <c r="BY1" s="710" t="s">
+      <c r="BY1" s="712" t="s">
         <v>56</v>
       </c>
-      <c r="BZ1" s="711"/>
-      <c r="CA1" s="711"/>
-      <c r="CB1" s="711"/>
-      <c r="CC1" s="711"/>
-      <c r="CD1" s="711"/>
-      <c r="CE1" s="711"/>
-      <c r="CF1" s="712"/>
-      <c r="CG1" s="712"/>
-      <c r="CH1" s="712"/>
-      <c r="CI1" s="712"/>
-      <c r="CJ1" s="712"/>
-      <c r="CK1" s="712"/>
-      <c r="CL1" s="712"/>
-      <c r="CM1" s="712"/>
-      <c r="CN1" s="712"/>
-      <c r="CO1" s="712"/>
-      <c r="CP1" s="712"/>
-      <c r="CQ1" s="712"/>
+      <c r="BZ1" s="713"/>
+      <c r="CA1" s="713"/>
+      <c r="CB1" s="713"/>
+      <c r="CC1" s="713"/>
+      <c r="CD1" s="713"/>
+      <c r="CE1" s="713"/>
+      <c r="CF1" s="714"/>
+      <c r="CG1" s="714"/>
+      <c r="CH1" s="714"/>
+      <c r="CI1" s="714"/>
+      <c r="CJ1" s="714"/>
+      <c r="CK1" s="714"/>
+      <c r="CL1" s="714"/>
+      <c r="CM1" s="714"/>
+      <c r="CN1" s="714"/>
+      <c r="CO1" s="714"/>
+      <c r="CP1" s="714"/>
+      <c r="CQ1" s="714"/>
     </row>
     <row r="2" spans="1:95" s="574" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -35600,18 +35578,18 @@
       <c r="G2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="713" t="s">
+      <c r="H2" s="715" t="s">
         <v>155</v>
       </c>
-      <c r="I2" s="714"/>
-      <c r="J2" s="714" t="s">
+      <c r="I2" s="716"/>
+      <c r="J2" s="716" t="s">
         <v>64</v>
       </c>
-      <c r="K2" s="714"/>
-      <c r="L2" s="714" t="s">
+      <c r="K2" s="716"/>
+      <c r="L2" s="716" t="s">
         <v>65</v>
       </c>
-      <c r="M2" s="715"/>
+      <c r="M2" s="717"/>
       <c r="N2" s="12" t="s">
         <v>57</v>
       </c>
@@ -35720,36 +35698,36 @@
       <c r="AW2" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="AX2" s="716" t="s">
+      <c r="AX2" s="718" t="s">
         <v>90</v>
       </c>
-      <c r="AY2" s="717"/>
-      <c r="AZ2" s="717"/>
-      <c r="BA2" s="717" t="s">
+      <c r="AY2" s="719"/>
+      <c r="AZ2" s="719"/>
+      <c r="BA2" s="719" t="s">
         <v>91</v>
       </c>
-      <c r="BB2" s="717"/>
-      <c r="BC2" s="718"/>
-      <c r="BD2" s="721" t="s">
+      <c r="BB2" s="719"/>
+      <c r="BC2" s="720"/>
+      <c r="BD2" s="723" t="s">
         <v>90</v>
       </c>
-      <c r="BE2" s="722"/>
-      <c r="BF2" s="722"/>
-      <c r="BG2" s="722" t="s">
+      <c r="BE2" s="724"/>
+      <c r="BF2" s="724"/>
+      <c r="BG2" s="724" t="s">
         <v>91</v>
       </c>
-      <c r="BH2" s="722"/>
-      <c r="BI2" s="723"/>
-      <c r="BJ2" s="724" t="s">
+      <c r="BH2" s="724"/>
+      <c r="BI2" s="725"/>
+      <c r="BJ2" s="726" t="s">
         <v>90</v>
       </c>
-      <c r="BK2" s="725"/>
-      <c r="BL2" s="725"/>
-      <c r="BM2" s="725" t="s">
+      <c r="BK2" s="727"/>
+      <c r="BL2" s="727"/>
+      <c r="BM2" s="727" t="s">
         <v>91</v>
       </c>
-      <c r="BN2" s="726"/>
-      <c r="BO2" s="726"/>
+      <c r="BN2" s="728"/>
+      <c r="BO2" s="728"/>
       <c r="BP2" s="24" t="s">
         <v>92</v>
       </c>
@@ -36794,7 +36772,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36862,124 +36840,124 @@
         <v>135</v>
       </c>
       <c r="L1" s="42"/>
-      <c r="M1" s="740" t="s">
+      <c r="M1" s="742" t="s">
         <v>136</v>
       </c>
-      <c r="N1" s="741" t="s">
+      <c r="N1" s="743" t="s">
         <v>137</v>
       </c>
-      <c r="O1" s="742"/>
-      <c r="P1" s="742"/>
-      <c r="Q1" s="742"/>
-      <c r="R1" s="743" t="s">
+      <c r="O1" s="744"/>
+      <c r="P1" s="744"/>
+      <c r="Q1" s="744"/>
+      <c r="R1" s="745" t="s">
         <v>138</v>
       </c>
-      <c r="S1" s="744"/>
-      <c r="T1" s="744"/>
-      <c r="U1" s="744"/>
-      <c r="V1" s="744"/>
-      <c r="W1" s="744"/>
-      <c r="X1" s="745"/>
-      <c r="Y1" s="746" t="s">
+      <c r="S1" s="746"/>
+      <c r="T1" s="746"/>
+      <c r="U1" s="746"/>
+      <c r="V1" s="746"/>
+      <c r="W1" s="746"/>
+      <c r="X1" s="747"/>
+      <c r="Y1" s="748" t="s">
         <v>139</v>
       </c>
-      <c r="Z1" s="747"/>
-      <c r="AA1" s="750" t="s">
+      <c r="Z1" s="749"/>
+      <c r="AA1" s="752" t="s">
         <v>140</v>
       </c>
-      <c r="AB1" s="752" t="s">
+      <c r="AB1" s="754" t="s">
         <v>141</v>
       </c>
-      <c r="AC1" s="760" t="s">
+      <c r="AC1" s="762" t="s">
         <v>457</v>
       </c>
-      <c r="AD1" s="761"/>
-      <c r="AE1" s="761"/>
-      <c r="AF1" s="762"/>
-      <c r="AG1" s="763" t="s">
+      <c r="AD1" s="763"/>
+      <c r="AE1" s="763"/>
+      <c r="AF1" s="764"/>
+      <c r="AG1" s="765" t="s">
         <v>142</v>
       </c>
-      <c r="AH1" s="744"/>
-      <c r="AI1" s="744"/>
-      <c r="AJ1" s="744"/>
-      <c r="AK1" s="744"/>
-      <c r="AL1" s="744"/>
-      <c r="AM1" s="744"/>
-      <c r="AN1" s="744"/>
-      <c r="AO1" s="752" t="s">
+      <c r="AH1" s="746"/>
+      <c r="AI1" s="746"/>
+      <c r="AJ1" s="746"/>
+      <c r="AK1" s="746"/>
+      <c r="AL1" s="746"/>
+      <c r="AM1" s="746"/>
+      <c r="AN1" s="746"/>
+      <c r="AO1" s="754" t="s">
         <v>143</v>
       </c>
-      <c r="AP1" s="746" t="s">
+      <c r="AP1" s="748" t="s">
         <v>144</v>
       </c>
-      <c r="AQ1" s="747"/>
-      <c r="AR1" s="747"/>
-      <c r="AS1" s="732"/>
-      <c r="AT1" s="764" t="s">
+      <c r="AQ1" s="749"/>
+      <c r="AR1" s="749"/>
+      <c r="AS1" s="734"/>
+      <c r="AT1" s="766" t="s">
         <v>145</v>
       </c>
-      <c r="AU1" s="765"/>
-      <c r="AV1" s="765"/>
-      <c r="AW1" s="765"/>
-      <c r="AX1" s="765"/>
-      <c r="AY1" s="765"/>
-      <c r="AZ1" s="765"/>
-      <c r="BA1" s="765"/>
-      <c r="BB1" s="765"/>
-      <c r="BC1" s="765"/>
-      <c r="BD1" s="765"/>
-      <c r="BE1" s="765"/>
-      <c r="BF1" s="765"/>
-      <c r="BG1" s="765"/>
-      <c r="BH1" s="765"/>
-      <c r="BI1" s="765"/>
-      <c r="BJ1" s="765"/>
-      <c r="BK1" s="765"/>
-      <c r="BL1" s="765"/>
-      <c r="BM1" s="765"/>
-      <c r="BN1" s="765"/>
-      <c r="BO1" s="765"/>
-      <c r="BP1" s="765"/>
-      <c r="BQ1" s="765"/>
-      <c r="BR1" s="765"/>
-      <c r="BS1" s="765"/>
-      <c r="BT1" s="765"/>
-      <c r="BU1" s="765"/>
-      <c r="BV1" s="765"/>
-      <c r="BW1" s="752" t="s">
+      <c r="AU1" s="767"/>
+      <c r="AV1" s="767"/>
+      <c r="AW1" s="767"/>
+      <c r="AX1" s="767"/>
+      <c r="AY1" s="767"/>
+      <c r="AZ1" s="767"/>
+      <c r="BA1" s="767"/>
+      <c r="BB1" s="767"/>
+      <c r="BC1" s="767"/>
+      <c r="BD1" s="767"/>
+      <c r="BE1" s="767"/>
+      <c r="BF1" s="767"/>
+      <c r="BG1" s="767"/>
+      <c r="BH1" s="767"/>
+      <c r="BI1" s="767"/>
+      <c r="BJ1" s="767"/>
+      <c r="BK1" s="767"/>
+      <c r="BL1" s="767"/>
+      <c r="BM1" s="767"/>
+      <c r="BN1" s="767"/>
+      <c r="BO1" s="767"/>
+      <c r="BP1" s="767"/>
+      <c r="BQ1" s="767"/>
+      <c r="BR1" s="767"/>
+      <c r="BS1" s="767"/>
+      <c r="BT1" s="767"/>
+      <c r="BU1" s="767"/>
+      <c r="BV1" s="767"/>
+      <c r="BW1" s="754" t="s">
         <v>146</v>
       </c>
-      <c r="BX1" s="746" t="s">
+      <c r="BX1" s="748" t="s">
         <v>147</v>
       </c>
-      <c r="BY1" s="747"/>
-      <c r="BZ1" s="747"/>
-      <c r="CA1" s="732"/>
-      <c r="CB1" s="754" t="s">
+      <c r="BY1" s="749"/>
+      <c r="BZ1" s="749"/>
+      <c r="CA1" s="734"/>
+      <c r="CB1" s="756" t="s">
         <v>50</v>
       </c>
-      <c r="CC1" s="754"/>
-      <c r="CD1" s="754"/>
-      <c r="CE1" s="754"/>
-      <c r="CF1" s="754"/>
-      <c r="CG1" s="754"/>
-      <c r="CH1" s="754"/>
-      <c r="CI1" s="754"/>
-      <c r="CJ1" s="754"/>
-      <c r="CK1" s="754"/>
-      <c r="CL1" s="754"/>
-      <c r="CM1" s="754"/>
+      <c r="CC1" s="756"/>
+      <c r="CD1" s="756"/>
+      <c r="CE1" s="756"/>
+      <c r="CF1" s="756"/>
+      <c r="CG1" s="756"/>
+      <c r="CH1" s="756"/>
+      <c r="CI1" s="756"/>
+      <c r="CJ1" s="756"/>
+      <c r="CK1" s="756"/>
+      <c r="CL1" s="756"/>
+      <c r="CM1" s="756"/>
       <c r="CN1" s="43"/>
-      <c r="CO1" s="755" t="s">
+      <c r="CO1" s="757" t="s">
         <v>55</v>
       </c>
-      <c r="CP1" s="701"/>
-      <c r="CQ1" s="701"/>
-      <c r="CR1" s="701"/>
-      <c r="CS1" s="701"/>
-      <c r="CT1" s="701"/>
-      <c r="CU1" s="701"/>
-      <c r="CV1" s="720"/>
+      <c r="CP1" s="703"/>
+      <c r="CQ1" s="703"/>
+      <c r="CR1" s="703"/>
+      <c r="CS1" s="703"/>
+      <c r="CT1" s="703"/>
+      <c r="CU1" s="703"/>
+      <c r="CV1" s="722"/>
     </row>
     <row r="2" spans="1:100" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
@@ -37018,7 +36996,7 @@
       <c r="L2" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="M2" s="740"/>
+      <c r="M2" s="742"/>
       <c r="N2" s="49" t="s">
         <v>152</v>
       </c>
@@ -37034,22 +37012,22 @@
       <c r="R2" s="579" t="s">
         <v>397</v>
       </c>
-      <c r="S2" s="756" t="s">
+      <c r="S2" s="758" t="s">
         <v>155</v>
       </c>
-      <c r="T2" s="726"/>
-      <c r="U2" s="757" t="s">
+      <c r="T2" s="728"/>
+      <c r="U2" s="759" t="s">
         <v>64</v>
       </c>
-      <c r="V2" s="757"/>
-      <c r="W2" s="757" t="s">
+      <c r="V2" s="759"/>
+      <c r="W2" s="759" t="s">
         <v>65</v>
       </c>
-      <c r="X2" s="758"/>
-      <c r="Y2" s="748"/>
-      <c r="Z2" s="749"/>
-      <c r="AA2" s="751"/>
-      <c r="AB2" s="753"/>
+      <c r="X2" s="760"/>
+      <c r="Y2" s="750"/>
+      <c r="Z2" s="751"/>
+      <c r="AA2" s="753"/>
+      <c r="AB2" s="755"/>
       <c r="AC2" s="50" t="s">
         <v>156</v>
       </c>
@@ -37062,81 +37040,81 @@
       <c r="AF2" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="AG2" s="759" t="s">
+      <c r="AG2" s="761" t="s">
         <v>160</v>
       </c>
-      <c r="AH2" s="738"/>
-      <c r="AI2" s="738" t="s">
+      <c r="AH2" s="740"/>
+      <c r="AI2" s="740" t="s">
         <v>161</v>
       </c>
-      <c r="AJ2" s="738"/>
-      <c r="AK2" s="738" t="s">
+      <c r="AJ2" s="740"/>
+      <c r="AK2" s="740" t="s">
         <v>162</v>
       </c>
-      <c r="AL2" s="738"/>
+      <c r="AL2" s="740"/>
       <c r="AM2" s="51" t="s">
         <v>461</v>
       </c>
       <c r="AN2" s="51" t="s">
         <v>462</v>
       </c>
-      <c r="AO2" s="753"/>
-      <c r="AP2" s="748" t="s">
+      <c r="AO2" s="755"/>
+      <c r="AP2" s="750" t="s">
         <v>163</v>
       </c>
-      <c r="AQ2" s="749"/>
-      <c r="AR2" s="736" t="s">
+      <c r="AQ2" s="751"/>
+      <c r="AR2" s="738" t="s">
         <v>164</v>
       </c>
-      <c r="AS2" s="737"/>
-      <c r="AT2" s="738" t="s">
+      <c r="AS2" s="739"/>
+      <c r="AT2" s="740" t="s">
         <v>165</v>
       </c>
-      <c r="AU2" s="738"/>
-      <c r="AV2" s="739" t="s">
+      <c r="AU2" s="740"/>
+      <c r="AV2" s="741" t="s">
         <v>166</v>
       </c>
-      <c r="AW2" s="739"/>
-      <c r="AX2" s="739" t="s">
+      <c r="AW2" s="741"/>
+      <c r="AX2" s="741" t="s">
         <v>167</v>
       </c>
-      <c r="AY2" s="739"/>
+      <c r="AY2" s="741"/>
       <c r="AZ2" s="51" t="s">
         <v>463</v>
       </c>
       <c r="BA2" s="51" t="s">
         <v>464</v>
       </c>
-      <c r="BB2" s="738" t="s">
+      <c r="BB2" s="740" t="s">
         <v>168</v>
       </c>
-      <c r="BC2" s="738"/>
-      <c r="BD2" s="739" t="s">
+      <c r="BC2" s="740"/>
+      <c r="BD2" s="741" t="s">
         <v>169</v>
       </c>
-      <c r="BE2" s="739"/>
-      <c r="BF2" s="739" t="s">
+      <c r="BE2" s="741"/>
+      <c r="BF2" s="741" t="s">
         <v>170</v>
       </c>
-      <c r="BG2" s="739"/>
+      <c r="BG2" s="741"/>
       <c r="BH2" s="51" t="s">
         <v>465</v>
       </c>
       <c r="BI2" s="51" t="s">
         <v>466</v>
       </c>
-      <c r="BJ2" s="738" t="s">
+      <c r="BJ2" s="740" t="s">
         <v>171</v>
       </c>
-      <c r="BK2" s="738"/>
-      <c r="BL2" s="739" t="s">
+      <c r="BK2" s="740"/>
+      <c r="BL2" s="741" t="s">
         <v>172</v>
       </c>
-      <c r="BM2" s="739"/>
-      <c r="BN2" s="739" t="s">
+      <c r="BM2" s="741"/>
+      <c r="BN2" s="741" t="s">
         <v>173</v>
       </c>
-      <c r="BO2" s="739"/>
+      <c r="BO2" s="741"/>
       <c r="BP2" s="51" t="s">
         <v>467</v>
       </c>
@@ -37158,15 +37136,15 @@
       <c r="BV2" s="51" t="s">
         <v>469</v>
       </c>
-      <c r="BW2" s="753"/>
-      <c r="BX2" s="748" t="s">
+      <c r="BW2" s="755"/>
+      <c r="BX2" s="750" t="s">
         <v>163</v>
       </c>
-      <c r="BY2" s="749"/>
-      <c r="BZ2" s="736" t="s">
+      <c r="BY2" s="751"/>
+      <c r="BZ2" s="738" t="s">
         <v>164</v>
       </c>
-      <c r="CA2" s="737"/>
+      <c r="CA2" s="739"/>
       <c r="CB2" s="20" t="s">
         <v>71</v>
       </c>
@@ -37206,22 +37184,22 @@
       <c r="CN2" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="CO2" s="768" t="s">
+      <c r="CO2" s="770" t="s">
         <v>178</v>
       </c>
-      <c r="CP2" s="769"/>
-      <c r="CQ2" s="766" t="s">
+      <c r="CP2" s="771"/>
+      <c r="CQ2" s="768" t="s">
         <v>179</v>
       </c>
-      <c r="CR2" s="766"/>
-      <c r="CS2" s="769" t="s">
+      <c r="CR2" s="768"/>
+      <c r="CS2" s="771" t="s">
         <v>180</v>
       </c>
-      <c r="CT2" s="769"/>
-      <c r="CU2" s="766" t="s">
+      <c r="CT2" s="771"/>
+      <c r="CU2" s="768" t="s">
         <v>181</v>
       </c>
-      <c r="CV2" s="767"/>
+      <c r="CV2" s="769"/>
     </row>
     <row r="3" spans="1:100" s="2" customFormat="1" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A3" s="597"/>
@@ -42503,8 +42481,8 @@
       <c r="B2" s="113" t="s">
         <v>196</v>
       </c>
-      <c r="C2" s="770"/>
-      <c r="D2" s="770"/>
+      <c r="C2" s="772"/>
+      <c r="D2" s="772"/>
       <c r="E2" s="111"/>
       <c r="F2" s="111"/>
       <c r="G2" s="111"/>
@@ -42629,32 +42607,32 @@
     </row>
     <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="110"/>
-      <c r="B7" s="771" t="s">
+      <c r="B7" s="773" t="s">
         <v>436</v>
       </c>
-      <c r="C7" s="771"/>
-      <c r="D7" s="771"/>
+      <c r="C7" s="773"/>
+      <c r="D7" s="773"/>
       <c r="E7" s="111"/>
       <c r="F7" s="111"/>
       <c r="G7" s="111"/>
       <c r="H7" s="111"/>
       <c r="I7" s="111"/>
-      <c r="J7" s="771" t="s">
+      <c r="J7" s="773" t="s">
         <v>200</v>
       </c>
-      <c r="K7" s="771"/>
-      <c r="L7" s="771"/>
+      <c r="K7" s="773"/>
+      <c r="L7" s="773"/>
       <c r="M7" s="111"/>
       <c r="N7" s="111"/>
       <c r="O7" s="111"/>
       <c r="P7" s="112" t="s">
         <v>201</v>
       </c>
-      <c r="Q7" s="771" t="s">
+      <c r="Q7" s="773" t="s">
         <v>200</v>
       </c>
-      <c r="R7" s="771"/>
-      <c r="S7" s="771"/>
+      <c r="R7" s="773"/>
+      <c r="S7" s="773"/>
       <c r="T7" s="111"/>
       <c r="U7" s="125" t="s">
         <v>202</v>
@@ -42688,41 +42666,41 @@
       <c r="B9" s="126" t="s">
         <v>433</v>
       </c>
-      <c r="C9" s="772" t="s">
+      <c r="C9" s="774" t="s">
         <v>204</v>
       </c>
-      <c r="D9" s="773"/>
-      <c r="E9" s="772" t="s">
+      <c r="D9" s="775"/>
+      <c r="E9" s="774" t="s">
         <v>205</v>
       </c>
-      <c r="F9" s="773"/>
+      <c r="F9" s="775"/>
       <c r="G9" s="111"/>
       <c r="H9" s="111"/>
       <c r="I9" s="111"/>
       <c r="J9" s="126" t="s">
         <v>433</v>
       </c>
-      <c r="K9" s="772" t="s">
+      <c r="K9" s="774" t="s">
         <v>204</v>
       </c>
-      <c r="L9" s="773"/>
-      <c r="M9" s="772" t="s">
+      <c r="L9" s="775"/>
+      <c r="M9" s="774" t="s">
         <v>205</v>
       </c>
-      <c r="N9" s="773"/>
+      <c r="N9" s="775"/>
       <c r="O9" s="111"/>
       <c r="P9" s="111"/>
       <c r="Q9" s="126" t="s">
         <v>203</v>
       </c>
-      <c r="R9" s="772" t="s">
+      <c r="R9" s="774" t="s">
         <v>204</v>
       </c>
-      <c r="S9" s="773"/>
-      <c r="T9" s="772" t="s">
+      <c r="S9" s="775"/>
+      <c r="T9" s="774" t="s">
         <v>205</v>
       </c>
-      <c r="U9" s="773"/>
+      <c r="U9" s="775"/>
     </row>
     <row r="10" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="110"/>
@@ -42784,10 +42762,10 @@
       </c>
       <c r="C11" s="131"/>
       <c r="D11" s="131"/>
-      <c r="E11" s="774" t="s">
+      <c r="E11" s="776" t="s">
         <v>210</v>
       </c>
-      <c r="F11" s="775"/>
+      <c r="F11" s="777"/>
       <c r="G11" s="132"/>
       <c r="H11" s="132"/>
       <c r="I11" s="132"/>
@@ -42796,10 +42774,10 @@
       </c>
       <c r="K11" s="111"/>
       <c r="L11" s="111"/>
-      <c r="M11" s="777" t="s">
+      <c r="M11" s="779" t="s">
         <v>210</v>
       </c>
-      <c r="N11" s="778"/>
+      <c r="N11" s="780"/>
       <c r="O11" s="132"/>
       <c r="P11" s="132"/>
       <c r="Q11" s="130" t="s">
@@ -42807,10 +42785,10 @@
       </c>
       <c r="R11" s="131"/>
       <c r="S11" s="131"/>
-      <c r="T11" s="774" t="s">
+      <c r="T11" s="776" t="s">
         <v>210</v>
       </c>
-      <c r="U11" s="775"/>
+      <c r="U11" s="777"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="110"/>
@@ -43045,10 +43023,10 @@
       </c>
       <c r="C20" s="426"/>
       <c r="D20" s="159"/>
-      <c r="E20" s="774" t="s">
+      <c r="E20" s="776" t="s">
         <v>449</v>
       </c>
-      <c r="F20" s="775"/>
+      <c r="F20" s="777"/>
       <c r="G20" s="140"/>
       <c r="H20" s="140"/>
       <c r="I20" s="111"/>
@@ -43057,10 +43035,10 @@
       </c>
       <c r="K20" s="426"/>
       <c r="L20" s="159"/>
-      <c r="M20" s="774" t="s">
+      <c r="M20" s="776" t="s">
         <v>449</v>
       </c>
-      <c r="N20" s="775"/>
+      <c r="N20" s="777"/>
       <c r="O20" s="150"/>
       <c r="P20" s="150"/>
       <c r="Q20" s="130" t="s">
@@ -43068,10 +43046,10 @@
       </c>
       <c r="R20" s="426"/>
       <c r="S20" s="159"/>
-      <c r="T20" s="774" t="s">
+      <c r="T20" s="776" t="s">
         <v>449</v>
       </c>
-      <c r="U20" s="775"/>
+      <c r="U20" s="777"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="110"/>
@@ -43335,10 +43313,10 @@
       </c>
       <c r="C30" s="426"/>
       <c r="D30" s="159"/>
-      <c r="E30" s="774" t="s">
+      <c r="E30" s="776" t="s">
         <v>449</v>
       </c>
-      <c r="F30" s="775"/>
+      <c r="F30" s="777"/>
       <c r="G30" s="140"/>
       <c r="H30" s="140"/>
       <c r="I30" s="111"/>
@@ -43347,10 +43325,10 @@
       </c>
       <c r="K30" s="426"/>
       <c r="L30" s="159"/>
-      <c r="M30" s="774" t="s">
+      <c r="M30" s="776" t="s">
         <v>449</v>
       </c>
-      <c r="N30" s="775"/>
+      <c r="N30" s="777"/>
       <c r="O30" s="150"/>
       <c r="P30" s="150"/>
       <c r="Q30" s="130" t="s">
@@ -43358,10 +43336,10 @@
       </c>
       <c r="R30" s="426"/>
       <c r="S30" s="159"/>
-      <c r="T30" s="774" t="s">
+      <c r="T30" s="776" t="s">
         <v>449</v>
       </c>
-      <c r="U30" s="775"/>
+      <c r="U30" s="777"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="172"/>
@@ -43684,11 +43662,11 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="110"/>
-      <c r="B42" s="776"/>
-      <c r="C42" s="776"/>
-      <c r="D42" s="776"/>
-      <c r="E42" s="776"/>
-      <c r="F42" s="776"/>
+      <c r="B42" s="778"/>
+      <c r="C42" s="778"/>
+      <c r="D42" s="778"/>
+      <c r="E42" s="778"/>
+      <c r="F42" s="778"/>
       <c r="G42" s="150"/>
       <c r="H42" s="111"/>
       <c r="I42" s="150"/>
@@ -43884,8 +43862,8 @@
       <c r="B3" s="194" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="779"/>
-      <c r="D3" s="779"/>
+      <c r="C3" s="781"/>
+      <c r="D3" s="781"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C4" s="195"/>
@@ -43918,10 +43896,10 @@
       <c r="D10" s="203" t="s">
         <v>232</v>
       </c>
-      <c r="E10" s="780" t="s">
+      <c r="E10" s="782" t="s">
         <v>233</v>
       </c>
-      <c r="F10" s="781"/>
+      <c r="F10" s="783"/>
     </row>
     <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="204" t="s">
@@ -44072,10 +44050,10 @@
       <c r="D30" s="215" t="s">
         <v>232</v>
       </c>
-      <c r="E30" s="780" t="s">
+      <c r="E30" s="782" t="s">
         <v>233</v>
       </c>
-      <c r="F30" s="781"/>
+      <c r="F30" s="783"/>
     </row>
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="204" t="s">
@@ -44223,10 +44201,10 @@
       <c r="D49" s="215" t="s">
         <v>232</v>
       </c>
-      <c r="E49" s="780" t="s">
+      <c r="E49" s="782" t="s">
         <v>233</v>
       </c>
-      <c r="F49" s="781"/>
+      <c r="F49" s="783"/>
     </row>
     <row r="50" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="204" t="s">
@@ -44394,8 +44372,8 @@
       </c>
       <c r="C2" s="113"/>
       <c r="D2" s="113"/>
-      <c r="E2" s="770"/>
-      <c r="F2" s="770"/>
+      <c r="E2" s="772"/>
+      <c r="F2" s="772"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="112"/>
@@ -44427,13 +44405,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="110"/>
-      <c r="B6" s="771" t="s">
+      <c r="B6" s="773" t="s">
         <v>432</v>
       </c>
-      <c r="C6" s="771"/>
-      <c r="D6" s="771"/>
-      <c r="E6" s="771"/>
-      <c r="F6" s="771"/>
+      <c r="C6" s="773"/>
+      <c r="D6" s="773"/>
+      <c r="E6" s="773"/>
+      <c r="F6" s="773"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="110"/>
@@ -44448,14 +44426,14 @@
       <c r="B8" s="461" t="s">
         <v>203</v>
       </c>
-      <c r="C8" s="782" t="s">
+      <c r="C8" s="784" t="s">
         <v>204</v>
       </c>
-      <c r="D8" s="783"/>
-      <c r="E8" s="784" t="s">
+      <c r="D8" s="785"/>
+      <c r="E8" s="786" t="s">
         <v>205</v>
       </c>
-      <c r="F8" s="783"/>
+      <c r="F8" s="785"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="110"/>
@@ -44591,11 +44569,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="110"/>
-      <c r="B22" s="776"/>
-      <c r="C22" s="776"/>
-      <c r="D22" s="776"/>
-      <c r="E22" s="776"/>
-      <c r="F22" s="776"/>
+      <c r="B22" s="778"/>
+      <c r="C22" s="778"/>
+      <c r="D22" s="778"/>
+      <c r="E22" s="778"/>
+      <c r="F22" s="778"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="110"/>
@@ -44665,13 +44643,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="785" t="s">
+      <c r="B2" s="787" t="s">
         <v>250</v>
       </c>
-      <c r="C2" s="786" t="s">
+      <c r="C2" s="788" t="s">
         <v>251</v>
       </c>
-      <c r="D2" s="786" t="s">
+      <c r="D2" s="788" t="s">
         <v>150</v>
       </c>
       <c r="E2" s="232" t="s">
@@ -44706,9 +44684,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="785"/>
-      <c r="C3" s="787"/>
-      <c r="D3" s="787"/>
+      <c r="B3" s="787"/>
+      <c r="C3" s="789"/>
+      <c r="D3" s="789"/>
       <c r="E3" s="672" t="s">
         <v>259</v>
       </c>
@@ -44741,7 +44719,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="788" t="s">
+      <c r="B4" s="790" t="s">
         <v>262</v>
       </c>
       <c r="C4" s="233" t="s">
@@ -44760,7 +44738,7 @@
       <c r="N4" s="235"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="788"/>
+      <c r="B5" s="790"/>
       <c r="C5" s="233" t="s">
         <v>60</v>
       </c>
@@ -44777,7 +44755,7 @@
       <c r="N5" s="235"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="789"/>
+      <c r="B6" s="791"/>
       <c r="C6" s="562" t="s">
         <v>453</v>
       </c>
@@ -44871,155 +44849,180 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="46.85546875" customWidth="1"/>
-    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="1" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="13" max="13" width="46.85546875" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="588" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="790" t="s">
+    <row r="1" spans="1:15" s="588" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="792" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="791"/>
-      <c r="C1" s="792"/>
-      <c r="D1" s="793" t="s">
+      <c r="B1" s="793"/>
+      <c r="C1" s="793"/>
+      <c r="D1" s="794"/>
+      <c r="E1" s="795" t="s">
         <v>458</v>
       </c>
-      <c r="E1" s="793"/>
-      <c r="F1" s="794"/>
-      <c r="G1" s="803" t="s">
+      <c r="F1" s="795"/>
+      <c r="G1" s="796"/>
+      <c r="H1" s="805" t="s">
         <v>264</v>
       </c>
-      <c r="H1" s="804"/>
-      <c r="I1" s="804"/>
-      <c r="J1" s="804"/>
-      <c r="K1" s="805"/>
-      <c r="L1" s="795" t="s">
+      <c r="I1" s="806"/>
+      <c r="J1" s="806"/>
+      <c r="K1" s="806"/>
+      <c r="L1" s="807"/>
+      <c r="M1" s="797" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" s="588" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="N1" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="39"/>
+    </row>
+    <row r="2" spans="1:15" s="588" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="243" t="s">
+        <v>546</v>
+      </c>
+      <c r="B2" s="244" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="244" t="s">
+      <c r="C2" s="244" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="245" t="s">
+      <c r="D2" s="245" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="246" t="s">
+      <c r="E2" s="246" t="s">
         <v>266</v>
       </c>
-      <c r="E2" s="247" t="s">
+      <c r="F2" s="247" t="s">
         <v>236</v>
       </c>
-      <c r="F2" s="248" t="s">
+      <c r="G2" s="248" t="s">
         <v>267</v>
       </c>
-      <c r="G2" s="249">
+      <c r="H2" s="249">
         <v>0</v>
       </c>
-      <c r="H2" s="249">
+      <c r="I2" s="249">
         <v>1</v>
       </c>
-      <c r="I2" s="249">
+      <c r="J2" s="249">
         <v>2</v>
       </c>
-      <c r="J2" s="250" t="s">
+      <c r="K2" s="250" t="s">
         <v>268</v>
       </c>
-      <c r="K2" s="251" t="s">
+      <c r="L2" s="251" t="s">
         <v>269</v>
       </c>
-      <c r="L2" s="796"/>
-    </row>
-    <row r="3" spans="1:12" s="588" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="798"/>
+      <c r="N2" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" s="45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="588" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="252"/>
       <c r="B3" s="253"/>
-      <c r="C3" s="254" t="s">
+      <c r="C3" s="253"/>
+      <c r="D3" s="254" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="797" t="s">
+      <c r="E3" s="799" t="s">
         <v>270</v>
       </c>
-      <c r="E3" s="798"/>
-      <c r="F3" s="799"/>
-      <c r="G3" s="800" t="s">
+      <c r="F3" s="800"/>
+      <c r="G3" s="801"/>
+      <c r="H3" s="802" t="s">
         <v>270</v>
       </c>
-      <c r="H3" s="801"/>
-      <c r="I3" s="801"/>
-      <c r="J3" s="801"/>
-      <c r="K3" s="802"/>
-      <c r="L3" s="796"/>
-    </row>
-    <row r="4" spans="1:12" s="588" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="803"/>
+      <c r="J3" s="803"/>
+      <c r="K3" s="803"/>
+      <c r="L3" s="804"/>
+      <c r="M3" s="798"/>
+      <c r="N3" s="597"/>
+      <c r="O3" s="598"/>
+    </row>
+    <row r="4" spans="1:15" s="588" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="252"/>
       <c r="B4" s="253"/>
       <c r="C4" s="253"/>
-      <c r="D4" s="567"/>
+      <c r="D4" s="253"/>
       <c r="E4" s="567"/>
       <c r="F4" s="567"/>
-      <c r="G4" s="568"/>
+      <c r="G4" s="567"/>
       <c r="H4" s="568"/>
       <c r="I4" s="568"/>
       <c r="J4" s="568"/>
       <c r="K4" s="568"/>
-      <c r="L4" s="566"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="568"/>
+      <c r="M4" s="566"/>
+      <c r="N4" s="597"/>
+      <c r="O4" s="597"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="302"/>
-      <c r="B5" s="303"/>
-      <c r="C5" s="304"/>
-      <c r="D5" s="481"/>
-      <c r="E5" s="483"/>
+      <c r="B5" s="690"/>
+      <c r="C5" s="303"/>
+      <c r="D5" s="304"/>
+      <c r="E5" s="481"/>
       <c r="F5" s="483"/>
       <c r="G5" s="483"/>
       <c r="H5" s="483"/>
       <c r="I5" s="483"/>
       <c r="J5" s="483"/>
       <c r="K5" s="483"/>
-      <c r="L5" s="305"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="483"/>
+      <c r="O5" s="305"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="306"/>
-      <c r="B6" s="307"/>
-      <c r="C6" s="308"/>
-      <c r="D6" s="482"/>
-      <c r="E6" s="484"/>
-      <c r="F6" s="482"/>
-      <c r="G6" s="484"/>
+      <c r="B6" s="691"/>
+      <c r="C6" s="307"/>
+      <c r="D6" s="308"/>
+      <c r="E6" s="482"/>
+      <c r="F6" s="484"/>
+      <c r="G6" s="482"/>
       <c r="H6" s="484"/>
       <c r="I6" s="484"/>
       <c r="J6" s="484"/>
       <c r="K6" s="484"/>
-      <c r="L6" s="309"/>
+      <c r="L6" s="484"/>
+      <c r="M6" s="484"/>
+      <c r="N6" s="484"/>
+      <c r="O6" s="309"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:L4"/>
+  <autoFilter ref="A4:O4"/>
   <mergeCells count="6">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="L1:L3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="M1:M3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="H1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Register correction in sumamry big city
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2018_register_model_20181015.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2018_register_model_20181015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="17" r:id="rId1"/>
@@ -5571,6 +5571,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="69" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6009,9 +6012,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -6378,7 +6378,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{74B5685F-79AC-4FD1-B4D9-8D9988094225}" type="CELLRANGE">
+                    <a:fld id="{691DA024-59E2-45C3-8177-1329B0CCD024}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6409,7 +6409,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5516AA31-1FCE-41F7-9B4D-6130FC31144A}" type="CELLRANGE">
+                    <a:fld id="{E04A1F23-8048-4902-87AB-3CFDCF68BA81}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6613,7 +6613,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{74FB3516-ADA4-46BF-BF84-7D7199A6B7A0}" type="CELLRANGE">
+                    <a:fld id="{15EDE4B4-55B2-41F3-8116-6A2F4DDEFC43}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6644,7 +6644,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29783046-DC8C-4D7E-AFAD-E4DF2C1E5780}" type="CELLRANGE">
+                    <a:fld id="{B921E833-1845-4B3E-998C-04A550BEC955}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6794,11 +6794,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1877310768"/>
-        <c:axId val="-1997249552"/>
+        <c:axId val="724010688"/>
+        <c:axId val="724015040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1877310768"/>
+        <c:axId val="724010688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6841,7 +6841,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1997249552"/>
+        <c:crossAx val="724015040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6849,7 +6849,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1997249552"/>
+        <c:axId val="724015040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6941,7 +6941,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1877310768"/>
+        <c:crossAx val="724010688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7327,11 +7327,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1829390048"/>
-        <c:axId val="-1829391136"/>
+        <c:axId val="724012320"/>
+        <c:axId val="724022656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829390048"/>
+        <c:axId val="724012320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7429,7 +7429,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829391136"/>
+        <c:crossAx val="724022656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7437,7 +7437,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1829391136"/>
+        <c:axId val="724022656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7557,7 +7557,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829390048"/>
+        <c:crossAx val="724012320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8441,11 +8441,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1829387872"/>
-        <c:axId val="-1829388960"/>
+        <c:axId val="724010144"/>
+        <c:axId val="724016128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829387872"/>
+        <c:axId val="724010144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8548,7 +8548,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829388960"/>
+        <c:crossAx val="724016128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8556,7 +8556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1829388960"/>
+        <c:axId val="724016128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8607,7 +8607,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829387872"/>
+        <c:crossAx val="724010144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8972,11 +8972,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1829392224"/>
-        <c:axId val="-1829397664"/>
+        <c:axId val="724013952"/>
+        <c:axId val="724023200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829392224"/>
+        <c:axId val="724013952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9087,7 +9087,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829397664"/>
+        <c:crossAx val="724023200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9095,7 +9095,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1829397664"/>
+        <c:axId val="724023200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9201,7 +9201,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829392224"/>
+        <c:crossAx val="724013952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9571,11 +9571,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1829386784"/>
-        <c:axId val="-1829397120"/>
+        <c:axId val="724017760"/>
+        <c:axId val="724014496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829386784"/>
+        <c:axId val="724017760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9686,7 +9686,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829397120"/>
+        <c:crossAx val="724014496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9694,7 +9694,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1829397120"/>
+        <c:axId val="724014496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9808,7 +9808,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829386784"/>
+        <c:crossAx val="724017760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10289,11 +10289,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1829387328"/>
-        <c:axId val="-1829386240"/>
+        <c:axId val="724016672"/>
+        <c:axId val="724023744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829387328"/>
+        <c:axId val="724016672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10399,7 +10399,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829386240"/>
+        <c:crossAx val="724023744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10407,7 +10407,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1829386240"/>
+        <c:axId val="724023744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10529,7 +10529,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829387328"/>
+        <c:crossAx val="724016672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10865,11 +10865,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1829385696"/>
-        <c:axId val="-1829385152"/>
+        <c:axId val="727366224"/>
+        <c:axId val="727364592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829385696"/>
+        <c:axId val="727366224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10980,7 +10980,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829385152"/>
+        <c:crossAx val="727364592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10988,7 +10988,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1829385152"/>
+        <c:axId val="727364592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11102,7 +11102,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829385696"/>
+        <c:crossAx val="727366224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11438,11 +11438,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1829399296"/>
-        <c:axId val="-1829396576"/>
+        <c:axId val="727374384"/>
+        <c:axId val="727368944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829399296"/>
+        <c:axId val="727374384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11553,7 +11553,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829396576"/>
+        <c:crossAx val="727368944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11561,7 +11561,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1829396576"/>
+        <c:axId val="727368944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11675,7 +11675,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829399296"/>
+        <c:crossAx val="727374384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12056,11 +12056,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1829395488"/>
-        <c:axId val="-1829396032"/>
+        <c:axId val="727364048"/>
+        <c:axId val="727359152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829395488"/>
+        <c:axId val="727364048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12158,7 +12158,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829396032"/>
+        <c:crossAx val="727359152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12166,7 +12166,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1829396032"/>
+        <c:axId val="727359152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12285,7 +12285,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829395488"/>
+        <c:crossAx val="727364048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12790,11 +12790,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1829394944"/>
-        <c:axId val="-1829393312"/>
+        <c:axId val="727359696"/>
+        <c:axId val="727368400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829394944"/>
+        <c:axId val="727359696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12837,7 +12837,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829393312"/>
+        <c:crossAx val="727368400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12845,7 +12845,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1829393312"/>
+        <c:axId val="727368400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12951,7 +12951,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829394944"/>
+        <c:crossAx val="727359696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13187,7 +13187,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F1EDF10-22E9-4DC0-9FE0-CB36F9F1D2CE}" type="CELLRANGE">
+                    <a:fld id="{013A282C-7CBE-4D56-A3F1-67BB1790A90D}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13218,7 +13218,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9A713EAA-C1C2-4B55-92CD-F77D864F553B}" type="CELLRANGE">
+                    <a:fld id="{7FCDCFF2-268A-4081-9394-44ED42075411}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13422,7 +13422,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4C92FC6-BDCE-4324-ABA9-B6019CACE480}" type="CELLRANGE">
+                    <a:fld id="{F5E53786-5973-4110-BB14-B26BFA18DCD8}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13453,7 +13453,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40AC505A-FA69-4A51-B32A-DA38D9F86AA6}" type="CELLRANGE">
+                    <a:fld id="{7B7DC801-0C6A-4B71-A08B-0AF48A46BCFE}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13603,11 +13603,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1997241392"/>
-        <c:axId val="-1997240848"/>
+        <c:axId val="724024288"/>
+        <c:axId val="724012864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1997241392"/>
+        <c:axId val="724024288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13705,7 +13705,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1997240848"/>
+        <c:crossAx val="724012864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13713,7 +13713,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1997240848"/>
+        <c:axId val="724012864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13813,7 +13813,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1997241392"/>
+        <c:crossAx val="724024288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14232,11 +14232,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1829392768"/>
-        <c:axId val="-1873589248"/>
+        <c:axId val="727365136"/>
+        <c:axId val="727360784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829392768"/>
+        <c:axId val="727365136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14279,7 +14279,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1873589248"/>
+        <c:crossAx val="727360784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14287,7 +14287,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1873589248"/>
+        <c:axId val="727360784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14368,7 +14368,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829392768"/>
+        <c:crossAx val="727365136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15276,11 +15276,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-59155056"/>
-        <c:axId val="-59153424"/>
+        <c:axId val="724019936"/>
+        <c:axId val="724019392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-59155056"/>
+        <c:axId val="724019936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15378,7 +15378,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-59153424"/>
+        <c:crossAx val="724019392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15386,7 +15386,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-59153424"/>
+        <c:axId val="724019392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15492,7 +15492,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-59155056"/>
+        <c:crossAx val="724019936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15950,11 +15950,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1829400384"/>
-        <c:axId val="-1829393856"/>
+        <c:axId val="724021024"/>
+        <c:axId val="724021568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829400384"/>
+        <c:axId val="724021024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16052,7 +16052,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829393856"/>
+        <c:crossAx val="724021568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16060,7 +16060,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1829393856"/>
+        <c:axId val="724021568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16160,7 +16160,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829400384"/>
+        <c:crossAx val="724021024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16618,11 +16618,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1829398752"/>
-        <c:axId val="-1829388416"/>
+        <c:axId val="724022112"/>
+        <c:axId val="724009600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829398752"/>
+        <c:axId val="724022112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16720,7 +16720,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829388416"/>
+        <c:crossAx val="724009600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16728,7 +16728,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1829388416"/>
+        <c:axId val="724009600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16828,7 +16828,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829398752"/>
+        <c:crossAx val="724022112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17359,11 +17359,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1829389504"/>
-        <c:axId val="-1829398208"/>
+        <c:axId val="724018848"/>
+        <c:axId val="724011232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829389504"/>
+        <c:axId val="724018848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17406,7 +17406,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829398208"/>
+        <c:crossAx val="724011232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17414,7 +17414,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1829398208"/>
+        <c:axId val="724011232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17525,7 +17525,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829389504"/>
+        <c:crossAx val="724018848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18055,11 +18055,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1829399840"/>
-        <c:axId val="-1829394400"/>
+        <c:axId val="724015584"/>
+        <c:axId val="724020480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829399840"/>
+        <c:axId val="724015584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18102,7 +18102,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829394400"/>
+        <c:crossAx val="724020480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18110,7 +18110,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1829394400"/>
+        <c:axId val="724020480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18229,7 +18229,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829399840"/>
+        <c:crossAx val="724015584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18569,11 +18569,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1829390592"/>
-        <c:axId val="-1829391680"/>
+        <c:axId val="724011776"/>
+        <c:axId val="724013408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1829390592"/>
+        <c:axId val="724011776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18668,7 +18668,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829391680"/>
+        <c:crossAx val="724013408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18676,7 +18676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1829391680"/>
+        <c:axId val="724013408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -18796,7 +18796,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1829390592"/>
+        <c:crossAx val="724011776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -30742,9 +30742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -31100,23 +31098,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="570" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="721" t="s">
+      <c r="A1" s="722" t="s">
         <v>271</v>
       </c>
-      <c r="B1" s="722"/>
-      <c r="C1" s="722"/>
-      <c r="D1" s="722"/>
+      <c r="B1" s="723"/>
+      <c r="C1" s="723"/>
+      <c r="D1" s="723"/>
       <c r="E1" s="561"/>
-      <c r="F1" s="808" t="s">
+      <c r="F1" s="809" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="809"/>
-      <c r="H1" s="809"/>
+      <c r="G1" s="810"/>
+      <c r="H1" s="810"/>
       <c r="I1" s="566"/>
       <c r="J1" s="253"/>
       <c r="K1" s="566"/>
       <c r="L1" s="254"/>
-      <c r="M1" s="803" t="s">
+      <c r="M1" s="804" t="s">
         <v>272</v>
       </c>
       <c r="N1" s="255"/>
@@ -31128,19 +31126,19 @@
       <c r="R1" s="253"/>
       <c r="S1" s="566"/>
       <c r="T1" s="254"/>
-      <c r="U1" s="803" t="s">
+      <c r="U1" s="804" t="s">
         <v>274</v>
       </c>
       <c r="V1" s="255"/>
-      <c r="W1" s="810" t="s">
+      <c r="W1" s="811" t="s">
         <v>275</v>
       </c>
-      <c r="X1" s="810"/>
-      <c r="Y1" s="810"/>
-      <c r="Z1" s="810"/>
-      <c r="AA1" s="810"/>
-      <c r="AB1" s="811"/>
-      <c r="AC1" s="803" t="s">
+      <c r="X1" s="811"/>
+      <c r="Y1" s="811"/>
+      <c r="Z1" s="811"/>
+      <c r="AA1" s="811"/>
+      <c r="AB1" s="812"/>
+      <c r="AC1" s="804" t="s">
         <v>276</v>
       </c>
     </row>
@@ -31154,52 +31152,52 @@
       <c r="C2" s="565" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="805" t="s">
+      <c r="D2" s="806" t="s">
         <v>454</v>
       </c>
-      <c r="E2" s="805"/>
+      <c r="E2" s="806"/>
       <c r="F2" s="257"/>
-      <c r="G2" s="806" t="s">
+      <c r="G2" s="807" t="s">
         <v>160</v>
       </c>
-      <c r="H2" s="806"/>
-      <c r="I2" s="806" t="s">
+      <c r="H2" s="807"/>
+      <c r="I2" s="807" t="s">
         <v>161</v>
       </c>
-      <c r="J2" s="806"/>
-      <c r="K2" s="806" t="s">
+      <c r="J2" s="807"/>
+      <c r="K2" s="807" t="s">
         <v>162</v>
       </c>
-      <c r="L2" s="807"/>
-      <c r="M2" s="804"/>
+      <c r="L2" s="808"/>
+      <c r="M2" s="805"/>
       <c r="N2" s="258"/>
-      <c r="O2" s="806" t="s">
+      <c r="O2" s="807" t="s">
         <v>160</v>
       </c>
-      <c r="P2" s="806"/>
-      <c r="Q2" s="806" t="s">
+      <c r="P2" s="807"/>
+      <c r="Q2" s="807" t="s">
         <v>161</v>
       </c>
-      <c r="R2" s="806"/>
-      <c r="S2" s="806" t="s">
+      <c r="R2" s="807"/>
+      <c r="S2" s="807" t="s">
         <v>162</v>
       </c>
-      <c r="T2" s="807"/>
-      <c r="U2" s="804"/>
+      <c r="T2" s="808"/>
+      <c r="U2" s="805"/>
       <c r="V2" s="258"/>
-      <c r="W2" s="806" t="s">
+      <c r="W2" s="807" t="s">
         <v>160</v>
       </c>
-      <c r="X2" s="806"/>
-      <c r="Y2" s="806" t="s">
+      <c r="X2" s="807"/>
+      <c r="Y2" s="807" t="s">
         <v>161</v>
       </c>
-      <c r="Z2" s="806"/>
-      <c r="AA2" s="806" t="s">
+      <c r="Z2" s="807"/>
+      <c r="AA2" s="807" t="s">
         <v>162</v>
       </c>
-      <c r="AB2" s="807"/>
-      <c r="AC2" s="804"/>
+      <c r="AB2" s="808"/>
+      <c r="AC2" s="805"/>
     </row>
     <row r="3" spans="1:29" s="585" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A3" s="45"/>
@@ -31594,35 +31592,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="823" t="s">
+      <c r="A1" s="824" t="s">
         <v>437</v>
       </c>
-      <c r="B1" s="824"/>
-      <c r="C1" s="824"/>
+      <c r="B1" s="825"/>
+      <c r="C1" s="825"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="831" t="s">
+      <c r="A3" s="832" t="s">
         <v>319</v>
       </c>
-      <c r="B3" s="833" t="s">
+      <c r="B3" s="834" t="s">
         <v>411</v>
       </c>
-      <c r="C3" s="834"/>
-      <c r="D3" s="829" t="s">
+      <c r="C3" s="835"/>
+      <c r="D3" s="830" t="s">
         <v>438</v>
       </c>
-      <c r="E3" s="830"/>
-      <c r="AA3" s="813" t="s">
+      <c r="E3" s="831"/>
+      <c r="AA3" s="814" t="s">
         <v>332</v>
       </c>
-      <c r="AB3" s="813"/>
-      <c r="AC3" s="813" t="s">
+      <c r="AB3" s="814"/>
+      <c r="AC3" s="814" t="s">
         <v>416</v>
       </c>
-      <c r="AD3" s="813"/>
+      <c r="AD3" s="814"/>
     </row>
     <row r="4" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="832"/>
+      <c r="A4" s="833"/>
       <c r="B4" s="307" t="s">
         <v>415</v>
       </c>
@@ -31765,14 +31763,14 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="Z10" s="359"/>
-      <c r="AA10" s="813" t="s">
+      <c r="AA10" s="814" t="s">
         <v>417</v>
       </c>
-      <c r="AB10" s="813"/>
-      <c r="AC10" s="813" t="s">
+      <c r="AB10" s="814"/>
+      <c r="AC10" s="814" t="s">
         <v>418</v>
       </c>
-      <c r="AD10" s="813"/>
+      <c r="AD10" s="814"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="Z11" s="359" t="s">
@@ -31817,7 +31815,7 @@
       </c>
     </row>
     <row r="13" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="831" t="s">
+      <c r="A13" s="832" t="s">
         <v>320</v>
       </c>
       <c r="B13" s="306" t="str">
@@ -31849,7 +31847,7 @@
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="832"/>
+      <c r="A14" s="833"/>
       <c r="B14" s="309" t="s">
         <v>321</v>
       </c>
@@ -31935,27 +31933,27 @@
       <c r="A21" t="s">
         <v>422</v>
       </c>
-      <c r="B21" s="812" t="s">
+      <c r="B21" s="813" t="s">
         <v>431</v>
       </c>
-      <c r="C21" s="812"/>
-      <c r="D21" s="812"/>
-      <c r="E21" s="812"/>
+      <c r="C21" s="813"/>
+      <c r="D21" s="813"/>
+      <c r="E21" s="813"/>
     </row>
     <row r="22" spans="1:32" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="311" t="s">
         <v>283</v>
       </c>
-      <c r="B22" s="835" t="str">
+      <c r="B22" s="836" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C22" s="836"/>
-      <c r="D22" s="835" t="str">
+      <c r="C22" s="837"/>
+      <c r="D22" s="836" t="str">
         <f>D3</f>
         <v>[#previous_year#]*</v>
       </c>
-      <c r="E22" s="836"/>
+      <c r="E22" s="837"/>
     </row>
     <row r="23" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="312"/>
@@ -32330,16 +32328,16 @@
       <c r="A41" s="314" t="s">
         <v>330</v>
       </c>
-      <c r="B41" s="825" t="str">
+      <c r="B41" s="826" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C41" s="826"/>
-      <c r="D41" s="827" t="str">
+      <c r="C41" s="827"/>
+      <c r="D41" s="828" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E41" s="828"/>
+      <c r="E41" s="829"/>
       <c r="AA41" t="s">
         <v>412</v>
       </c>
@@ -32489,11 +32487,11 @@
       <c r="AA48" t="s">
         <v>422</v>
       </c>
-      <c r="AB48" s="812" t="s">
+      <c r="AB48" s="813" t="s">
         <v>443</v>
       </c>
-      <c r="AC48" s="812"/>
-      <c r="AD48" s="812"/>
+      <c r="AC48" s="813"/>
+      <c r="AD48" s="813"/>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" s="380" t="s">
@@ -32767,11 +32765,11 @@
       <c r="AA62" t="s">
         <v>422</v>
       </c>
-      <c r="AB62" s="812" t="s">
+      <c r="AB62" s="813" t="s">
         <v>444</v>
       </c>
-      <c r="AC62" s="812"/>
-      <c r="AD62" s="812"/>
+      <c r="AC62" s="813"/>
+      <c r="AD62" s="813"/>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A63" s="308"/>
@@ -33006,12 +33004,12 @@
       <c r="A74" s="526" t="s">
         <v>426</v>
       </c>
-      <c r="B74" s="812" t="s">
+      <c r="B74" s="813" t="s">
         <v>427</v>
       </c>
-      <c r="C74" s="812"/>
-      <c r="D74" s="812"/>
-      <c r="E74" s="812"/>
+      <c r="C74" s="813"/>
+      <c r="D74" s="813"/>
+      <c r="E74" s="813"/>
     </row>
     <row r="75" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="329" t="s">
@@ -33304,16 +33302,16 @@
       </c>
     </row>
     <row r="85" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B85" s="816" t="str">
+      <c r="B85" s="817" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C85" s="817"/>
-      <c r="D85" s="816" t="str">
+      <c r="C85" s="818"/>
+      <c r="D85" s="817" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E85" s="817"/>
+      <c r="E85" s="818"/>
       <c r="Z85" t="s">
         <v>401</v>
       </c>
@@ -33327,14 +33325,14 @@
     </row>
     <row r="86" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="201"/>
-      <c r="B86" s="818" t="s">
+      <c r="B86" s="819" t="s">
         <v>233</v>
       </c>
-      <c r="C86" s="779"/>
-      <c r="D86" s="818" t="s">
+      <c r="C86" s="780"/>
+      <c r="D86" s="819" t="s">
         <v>233</v>
       </c>
-      <c r="E86" s="779"/>
+      <c r="E86" s="780"/>
       <c r="Z86" s="337" t="s">
         <v>234</v>
       </c>
@@ -33540,27 +33538,27 @@
       </c>
     </row>
     <row r="101" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B101" s="816" t="str">
+      <c r="B101" s="817" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C101" s="817"/>
-      <c r="D101" s="816" t="str">
+      <c r="C101" s="818"/>
+      <c r="D101" s="817" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E101" s="817"/>
+      <c r="E101" s="818"/>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A102" s="201"/>
-      <c r="B102" s="818" t="s">
+      <c r="B102" s="819" t="s">
         <v>233</v>
       </c>
-      <c r="C102" s="779"/>
-      <c r="D102" s="818" t="s">
+      <c r="C102" s="780"/>
+      <c r="D102" s="819" t="s">
         <v>233</v>
       </c>
-      <c r="E102" s="779"/>
+      <c r="E102" s="780"/>
       <c r="Z102" t="s">
         <v>401</v>
       </c>
@@ -33774,27 +33772,27 @@
       </c>
     </row>
     <row r="116" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B116" s="819" t="str">
+      <c r="B116" s="820" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C116" s="820"/>
-      <c r="D116" s="819" t="str">
+      <c r="C116" s="821"/>
+      <c r="D116" s="820" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E116" s="820"/>
+      <c r="E116" s="821"/>
     </row>
     <row r="117" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A117" s="342"/>
-      <c r="B117" s="821" t="s">
+      <c r="B117" s="822" t="s">
         <v>233</v>
       </c>
-      <c r="C117" s="822"/>
-      <c r="D117" s="821" t="s">
+      <c r="C117" s="823"/>
+      <c r="D117" s="822" t="s">
         <v>233</v>
       </c>
-      <c r="E117" s="822"/>
+      <c r="E117" s="823"/>
       <c r="Z117" t="s">
         <v>401</v>
       </c>
@@ -34026,12 +34024,12 @@
       <c r="A129" s="346" t="s">
         <v>320</v>
       </c>
-      <c r="B129" s="814" t="str">
+      <c r="B129" s="815" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C129" s="815"/>
-      <c r="D129" s="815"/>
+      <c r="C129" s="816"/>
+      <c r="D129" s="816"/>
       <c r="Z129" t="str">
         <f>CONCATENATE("Collection 
 ", B3, " : target ", AB118, " p.e.")</f>
@@ -35158,54 +35156,54 @@
       <c r="AR3" s="5"/>
     </row>
     <row r="4" spans="1:44" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="688" t="s">
+      <c r="A4" s="689" t="s">
         <v>448</v>
       </c>
-      <c r="B4" s="689"/>
-      <c r="C4" s="689"/>
-      <c r="D4" s="689"/>
-      <c r="E4" s="690"/>
-      <c r="F4" s="690"/>
-      <c r="G4" s="690"/>
-      <c r="H4" s="690"/>
-      <c r="I4" s="690"/>
-      <c r="J4" s="690"/>
-      <c r="K4" s="690"/>
-      <c r="L4" s="690"/>
-      <c r="M4" s="690"/>
-      <c r="N4" s="690"/>
-      <c r="O4" s="690"/>
-      <c r="P4" s="690"/>
-      <c r="Q4" s="690"/>
-      <c r="R4" s="690"/>
-      <c r="S4" s="690"/>
-      <c r="T4" s="690"/>
-      <c r="U4" s="690"/>
-      <c r="V4" s="690"/>
-      <c r="W4" s="690"/>
-      <c r="X4" s="690"/>
-      <c r="Y4" s="690"/>
-      <c r="Z4" s="690"/>
-      <c r="AA4" s="690"/>
-      <c r="AB4" s="690"/>
-      <c r="AC4" s="690"/>
-      <c r="AD4" s="690"/>
-      <c r="AE4" s="690"/>
-      <c r="AF4" s="690"/>
-      <c r="AG4" s="690"/>
-      <c r="AH4" s="690"/>
-      <c r="AI4" s="690"/>
-      <c r="AJ4" s="690"/>
-      <c r="AK4" s="690"/>
-      <c r="AL4" s="690"/>
-      <c r="AM4" s="690"/>
-      <c r="AN4" s="690"/>
-      <c r="AO4" s="690"/>
-      <c r="AP4" s="690"/>
-      <c r="AQ4" s="691" t="s">
+      <c r="B4" s="690"/>
+      <c r="C4" s="690"/>
+      <c r="D4" s="690"/>
+      <c r="E4" s="691"/>
+      <c r="F4" s="691"/>
+      <c r="G4" s="691"/>
+      <c r="H4" s="691"/>
+      <c r="I4" s="691"/>
+      <c r="J4" s="691"/>
+      <c r="K4" s="691"/>
+      <c r="L4" s="691"/>
+      <c r="M4" s="691"/>
+      <c r="N4" s="691"/>
+      <c r="O4" s="691"/>
+      <c r="P4" s="691"/>
+      <c r="Q4" s="691"/>
+      <c r="R4" s="691"/>
+      <c r="S4" s="691"/>
+      <c r="T4" s="691"/>
+      <c r="U4" s="691"/>
+      <c r="V4" s="691"/>
+      <c r="W4" s="691"/>
+      <c r="X4" s="691"/>
+      <c r="Y4" s="691"/>
+      <c r="Z4" s="691"/>
+      <c r="AA4" s="691"/>
+      <c r="AB4" s="691"/>
+      <c r="AC4" s="691"/>
+      <c r="AD4" s="691"/>
+      <c r="AE4" s="691"/>
+      <c r="AF4" s="691"/>
+      <c r="AG4" s="691"/>
+      <c r="AH4" s="691"/>
+      <c r="AI4" s="691"/>
+      <c r="AJ4" s="691"/>
+      <c r="AK4" s="691"/>
+      <c r="AL4" s="691"/>
+      <c r="AM4" s="691"/>
+      <c r="AN4" s="691"/>
+      <c r="AO4" s="691"/>
+      <c r="AP4" s="691"/>
+      <c r="AQ4" s="692" t="s">
         <v>2</v>
       </c>
-      <c r="AR4" s="691"/>
+      <c r="AR4" s="692"/>
     </row>
     <row r="5" spans="1:44" s="569" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="297" t="s">
@@ -35393,123 +35391,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" s="570" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="721" t="s">
+      <c r="A1" s="722" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="722"/>
-      <c r="C1" s="722"/>
-      <c r="D1" s="722"/>
-      <c r="E1" s="722"/>
-      <c r="F1" s="722"/>
-      <c r="G1" s="722"/>
-      <c r="H1" s="723" t="s">
+      <c r="B1" s="723"/>
+      <c r="C1" s="723"/>
+      <c r="D1" s="723"/>
+      <c r="E1" s="723"/>
+      <c r="F1" s="723"/>
+      <c r="G1" s="723"/>
+      <c r="H1" s="724" t="s">
         <v>138</v>
       </c>
-      <c r="I1" s="724"/>
-      <c r="J1" s="724"/>
-      <c r="K1" s="724"/>
-      <c r="L1" s="724"/>
-      <c r="M1" s="725"/>
-      <c r="N1" s="726" t="s">
+      <c r="I1" s="725"/>
+      <c r="J1" s="725"/>
+      <c r="K1" s="725"/>
+      <c r="L1" s="725"/>
+      <c r="M1" s="726"/>
+      <c r="N1" s="727" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="704"/>
-      <c r="P1" s="704"/>
-      <c r="Q1" s="727"/>
-      <c r="R1" s="727"/>
-      <c r="S1" s="704"/>
-      <c r="T1" s="704"/>
-      <c r="U1" s="704"/>
-      <c r="V1" s="728" t="s">
+      <c r="O1" s="705"/>
+      <c r="P1" s="705"/>
+      <c r="Q1" s="728"/>
+      <c r="R1" s="728"/>
+      <c r="S1" s="705"/>
+      <c r="T1" s="705"/>
+      <c r="U1" s="705"/>
+      <c r="V1" s="729" t="s">
         <v>49</v>
       </c>
-      <c r="W1" s="729"/>
-      <c r="X1" s="730"/>
-      <c r="Y1" s="730"/>
-      <c r="Z1" s="731"/>
-      <c r="AA1" s="732" t="s">
+      <c r="W1" s="730"/>
+      <c r="X1" s="731"/>
+      <c r="Y1" s="731"/>
+      <c r="Z1" s="732"/>
+      <c r="AA1" s="733" t="s">
         <v>50</v>
       </c>
-      <c r="AB1" s="733"/>
-      <c r="AC1" s="733"/>
-      <c r="AD1" s="733"/>
-      <c r="AE1" s="733"/>
-      <c r="AF1" s="733"/>
-      <c r="AG1" s="733"/>
-      <c r="AH1" s="733"/>
-      <c r="AI1" s="733"/>
-      <c r="AJ1" s="733"/>
-      <c r="AK1" s="733"/>
-      <c r="AL1" s="733"/>
-      <c r="AM1" s="733"/>
+      <c r="AB1" s="734"/>
+      <c r="AC1" s="734"/>
+      <c r="AD1" s="734"/>
+      <c r="AE1" s="734"/>
+      <c r="AF1" s="734"/>
+      <c r="AG1" s="734"/>
+      <c r="AH1" s="734"/>
+      <c r="AI1" s="734"/>
+      <c r="AJ1" s="734"/>
+      <c r="AK1" s="734"/>
+      <c r="AL1" s="734"/>
+      <c r="AM1" s="734"/>
       <c r="AN1" s="7"/>
       <c r="AO1" s="8"/>
-      <c r="AP1" s="703" t="s">
+      <c r="AP1" s="704" t="s">
         <v>51</v>
       </c>
-      <c r="AQ1" s="704"/>
-      <c r="AR1" s="704"/>
-      <c r="AS1" s="704"/>
-      <c r="AT1" s="704"/>
-      <c r="AU1" s="704"/>
-      <c r="AV1" s="704"/>
-      <c r="AW1" s="705"/>
-      <c r="AX1" s="712" t="s">
+      <c r="AQ1" s="705"/>
+      <c r="AR1" s="705"/>
+      <c r="AS1" s="705"/>
+      <c r="AT1" s="705"/>
+      <c r="AU1" s="705"/>
+      <c r="AV1" s="705"/>
+      <c r="AW1" s="706"/>
+      <c r="AX1" s="713" t="s">
         <v>52</v>
       </c>
-      <c r="AY1" s="713"/>
-      <c r="AZ1" s="713"/>
-      <c r="BA1" s="713"/>
-      <c r="BB1" s="713"/>
-      <c r="BC1" s="714"/>
-      <c r="BD1" s="715" t="s">
+      <c r="AY1" s="714"/>
+      <c r="AZ1" s="714"/>
+      <c r="BA1" s="714"/>
+      <c r="BB1" s="714"/>
+      <c r="BC1" s="715"/>
+      <c r="BD1" s="716" t="s">
         <v>53</v>
       </c>
-      <c r="BE1" s="716"/>
-      <c r="BF1" s="716"/>
-      <c r="BG1" s="716"/>
-      <c r="BH1" s="716"/>
-      <c r="BI1" s="717"/>
-      <c r="BJ1" s="718" t="s">
+      <c r="BE1" s="717"/>
+      <c r="BF1" s="717"/>
+      <c r="BG1" s="717"/>
+      <c r="BH1" s="717"/>
+      <c r="BI1" s="718"/>
+      <c r="BJ1" s="719" t="s">
         <v>54</v>
       </c>
-      <c r="BK1" s="719"/>
-      <c r="BL1" s="719"/>
-      <c r="BM1" s="719"/>
-      <c r="BN1" s="719"/>
-      <c r="BO1" s="719"/>
-      <c r="BP1" s="720"/>
-      <c r="BQ1" s="692" t="s">
+      <c r="BK1" s="720"/>
+      <c r="BL1" s="720"/>
+      <c r="BM1" s="720"/>
+      <c r="BN1" s="720"/>
+      <c r="BO1" s="720"/>
+      <c r="BP1" s="721"/>
+      <c r="BQ1" s="693" t="s">
         <v>55</v>
       </c>
-      <c r="BR1" s="693"/>
-      <c r="BS1" s="693"/>
-      <c r="BT1" s="693"/>
-      <c r="BU1" s="693"/>
-      <c r="BV1" s="693"/>
+      <c r="BR1" s="694"/>
+      <c r="BS1" s="694"/>
+      <c r="BT1" s="694"/>
+      <c r="BU1" s="694"/>
+      <c r="BV1" s="694"/>
       <c r="BW1" s="8"/>
       <c r="BX1" s="9"/>
-      <c r="BY1" s="694" t="s">
+      <c r="BY1" s="695" t="s">
         <v>56</v>
       </c>
-      <c r="BZ1" s="695"/>
-      <c r="CA1" s="695"/>
-      <c r="CB1" s="695"/>
-      <c r="CC1" s="695"/>
-      <c r="CD1" s="695"/>
-      <c r="CE1" s="695"/>
-      <c r="CF1" s="696"/>
-      <c r="CG1" s="696"/>
-      <c r="CH1" s="696"/>
-      <c r="CI1" s="696"/>
-      <c r="CJ1" s="696"/>
-      <c r="CK1" s="696"/>
-      <c r="CL1" s="696"/>
-      <c r="CM1" s="696"/>
-      <c r="CN1" s="696"/>
-      <c r="CO1" s="696"/>
-      <c r="CP1" s="696"/>
-      <c r="CQ1" s="696"/>
+      <c r="BZ1" s="696"/>
+      <c r="CA1" s="696"/>
+      <c r="CB1" s="696"/>
+      <c r="CC1" s="696"/>
+      <c r="CD1" s="696"/>
+      <c r="CE1" s="696"/>
+      <c r="CF1" s="697"/>
+      <c r="CG1" s="697"/>
+      <c r="CH1" s="697"/>
+      <c r="CI1" s="697"/>
+      <c r="CJ1" s="697"/>
+      <c r="CK1" s="697"/>
+      <c r="CL1" s="697"/>
+      <c r="CM1" s="697"/>
+      <c r="CN1" s="697"/>
+      <c r="CO1" s="697"/>
+      <c r="CP1" s="697"/>
+      <c r="CQ1" s="697"/>
     </row>
     <row r="2" spans="1:95" s="570" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -35533,18 +35531,18 @@
       <c r="G2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="697" t="s">
+      <c r="H2" s="698" t="s">
         <v>155</v>
       </c>
-      <c r="I2" s="698"/>
-      <c r="J2" s="698" t="s">
+      <c r="I2" s="699"/>
+      <c r="J2" s="699" t="s">
         <v>64</v>
       </c>
-      <c r="K2" s="698"/>
-      <c r="L2" s="698" t="s">
+      <c r="K2" s="699"/>
+      <c r="L2" s="699" t="s">
         <v>65</v>
       </c>
-      <c r="M2" s="699"/>
+      <c r="M2" s="700"/>
       <c r="N2" s="12" t="s">
         <v>57</v>
       </c>
@@ -35653,36 +35651,36 @@
       <c r="AW2" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="AX2" s="700" t="s">
+      <c r="AX2" s="701" t="s">
         <v>90</v>
       </c>
-      <c r="AY2" s="701"/>
-      <c r="AZ2" s="701"/>
-      <c r="BA2" s="701" t="s">
+      <c r="AY2" s="702"/>
+      <c r="AZ2" s="702"/>
+      <c r="BA2" s="702" t="s">
         <v>91</v>
       </c>
-      <c r="BB2" s="701"/>
-      <c r="BC2" s="702"/>
-      <c r="BD2" s="706" t="s">
+      <c r="BB2" s="702"/>
+      <c r="BC2" s="703"/>
+      <c r="BD2" s="707" t="s">
         <v>90</v>
       </c>
-      <c r="BE2" s="707"/>
-      <c r="BF2" s="707"/>
-      <c r="BG2" s="707" t="s">
+      <c r="BE2" s="708"/>
+      <c r="BF2" s="708"/>
+      <c r="BG2" s="708" t="s">
         <v>91</v>
       </c>
-      <c r="BH2" s="707"/>
-      <c r="BI2" s="708"/>
-      <c r="BJ2" s="709" t="s">
+      <c r="BH2" s="708"/>
+      <c r="BI2" s="709"/>
+      <c r="BJ2" s="710" t="s">
         <v>90</v>
       </c>
-      <c r="BK2" s="710"/>
-      <c r="BL2" s="710"/>
-      <c r="BM2" s="710" t="s">
+      <c r="BK2" s="711"/>
+      <c r="BL2" s="711"/>
+      <c r="BM2" s="711" t="s">
         <v>91</v>
       </c>
-      <c r="BN2" s="711"/>
-      <c r="BO2" s="711"/>
+      <c r="BN2" s="712"/>
+      <c r="BO2" s="712"/>
       <c r="BP2" s="24" t="s">
         <v>92</v>
       </c>
@@ -36795,124 +36793,124 @@
         <v>135</v>
       </c>
       <c r="L1" s="42"/>
-      <c r="M1" s="761" t="s">
+      <c r="M1" s="762" t="s">
         <v>136</v>
       </c>
-      <c r="N1" s="762" t="s">
+      <c r="N1" s="763" t="s">
         <v>137</v>
       </c>
-      <c r="O1" s="763"/>
-      <c r="P1" s="763"/>
-      <c r="Q1" s="763"/>
-      <c r="R1" s="764" t="s">
+      <c r="O1" s="764"/>
+      <c r="P1" s="764"/>
+      <c r="Q1" s="764"/>
+      <c r="R1" s="765" t="s">
         <v>138</v>
       </c>
-      <c r="S1" s="756"/>
-      <c r="T1" s="756"/>
-      <c r="U1" s="756"/>
-      <c r="V1" s="756"/>
-      <c r="W1" s="756"/>
-      <c r="X1" s="765"/>
-      <c r="Y1" s="744" t="s">
+      <c r="S1" s="757"/>
+      <c r="T1" s="757"/>
+      <c r="U1" s="757"/>
+      <c r="V1" s="757"/>
+      <c r="W1" s="757"/>
+      <c r="X1" s="766"/>
+      <c r="Y1" s="745" t="s">
         <v>139</v>
       </c>
-      <c r="Z1" s="745"/>
-      <c r="AA1" s="766" t="s">
+      <c r="Z1" s="746"/>
+      <c r="AA1" s="767" t="s">
         <v>140</v>
       </c>
-      <c r="AB1" s="757" t="s">
+      <c r="AB1" s="758" t="s">
         <v>141</v>
       </c>
-      <c r="AC1" s="752" t="s">
+      <c r="AC1" s="753" t="s">
         <v>457</v>
       </c>
-      <c r="AD1" s="753"/>
-      <c r="AE1" s="753"/>
-      <c r="AF1" s="754"/>
-      <c r="AG1" s="755" t="s">
+      <c r="AD1" s="754"/>
+      <c r="AE1" s="754"/>
+      <c r="AF1" s="755"/>
+      <c r="AG1" s="756" t="s">
         <v>142</v>
       </c>
-      <c r="AH1" s="756"/>
-      <c r="AI1" s="756"/>
-      <c r="AJ1" s="756"/>
-      <c r="AK1" s="756"/>
-      <c r="AL1" s="756"/>
-      <c r="AM1" s="756"/>
-      <c r="AN1" s="756"/>
-      <c r="AO1" s="757" t="s">
+      <c r="AH1" s="757"/>
+      <c r="AI1" s="757"/>
+      <c r="AJ1" s="757"/>
+      <c r="AK1" s="757"/>
+      <c r="AL1" s="757"/>
+      <c r="AM1" s="757"/>
+      <c r="AN1" s="757"/>
+      <c r="AO1" s="758" t="s">
         <v>143</v>
       </c>
-      <c r="AP1" s="744" t="s">
+      <c r="AP1" s="745" t="s">
         <v>144</v>
       </c>
-      <c r="AQ1" s="745"/>
-      <c r="AR1" s="745"/>
-      <c r="AS1" s="717"/>
-      <c r="AT1" s="759" t="s">
+      <c r="AQ1" s="746"/>
+      <c r="AR1" s="746"/>
+      <c r="AS1" s="718"/>
+      <c r="AT1" s="760" t="s">
         <v>145</v>
       </c>
-      <c r="AU1" s="760"/>
-      <c r="AV1" s="760"/>
-      <c r="AW1" s="760"/>
-      <c r="AX1" s="760"/>
-      <c r="AY1" s="760"/>
-      <c r="AZ1" s="760"/>
-      <c r="BA1" s="760"/>
-      <c r="BB1" s="760"/>
-      <c r="BC1" s="760"/>
-      <c r="BD1" s="760"/>
-      <c r="BE1" s="760"/>
-      <c r="BF1" s="760"/>
-      <c r="BG1" s="760"/>
-      <c r="BH1" s="760"/>
-      <c r="BI1" s="760"/>
-      <c r="BJ1" s="760"/>
-      <c r="BK1" s="760"/>
-      <c r="BL1" s="760"/>
-      <c r="BM1" s="760"/>
-      <c r="BN1" s="760"/>
-      <c r="BO1" s="760"/>
-      <c r="BP1" s="760"/>
-      <c r="BQ1" s="760"/>
-      <c r="BR1" s="760"/>
-      <c r="BS1" s="760"/>
-      <c r="BT1" s="760"/>
-      <c r="BU1" s="760"/>
-      <c r="BV1" s="760"/>
-      <c r="BW1" s="757" t="s">
+      <c r="AU1" s="761"/>
+      <c r="AV1" s="761"/>
+      <c r="AW1" s="761"/>
+      <c r="AX1" s="761"/>
+      <c r="AY1" s="761"/>
+      <c r="AZ1" s="761"/>
+      <c r="BA1" s="761"/>
+      <c r="BB1" s="761"/>
+      <c r="BC1" s="761"/>
+      <c r="BD1" s="761"/>
+      <c r="BE1" s="761"/>
+      <c r="BF1" s="761"/>
+      <c r="BG1" s="761"/>
+      <c r="BH1" s="761"/>
+      <c r="BI1" s="761"/>
+      <c r="BJ1" s="761"/>
+      <c r="BK1" s="761"/>
+      <c r="BL1" s="761"/>
+      <c r="BM1" s="761"/>
+      <c r="BN1" s="761"/>
+      <c r="BO1" s="761"/>
+      <c r="BP1" s="761"/>
+      <c r="BQ1" s="761"/>
+      <c r="BR1" s="761"/>
+      <c r="BS1" s="761"/>
+      <c r="BT1" s="761"/>
+      <c r="BU1" s="761"/>
+      <c r="BV1" s="761"/>
+      <c r="BW1" s="758" t="s">
         <v>146</v>
       </c>
-      <c r="BX1" s="744" t="s">
+      <c r="BX1" s="745" t="s">
         <v>147</v>
       </c>
-      <c r="BY1" s="745"/>
-      <c r="BZ1" s="745"/>
-      <c r="CA1" s="717"/>
-      <c r="CB1" s="746" t="s">
+      <c r="BY1" s="746"/>
+      <c r="BZ1" s="746"/>
+      <c r="CA1" s="718"/>
+      <c r="CB1" s="747" t="s">
         <v>50</v>
       </c>
-      <c r="CC1" s="746"/>
-      <c r="CD1" s="746"/>
-      <c r="CE1" s="746"/>
-      <c r="CF1" s="746"/>
-      <c r="CG1" s="746"/>
-      <c r="CH1" s="746"/>
-      <c r="CI1" s="746"/>
-      <c r="CJ1" s="746"/>
-      <c r="CK1" s="746"/>
-      <c r="CL1" s="746"/>
-      <c r="CM1" s="746"/>
+      <c r="CC1" s="747"/>
+      <c r="CD1" s="747"/>
+      <c r="CE1" s="747"/>
+      <c r="CF1" s="747"/>
+      <c r="CG1" s="747"/>
+      <c r="CH1" s="747"/>
+      <c r="CI1" s="747"/>
+      <c r="CJ1" s="747"/>
+      <c r="CK1" s="747"/>
+      <c r="CL1" s="747"/>
+      <c r="CM1" s="747"/>
       <c r="CN1" s="43"/>
-      <c r="CO1" s="747" t="s">
+      <c r="CO1" s="748" t="s">
         <v>55</v>
       </c>
-      <c r="CP1" s="727"/>
-      <c r="CQ1" s="727"/>
-      <c r="CR1" s="727"/>
-      <c r="CS1" s="727"/>
-      <c r="CT1" s="727"/>
-      <c r="CU1" s="727"/>
-      <c r="CV1" s="705"/>
+      <c r="CP1" s="728"/>
+      <c r="CQ1" s="728"/>
+      <c r="CR1" s="728"/>
+      <c r="CS1" s="728"/>
+      <c r="CT1" s="728"/>
+      <c r="CU1" s="728"/>
+      <c r="CV1" s="706"/>
     </row>
     <row r="2" spans="1:100" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
@@ -36951,7 +36949,7 @@
       <c r="L2" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="M2" s="761"/>
+      <c r="M2" s="762"/>
       <c r="N2" s="49" t="s">
         <v>152</v>
       </c>
@@ -36967,22 +36965,22 @@
       <c r="R2" s="575" t="s">
         <v>397</v>
       </c>
-      <c r="S2" s="748" t="s">
+      <c r="S2" s="749" t="s">
         <v>155</v>
       </c>
-      <c r="T2" s="711"/>
-      <c r="U2" s="749" t="s">
+      <c r="T2" s="712"/>
+      <c r="U2" s="750" t="s">
         <v>64</v>
       </c>
-      <c r="V2" s="749"/>
-      <c r="W2" s="749" t="s">
+      <c r="V2" s="750"/>
+      <c r="W2" s="750" t="s">
         <v>65</v>
       </c>
-      <c r="X2" s="750"/>
-      <c r="Y2" s="738"/>
-      <c r="Z2" s="739"/>
-      <c r="AA2" s="767"/>
-      <c r="AB2" s="758"/>
+      <c r="X2" s="751"/>
+      <c r="Y2" s="739"/>
+      <c r="Z2" s="740"/>
+      <c r="AA2" s="768"/>
+      <c r="AB2" s="759"/>
       <c r="AC2" s="50" t="s">
         <v>156</v>
       </c>
@@ -36995,81 +36993,81 @@
       <c r="AF2" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="AG2" s="751" t="s">
+      <c r="AG2" s="752" t="s">
         <v>160</v>
       </c>
-      <c r="AH2" s="736"/>
-      <c r="AI2" s="736" t="s">
+      <c r="AH2" s="737"/>
+      <c r="AI2" s="737" t="s">
         <v>161</v>
       </c>
-      <c r="AJ2" s="736"/>
-      <c r="AK2" s="736" t="s">
+      <c r="AJ2" s="737"/>
+      <c r="AK2" s="737" t="s">
         <v>162</v>
       </c>
-      <c r="AL2" s="736"/>
+      <c r="AL2" s="737"/>
       <c r="AM2" s="51" t="s">
         <v>461</v>
       </c>
       <c r="AN2" s="51" t="s">
         <v>462</v>
       </c>
-      <c r="AO2" s="758"/>
-      <c r="AP2" s="738" t="s">
+      <c r="AO2" s="759"/>
+      <c r="AP2" s="739" t="s">
         <v>163</v>
       </c>
-      <c r="AQ2" s="739"/>
-      <c r="AR2" s="740" t="s">
+      <c r="AQ2" s="740"/>
+      <c r="AR2" s="741" t="s">
         <v>164</v>
       </c>
-      <c r="AS2" s="741"/>
-      <c r="AT2" s="736" t="s">
+      <c r="AS2" s="742"/>
+      <c r="AT2" s="737" t="s">
         <v>165</v>
       </c>
-      <c r="AU2" s="736"/>
-      <c r="AV2" s="737" t="s">
+      <c r="AU2" s="737"/>
+      <c r="AV2" s="738" t="s">
         <v>166</v>
       </c>
-      <c r="AW2" s="737"/>
-      <c r="AX2" s="737" t="s">
+      <c r="AW2" s="738"/>
+      <c r="AX2" s="738" t="s">
         <v>167</v>
       </c>
-      <c r="AY2" s="737"/>
+      <c r="AY2" s="738"/>
       <c r="AZ2" s="51" t="s">
         <v>463</v>
       </c>
       <c r="BA2" s="51" t="s">
         <v>464</v>
       </c>
-      <c r="BB2" s="736" t="s">
+      <c r="BB2" s="737" t="s">
         <v>168</v>
       </c>
-      <c r="BC2" s="736"/>
-      <c r="BD2" s="737" t="s">
+      <c r="BC2" s="737"/>
+      <c r="BD2" s="738" t="s">
         <v>169</v>
       </c>
-      <c r="BE2" s="737"/>
-      <c r="BF2" s="737" t="s">
+      <c r="BE2" s="738"/>
+      <c r="BF2" s="738" t="s">
         <v>170</v>
       </c>
-      <c r="BG2" s="737"/>
+      <c r="BG2" s="738"/>
       <c r="BH2" s="51" t="s">
         <v>465</v>
       </c>
       <c r="BI2" s="51" t="s">
         <v>466</v>
       </c>
-      <c r="BJ2" s="736" t="s">
+      <c r="BJ2" s="737" t="s">
         <v>171</v>
       </c>
-      <c r="BK2" s="736"/>
-      <c r="BL2" s="737" t="s">
+      <c r="BK2" s="737"/>
+      <c r="BL2" s="738" t="s">
         <v>172</v>
       </c>
-      <c r="BM2" s="737"/>
-      <c r="BN2" s="737" t="s">
+      <c r="BM2" s="738"/>
+      <c r="BN2" s="738" t="s">
         <v>173</v>
       </c>
-      <c r="BO2" s="737"/>
+      <c r="BO2" s="738"/>
       <c r="BP2" s="51" t="s">
         <v>467</v>
       </c>
@@ -37091,15 +37089,15 @@
       <c r="BV2" s="51" t="s">
         <v>469</v>
       </c>
-      <c r="BW2" s="758"/>
-      <c r="BX2" s="738" t="s">
+      <c r="BW2" s="759"/>
+      <c r="BX2" s="739" t="s">
         <v>163</v>
       </c>
-      <c r="BY2" s="739"/>
-      <c r="BZ2" s="740" t="s">
+      <c r="BY2" s="740"/>
+      <c r="BZ2" s="741" t="s">
         <v>164</v>
       </c>
-      <c r="CA2" s="741"/>
+      <c r="CA2" s="742"/>
       <c r="CB2" s="20" t="s">
         <v>71</v>
       </c>
@@ -37139,22 +37137,22 @@
       <c r="CN2" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="CO2" s="742" t="s">
+      <c r="CO2" s="743" t="s">
         <v>178</v>
       </c>
-      <c r="CP2" s="743"/>
-      <c r="CQ2" s="734" t="s">
+      <c r="CP2" s="744"/>
+      <c r="CQ2" s="735" t="s">
         <v>179</v>
       </c>
-      <c r="CR2" s="734"/>
-      <c r="CS2" s="743" t="s">
+      <c r="CR2" s="735"/>
+      <c r="CS2" s="744" t="s">
         <v>180</v>
       </c>
-      <c r="CT2" s="743"/>
-      <c r="CU2" s="734" t="s">
+      <c r="CT2" s="744"/>
+      <c r="CU2" s="735" t="s">
         <v>181</v>
       </c>
-      <c r="CV2" s="735"/>
+      <c r="CV2" s="736"/>
     </row>
     <row r="3" spans="1:100" s="2" customFormat="1" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A3" s="593"/>
@@ -42436,8 +42434,8 @@
       <c r="B2" s="113" t="s">
         <v>196</v>
       </c>
-      <c r="C2" s="775"/>
-      <c r="D2" s="775"/>
+      <c r="C2" s="776"/>
+      <c r="D2" s="776"/>
       <c r="E2" s="111"/>
       <c r="F2" s="111"/>
       <c r="G2" s="111"/>
@@ -42562,32 +42560,32 @@
     </row>
     <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="110"/>
-      <c r="B7" s="776" t="s">
+      <c r="B7" s="777" t="s">
         <v>436</v>
       </c>
-      <c r="C7" s="776"/>
-      <c r="D7" s="776"/>
+      <c r="C7" s="777"/>
+      <c r="D7" s="777"/>
       <c r="E7" s="111"/>
       <c r="F7" s="111"/>
       <c r="G7" s="111"/>
       <c r="H7" s="111"/>
       <c r="I7" s="111"/>
-      <c r="J7" s="776" t="s">
+      <c r="J7" s="777" t="s">
         <v>200</v>
       </c>
-      <c r="K7" s="776"/>
-      <c r="L7" s="776"/>
+      <c r="K7" s="777"/>
+      <c r="L7" s="777"/>
       <c r="M7" s="111"/>
       <c r="N7" s="111"/>
       <c r="O7" s="111"/>
       <c r="P7" s="112" t="s">
         <v>201</v>
       </c>
-      <c r="Q7" s="776" t="s">
+      <c r="Q7" s="777" t="s">
         <v>200</v>
       </c>
-      <c r="R7" s="776"/>
-      <c r="S7" s="776"/>
+      <c r="R7" s="777"/>
+      <c r="S7" s="777"/>
       <c r="T7" s="111"/>
       <c r="U7" s="125" t="s">
         <v>202</v>
@@ -42621,41 +42619,41 @@
       <c r="B9" s="126" t="s">
         <v>433</v>
       </c>
-      <c r="C9" s="771" t="s">
+      <c r="C9" s="772" t="s">
         <v>204</v>
       </c>
-      <c r="D9" s="772"/>
-      <c r="E9" s="771" t="s">
+      <c r="D9" s="773"/>
+      <c r="E9" s="772" t="s">
         <v>205</v>
       </c>
-      <c r="F9" s="772"/>
+      <c r="F9" s="773"/>
       <c r="G9" s="111"/>
       <c r="H9" s="111"/>
       <c r="I9" s="111"/>
       <c r="J9" s="126" t="s">
         <v>433</v>
       </c>
-      <c r="K9" s="771" t="s">
+      <c r="K9" s="772" t="s">
         <v>204</v>
       </c>
-      <c r="L9" s="772"/>
-      <c r="M9" s="771" t="s">
+      <c r="L9" s="773"/>
+      <c r="M9" s="772" t="s">
         <v>205</v>
       </c>
-      <c r="N9" s="772"/>
+      <c r="N9" s="773"/>
       <c r="O9" s="111"/>
       <c r="P9" s="111"/>
       <c r="Q9" s="126" t="s">
         <v>203</v>
       </c>
-      <c r="R9" s="771" t="s">
+      <c r="R9" s="772" t="s">
         <v>204</v>
       </c>
-      <c r="S9" s="772"/>
-      <c r="T9" s="771" t="s">
+      <c r="S9" s="773"/>
+      <c r="T9" s="772" t="s">
         <v>205</v>
       </c>
-      <c r="U9" s="772"/>
+      <c r="U9" s="773"/>
     </row>
     <row r="10" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="110"/>
@@ -42717,10 +42715,10 @@
       </c>
       <c r="C11" s="131"/>
       <c r="D11" s="131"/>
-      <c r="E11" s="768" t="s">
+      <c r="E11" s="769" t="s">
         <v>210</v>
       </c>
-      <c r="F11" s="769"/>
+      <c r="F11" s="770"/>
       <c r="G11" s="132"/>
       <c r="H11" s="132"/>
       <c r="I11" s="132"/>
@@ -42729,10 +42727,10 @@
       </c>
       <c r="K11" s="111"/>
       <c r="L11" s="111"/>
-      <c r="M11" s="773" t="s">
+      <c r="M11" s="774" t="s">
         <v>210</v>
       </c>
-      <c r="N11" s="774"/>
+      <c r="N11" s="775"/>
       <c r="O11" s="132"/>
       <c r="P11" s="132"/>
       <c r="Q11" s="130" t="s">
@@ -42740,10 +42738,10 @@
       </c>
       <c r="R11" s="131"/>
       <c r="S11" s="131"/>
-      <c r="T11" s="768" t="s">
+      <c r="T11" s="769" t="s">
         <v>210</v>
       </c>
-      <c r="U11" s="769"/>
+      <c r="U11" s="770"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="110"/>
@@ -42978,10 +42976,10 @@
       </c>
       <c r="C20" s="422"/>
       <c r="D20" s="159"/>
-      <c r="E20" s="768" t="s">
+      <c r="E20" s="769" t="s">
         <v>449</v>
       </c>
-      <c r="F20" s="769"/>
+      <c r="F20" s="770"/>
       <c r="G20" s="140"/>
       <c r="H20" s="140"/>
       <c r="I20" s="111"/>
@@ -42990,10 +42988,10 @@
       </c>
       <c r="K20" s="422"/>
       <c r="L20" s="159"/>
-      <c r="M20" s="768" t="s">
+      <c r="M20" s="769" t="s">
         <v>449</v>
       </c>
-      <c r="N20" s="769"/>
+      <c r="N20" s="770"/>
       <c r="O20" s="150"/>
       <c r="P20" s="150"/>
       <c r="Q20" s="130" t="s">
@@ -43001,10 +42999,10 @@
       </c>
       <c r="R20" s="422"/>
       <c r="S20" s="159"/>
-      <c r="T20" s="768" t="s">
+      <c r="T20" s="769" t="s">
         <v>449</v>
       </c>
-      <c r="U20" s="769"/>
+      <c r="U20" s="770"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="110"/>
@@ -43268,10 +43266,10 @@
       </c>
       <c r="C30" s="422"/>
       <c r="D30" s="159"/>
-      <c r="E30" s="768" t="s">
+      <c r="E30" s="769" t="s">
         <v>449</v>
       </c>
-      <c r="F30" s="769"/>
+      <c r="F30" s="770"/>
       <c r="G30" s="140"/>
       <c r="H30" s="140"/>
       <c r="I30" s="111"/>
@@ -43280,10 +43278,10 @@
       </c>
       <c r="K30" s="422"/>
       <c r="L30" s="159"/>
-      <c r="M30" s="768" t="s">
+      <c r="M30" s="769" t="s">
         <v>449</v>
       </c>
-      <c r="N30" s="769"/>
+      <c r="N30" s="770"/>
       <c r="O30" s="150"/>
       <c r="P30" s="150"/>
       <c r="Q30" s="130" t="s">
@@ -43291,10 +43289,10 @@
       </c>
       <c r="R30" s="422"/>
       <c r="S30" s="159"/>
-      <c r="T30" s="768" t="s">
+      <c r="T30" s="769" t="s">
         <v>449</v>
       </c>
-      <c r="U30" s="769"/>
+      <c r="U30" s="770"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="172"/>
@@ -43617,11 +43615,11 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="110"/>
-      <c r="B42" s="770"/>
-      <c r="C42" s="770"/>
-      <c r="D42" s="770"/>
-      <c r="E42" s="770"/>
-      <c r="F42" s="770"/>
+      <c r="B42" s="771"/>
+      <c r="C42" s="771"/>
+      <c r="D42" s="771"/>
+      <c r="E42" s="771"/>
+      <c r="F42" s="771"/>
       <c r="G42" s="150"/>
       <c r="H42" s="111"/>
       <c r="I42" s="150"/>
@@ -43817,8 +43815,8 @@
       <c r="B3" s="194" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="777"/>
-      <c r="D3" s="777"/>
+      <c r="C3" s="778"/>
+      <c r="D3" s="778"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C4" s="195"/>
@@ -43851,10 +43849,10 @@
       <c r="D10" s="203" t="s">
         <v>232</v>
       </c>
-      <c r="E10" s="778" t="s">
+      <c r="E10" s="779" t="s">
         <v>233</v>
       </c>
-      <c r="F10" s="779"/>
+      <c r="F10" s="780"/>
     </row>
     <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="204" t="s">
@@ -44005,10 +44003,10 @@
       <c r="D30" s="215" t="s">
         <v>232</v>
       </c>
-      <c r="E30" s="778" t="s">
+      <c r="E30" s="779" t="s">
         <v>233</v>
       </c>
-      <c r="F30" s="779"/>
+      <c r="F30" s="780"/>
     </row>
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="204" t="s">
@@ -44156,10 +44154,10 @@
       <c r="D49" s="215" t="s">
         <v>232</v>
       </c>
-      <c r="E49" s="778" t="s">
+      <c r="E49" s="779" t="s">
         <v>233</v>
       </c>
-      <c r="F49" s="779"/>
+      <c r="F49" s="780"/>
     </row>
     <row r="50" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="204" t="s">
@@ -44327,8 +44325,8 @@
       </c>
       <c r="C2" s="113"/>
       <c r="D2" s="113"/>
-      <c r="E2" s="775"/>
-      <c r="F2" s="775"/>
+      <c r="E2" s="776"/>
+      <c r="F2" s="776"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="112"/>
@@ -44360,13 +44358,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="110"/>
-      <c r="B6" s="776" t="s">
+      <c r="B6" s="777" t="s">
         <v>432</v>
       </c>
-      <c r="C6" s="776"/>
-      <c r="D6" s="776"/>
-      <c r="E6" s="776"/>
-      <c r="F6" s="776"/>
+      <c r="C6" s="777"/>
+      <c r="D6" s="777"/>
+      <c r="E6" s="777"/>
+      <c r="F6" s="777"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="110"/>
@@ -44381,14 +44379,14 @@
       <c r="B8" s="457" t="s">
         <v>203</v>
       </c>
-      <c r="C8" s="780" t="s">
+      <c r="C8" s="781" t="s">
         <v>204</v>
       </c>
-      <c r="D8" s="781"/>
-      <c r="E8" s="782" t="s">
+      <c r="D8" s="782"/>
+      <c r="E8" s="783" t="s">
         <v>205</v>
       </c>
-      <c r="F8" s="781"/>
+      <c r="F8" s="782"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="110"/>
@@ -44524,11 +44522,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="110"/>
-      <c r="B22" s="770"/>
-      <c r="C22" s="770"/>
-      <c r="D22" s="770"/>
-      <c r="E22" s="770"/>
-      <c r="F22" s="770"/>
+      <c r="B22" s="771"/>
+      <c r="C22" s="771"/>
+      <c r="D22" s="771"/>
+      <c r="E22" s="771"/>
+      <c r="F22" s="771"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="110"/>
@@ -44598,13 +44596,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="783" t="s">
+      <c r="B2" s="784" t="s">
         <v>250</v>
       </c>
-      <c r="C2" s="784" t="s">
+      <c r="C2" s="785" t="s">
         <v>251</v>
       </c>
-      <c r="D2" s="784" t="s">
+      <c r="D2" s="785" t="s">
         <v>150</v>
       </c>
       <c r="E2" s="232" t="s">
@@ -44639,9 +44637,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="783"/>
-      <c r="C3" s="785"/>
-      <c r="D3" s="785"/>
+      <c r="B3" s="784"/>
+      <c r="C3" s="786"/>
+      <c r="D3" s="786"/>
       <c r="E3" s="668" t="s">
         <v>259</v>
       </c>
@@ -44674,7 +44672,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="786" t="s">
+      <c r="B4" s="787" t="s">
         <v>262</v>
       </c>
       <c r="C4" s="233" t="s">
@@ -44693,7 +44691,7 @@
       <c r="N4" s="235"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="786"/>
+      <c r="B5" s="787"/>
       <c r="C5" s="233" t="s">
         <v>60</v>
       </c>
@@ -44710,7 +44708,7 @@
       <c r="N5" s="235"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="787"/>
+      <c r="B6" s="788"/>
       <c r="C6" s="558" t="s">
         <v>453</v>
       </c>
@@ -44806,11 +44804,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44818,30 +44816,31 @@
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="12" max="12" width="46.85546875" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="584" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="788" t="s">
+      <c r="A1" s="789" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="789"/>
-      <c r="C1" s="837"/>
-      <c r="D1" s="790" t="s">
+      <c r="B1" s="790"/>
+      <c r="C1" s="688"/>
+      <c r="D1" s="791" t="s">
         <v>458</v>
       </c>
-      <c r="E1" s="790"/>
-      <c r="F1" s="791"/>
-      <c r="G1" s="800" t="s">
+      <c r="E1" s="791"/>
+      <c r="F1" s="792"/>
+      <c r="G1" s="801" t="s">
         <v>264</v>
       </c>
-      <c r="H1" s="801"/>
-      <c r="I1" s="801"/>
-      <c r="J1" s="801"/>
-      <c r="K1" s="802"/>
-      <c r="L1" s="792" t="s">
+      <c r="H1" s="802"/>
+      <c r="I1" s="802"/>
+      <c r="J1" s="802"/>
+      <c r="K1" s="803"/>
+      <c r="L1" s="793" t="s">
         <v>265</v>
       </c>
       <c r="M1" s="38" t="s">
@@ -44883,7 +44882,7 @@
       <c r="K2" s="250" t="s">
         <v>269</v>
       </c>
-      <c r="L2" s="793"/>
+      <c r="L2" s="794"/>
       <c r="M2" s="44" t="s">
         <v>57</v>
       </c>
@@ -44897,19 +44896,19 @@
       <c r="C3" s="252" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="794" t="s">
+      <c r="D3" s="795" t="s">
         <v>270</v>
       </c>
-      <c r="E3" s="795"/>
-      <c r="F3" s="796"/>
-      <c r="G3" s="797" t="s">
+      <c r="E3" s="796"/>
+      <c r="F3" s="797"/>
+      <c r="G3" s="798" t="s">
         <v>270</v>
       </c>
-      <c r="H3" s="798"/>
-      <c r="I3" s="798"/>
-      <c r="J3" s="798"/>
-      <c r="K3" s="799"/>
-      <c r="L3" s="793"/>
+      <c r="H3" s="799"/>
+      <c r="I3" s="799"/>
+      <c r="J3" s="799"/>
+      <c r="K3" s="800"/>
+      <c r="L3" s="794"/>
       <c r="M3" s="593"/>
       <c r="N3" s="594"/>
     </row>
@@ -44962,12 +44961,12 @@
   </sheetData>
   <autoFilter ref="A4:N4"/>
   <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="L1:L3"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:K3"/>
     <mergeCell ref="G1:K1"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>